<commit_message>
Code updated 23-03-27 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -29,12 +29,32 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -56,11 +76,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -358,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,6 +411,21 @@
           <t>Season</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Now</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>03-26_A</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>03-26_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -405,6 +444,19 @@
       <c r="D2" t="n">
         <v>3664</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -423,6 +475,9 @@
       <c r="D3" t="n">
         <v>7573</v>
       </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" s="3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -441,6 +496,9 @@
       <c r="D4" t="n">
         <v>7472</v>
       </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" s="3" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -459,6 +517,9 @@
       <c r="D5" t="n">
         <v>7383</v>
       </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" s="3" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -477,6 +538,9 @@
       <c r="D6" t="n">
         <v>6817</v>
       </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" s="3" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -495,6 +559,9 @@
       <c r="D7" t="n">
         <v>6415</v>
       </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" s="3" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -513,6 +580,9 @@
       <c r="D8" t="n">
         <v>7589</v>
       </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" s="3" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -531,6 +601,9 @@
       <c r="D9" t="n">
         <v>7371</v>
       </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" s="3" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -549,6 +622,19 @@
       <c r="D10" t="n">
         <v>7257</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>3113</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -567,6 +653,9 @@
       <c r="D11" t="n">
         <v>7062</v>
       </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" s="3" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -585,6 +674,19 @@
       <c r="D12" t="n">
         <v>6027</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2914</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -603,6 +705,19 @@
       <c r="D13" t="n">
         <v>5957</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2856</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -621,6 +736,19 @@
       <c r="D14" t="n">
         <v>5937</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2836</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -639,6 +767,19 @@
       <c r="D15" t="n">
         <v>5785</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2499</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -657,6 +798,19 @@
       <c r="D16" t="n">
         <v>7601</v>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>3040</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -675,6 +829,9 @@
       <c r="D17" t="n">
         <v>7362</v>
       </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" s="3" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -693,6 +850,9 @@
       <c r="D18" t="n">
         <v>7232</v>
       </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" s="3" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -711,6 +871,9 @@
       <c r="D19" t="n">
         <v>7103</v>
       </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" s="3" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -729,6 +892,9 @@
       <c r="D20" t="n">
         <v>7060</v>
       </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" s="3" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -747,6 +913,19 @@
       <c r="D21" t="n">
         <v>7033</v>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>3032</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -765,6 +944,9 @@
       <c r="D22" t="n">
         <v>7017</v>
       </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" s="3" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -783,6 +965,9 @@
       <c r="D23" t="n">
         <v>6909</v>
       </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" s="3" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -801,6 +986,19 @@
       <c r="D24" t="n">
         <v>6833</v>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2975</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -819,6 +1017,9 @@
       <c r="D25" t="n">
         <v>6818</v>
       </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" s="3" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -837,6 +1038,9 @@
       <c r="D26" t="n">
         <v>6813</v>
       </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" s="3" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -855,6 +1059,9 @@
       <c r="D27" t="n">
         <v>6752</v>
       </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" s="3" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -873,6 +1080,9 @@
       <c r="D28" t="n">
         <v>6670</v>
       </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" s="3" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -891,6 +1101,9 @@
       <c r="D29" t="n">
         <v>6658</v>
       </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" s="3" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -909,6 +1122,9 @@
       <c r="D30" t="n">
         <v>6692</v>
       </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" s="3" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -927,6 +1143,9 @@
       <c r="D31" t="n">
         <v>6501</v>
       </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" s="3" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -945,6 +1164,9 @@
       <c r="D32" t="n">
         <v>6463</v>
       </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" s="3" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -963,6 +1185,9 @@
       <c r="D33" t="n">
         <v>6446</v>
       </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" s="3" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -981,6 +1206,9 @@
       <c r="D34" t="n">
         <v>6433</v>
       </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" s="3" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -999,6 +1227,19 @@
       <c r="D35" t="n">
         <v>6365</v>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1017,6 +1258,19 @@
       <c r="D36" t="n">
         <v>6170</v>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2877</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1035,6 +1289,9 @@
       <c r="D37" t="n">
         <v>6078</v>
       </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" s="3" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1053,6 +1310,9 @@
       <c r="D38" t="n">
         <v>6047</v>
       </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" s="3" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1071,6 +1331,19 @@
       <c r="D39" t="n">
         <v>5740</v>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2798</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -1089,6 +1362,19 @@
       <c r="D40" t="n">
         <v>5596</v>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2840</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -1107,6 +1393,9 @@
       <c r="D41" t="n">
         <v>5375</v>
       </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" s="3" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1125,6 +1414,19 @@
       <c r="D42" t="n">
         <v>5283</v>
       </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2960</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -1143,6 +1445,9 @@
       <c r="D43" t="n">
         <v>5280</v>
       </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" s="3" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1161,6 +1466,19 @@
       <c r="D44" t="n">
         <v>5300</v>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2819</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1179,6 +1497,19 @@
       <c r="D45" t="n">
         <v>4948</v>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2838</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1197,6 +1528,19 @@
       <c r="D46" t="n">
         <v>4932</v>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1215,6 +1559,19 @@
       <c r="D47" t="n">
         <v>3368</v>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1233,6 +1590,19 @@
       <c r="D48" t="n">
         <v>2548</v>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1251,6 +1621,19 @@
       <c r="D49" t="n">
         <v>0</v>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1269,6 +1652,9 @@
       <c r="D50" t="n">
         <v>6585</v>
       </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" s="3" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1287,6 +1673,9 @@
       <c r="D51" t="n">
         <v>6330</v>
       </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" s="3" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1305,6 +1694,19 @@
       <c r="D52" t="n">
         <v>5740</v>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2916</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1323,6 +1725,19 @@
       <c r="D53" t="n">
         <v>5275</v>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2762</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1341,6 +1756,9 @@
       <c r="D54" t="n">
         <v>5952</v>
       </c>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" s="3" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1359,6 +1777,19 @@
       <c r="D55" t="n">
         <v>5873</v>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2966</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1377,6 +1808,19 @@
       <c r="D56" t="n">
         <v>5653</v>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>3063</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1395,6 +1839,19 @@
       <c r="D57" t="n">
         <v>5654</v>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>3019</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1413,6 +1870,19 @@
       <c r="D58" t="n">
         <v>5474</v>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>3019</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1431,6 +1901,19 @@
       <c r="D59" t="n">
         <v>5305</v>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>3065</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1449,6 +1932,19 @@
       <c r="D60" t="n">
         <v>5277</v>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2945</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1467,6 +1963,19 @@
       <c r="D61" t="n">
         <v>4938</v>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2881</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1485,6 +1994,19 @@
       <c r="D62" t="n">
         <v>6244</v>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>3009</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1503,6 +2025,19 @@
       <c r="D63" t="n">
         <v>6168</v>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2884</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1521,6 +2056,19 @@
       <c r="D64" t="n">
         <v>5996</v>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>3042</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1539,6 +2087,9 @@
       <c r="D65" t="n">
         <v>5857</v>
       </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" s="3" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1557,6 +2108,19 @@
       <c r="D66" t="n">
         <v>5465</v>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>3020</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1575,6 +2139,19 @@
       <c r="D67" t="n">
         <v>5410</v>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2809</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1593,6 +2170,19 @@
       <c r="D68" t="n">
         <v>5346</v>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>3067</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1611,6 +2201,19 @@
       <c r="D69" t="n">
         <v>5172</v>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2885</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1629,6 +2232,19 @@
       <c r="D70" t="n">
         <v>5083</v>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2869</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1647,6 +2263,19 @@
       <c r="D71" t="n">
         <v>4918</v>
       </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2922</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1665,6 +2294,19 @@
       <c r="D72" t="n">
         <v>4856</v>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2984</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1683,6 +2325,19 @@
       <c r="D73" t="n">
         <v>4834</v>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F73" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2492</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1701,6 +2356,19 @@
       <c r="D74" t="n">
         <v>4773</v>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F74" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2709</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1719,6 +2387,19 @@
       <c r="D75" t="n">
         <v>4625</v>
       </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2491</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1737,6 +2418,19 @@
       <c r="D76" t="n">
         <v>4530</v>
       </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2800</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1755,6 +2449,19 @@
       <c r="D77" t="n">
         <v>4529</v>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2840</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1773,6 +2480,19 @@
       <c r="D78" t="n">
         <v>4505</v>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2816</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1791,6 +2511,19 @@
       <c r="D79" t="n">
         <v>4128</v>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2739</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1809,6 +2542,19 @@
       <c r="D80" t="n">
         <v>4059</v>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F80" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2735</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1827,6 +2573,19 @@
       <c r="D81" t="n">
         <v>4007</v>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F81" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2697</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1845,6 +2604,19 @@
       <c r="D82" t="n">
         <v>3370</v>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2618</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1863,6 +2635,19 @@
       <c r="D83" t="n">
         <v>3330</v>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1881,6 +2666,19 @@
       <c r="D84" t="n">
         <v>3221</v>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2498</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1899,6 +2697,19 @@
       <c r="D85" t="n">
         <v>2943</v>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1917,6 +2728,19 @@
       <c r="D86" t="n">
         <v>2915</v>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1935,6 +2759,19 @@
       <c r="D87" t="n">
         <v>2689</v>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1953,6 +2790,19 @@
       <c r="D88" t="n">
         <v>2499</v>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1971,6 +2821,9 @@
       <c r="D89" t="n">
         <v>0</v>
       </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" s="3" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1989,6 +2842,19 @@
       <c r="D90" t="n">
         <v>5411</v>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>3056</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -2007,6 +2873,19 @@
       <c r="D91" t="n">
         <v>3953</v>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2025,6 +2904,19 @@
       <c r="D92" t="n">
         <v>3139</v>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2531</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2043,6 +2935,19 @@
       <c r="D93" t="n">
         <v>2500</v>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2061,6 +2966,19 @@
       <c r="D94" t="n">
         <v>5028</v>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>2614</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2079,6 +2997,19 @@
       <c r="D95" t="n">
         <v>4937</v>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>2807</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2097,6 +3028,19 @@
       <c r="D96" t="n">
         <v>4910</v>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>2494</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2115,6 +3059,19 @@
       <c r="D97" t="n">
         <v>4808</v>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F97" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>2851</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2133,6 +3090,19 @@
       <c r="D98" t="n">
         <v>3127</v>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>2672</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2151,6 +3121,19 @@
       <c r="D99" t="n">
         <v>4835</v>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F99" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>2662</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -2169,6 +3152,19 @@
       <c r="D100" t="n">
         <v>4673</v>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F100" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>2517</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -2187,6 +3183,19 @@
       <c r="D101" t="n">
         <v>4635</v>
       </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F101" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>2727</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -2205,6 +3214,19 @@
       <c r="D102" t="n">
         <v>4570</v>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F102" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>2786</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -2223,6 +3245,19 @@
       <c r="D103" t="n">
         <v>4428</v>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>2712</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -2241,6 +3276,19 @@
       <c r="D104" t="n">
         <v>4417</v>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>2821</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -2259,6 +3307,19 @@
       <c r="D105" t="n">
         <v>4405</v>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -2277,6 +3338,19 @@
       <c r="D106" t="n">
         <v>4397</v>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F106" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>2899</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -2295,6 +3369,19 @@
       <c r="D107" t="n">
         <v>4356</v>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>2879</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -2313,6 +3400,19 @@
       <c r="D108" t="n">
         <v>4306</v>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F108" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>2777</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -2331,6 +3431,19 @@
       <c r="D109" t="n">
         <v>4262</v>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>2517</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -2349,6 +3462,19 @@
       <c r="D110" t="n">
         <v>4184</v>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F110" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>2767</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -2367,6 +3493,9 @@
       <c r="D111" t="n">
         <v>4014</v>
       </c>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" s="3" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -2385,6 +3514,19 @@
       <c r="D112" t="n">
         <v>3998</v>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F112" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>2654</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -2403,6 +3545,19 @@
       <c r="D113" t="n">
         <v>3922</v>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>2589</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -2421,6 +3576,19 @@
       <c r="D114" t="n">
         <v>3648</v>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -2439,6 +3607,19 @@
       <c r="D115" t="n">
         <v>3633</v>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>2616</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -2457,6 +3638,19 @@
       <c r="D116" t="n">
         <v>3448</v>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>2768</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -2475,6 +3669,19 @@
       <c r="D117" t="n">
         <v>3256</v>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F117" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>2537</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -2493,6 +3700,9 @@
       <c r="D118" t="n">
         <v>3130</v>
       </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" s="3" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -2511,6 +3721,19 @@
       <c r="D119" t="n">
         <v>2810</v>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>2499</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -2529,6 +3752,19 @@
       <c r="D120" t="n">
         <v>2681</v>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F120" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>2544</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -2547,6 +3783,19 @@
       <c r="D121" t="n">
         <v>2664</v>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2565,6 +3814,19 @@
       <c r="D122" t="n">
         <v>2643</v>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>2497</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2583,6 +3845,19 @@
       <c r="D123" t="n">
         <v>2642</v>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2601,6 +3876,19 @@
       <c r="D124" t="n">
         <v>2626</v>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>2484</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2619,6 +3907,19 @@
       <c r="D125" t="n">
         <v>2395</v>
       </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2637,6 +3938,19 @@
       <c r="D126" t="n">
         <v>1998</v>
       </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -2655,6 +3969,19 @@
       <c r="D127" t="n">
         <v>1806</v>
       </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>1527</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -2673,6 +4000,19 @@
       <c r="D128" t="n">
         <v>1156</v>
       </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>1126</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -2691,6 +4031,19 @@
       <c r="D129" t="n">
         <v>0</v>
       </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -2709,6 +4062,19 @@
       <c r="D130" t="n">
         <v>0</v>
       </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -2727,6 +4093,19 @@
       <c r="D131" t="n">
         <v>0</v>
       </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -2745,6 +4124,19 @@
       <c r="D132" t="n">
         <v>0</v>
       </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -2763,6 +4155,19 @@
       <c r="D133" t="n">
         <v>0</v>
       </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -2781,6 +4186,19 @@
       <c r="D134" t="n">
         <v>0</v>
       </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -2799,6 +4217,19 @@
       <c r="D135" t="n">
         <v>3207</v>
       </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>2536</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -2817,6 +4248,19 @@
       <c r="D136" t="n">
         <v>3743</v>
       </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -2835,6 +4279,19 @@
       <c r="D137" t="n">
         <v>0</v>
       </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -2853,6 +4310,19 @@
       <c r="D138" t="n">
         <v>3260</v>
       </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F138" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>2565</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -2871,6 +4341,19 @@
       <c r="D139" t="n">
         <v>0</v>
       </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -2889,6 +4372,19 @@
       <c r="D140" t="n">
         <v>2230</v>
       </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -2907,6 +4403,19 @@
       <c r="D141" t="n">
         <v>2180</v>
       </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -2925,6 +4434,19 @@
       <c r="D142" t="n">
         <v>1580</v>
       </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -2943,6 +4465,19 @@
       <c r="D143" t="n">
         <v>1498</v>
       </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>1400</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -2961,6 +4496,19 @@
       <c r="D144" t="n">
         <v>0</v>
       </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -2979,6 +4527,19 @@
       <c r="D145" t="n">
         <v>0</v>
       </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -2997,6 +4558,19 @@
       <c r="D146" t="n">
         <v>0</v>
       </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -3015,6 +4589,19 @@
       <c r="D147" t="n">
         <v>0</v>
       </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -3033,6 +4620,19 @@
       <c r="D148" t="n">
         <v>0</v>
       </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -3051,6 +4651,19 @@
       <c r="D149" t="n">
         <v>0</v>
       </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -3069,6 +4682,19 @@
       <c r="D150" t="n">
         <v>2938</v>
       </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -3087,6 +4713,19 @@
       <c r="D151" t="n">
         <v>3310</v>
       </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -3105,6 +4744,19 @@
       <c r="D152" t="n">
         <v>2620</v>
       </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -3123,6 +4775,19 @@
       <c r="D153" t="n">
         <v>0</v>
       </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -3141,6 +4806,19 @@
       <c r="D154" t="n">
         <v>0</v>
       </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -3159,6 +4837,19 @@
       <c r="D155" t="n">
         <v>0</v>
       </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -3177,6 +4868,19 @@
       <c r="D156" t="n">
         <v>0</v>
       </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -3195,6 +4899,19 @@
       <c r="D157" t="n">
         <v>0</v>
       </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -3212,6 +4929,100 @@
       </c>
       <c r="D158" t="n">
         <v>0</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>42542275</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>"同 风 雨"</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr"/>
+      <c r="D159" t="inlineStr"/>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>2492</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>59100545</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>"black dragon"</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr"/>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F160" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>1678</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>59106471</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>anime</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F161" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>1357</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code updated 23-03-27 15:08:56
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -4945,10 +4945,8 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>42542275</t>
-        </is>
+      <c r="A159" t="n">
+        <v>42542275</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -4972,10 +4970,8 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>59100545</t>
-        </is>
+      <c r="A160" t="n">
+        <v>59100545</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -4999,10 +4995,8 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>59106471</t>
-        </is>
+      <c r="A161" t="n">
+        <v>59106471</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-03-28 11:30:53
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:I162"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>03-26_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>03-27_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>03-27_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -478,6 +494,8 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" s="3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -499,6 +517,8 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" s="3" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
+      <c r="H4" s="3" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -520,6 +540,8 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" s="3" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -541,6 +563,8 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" s="3" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -562,6 +586,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" s="3" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -583,6 +609,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" s="3" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -604,6 +632,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="3" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -630,9 +660,15 @@
       <c r="F10" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>3113</t>
+      <c r="G10" t="n">
+        <v>3113</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>3589</t>
         </is>
       </c>
     </row>
@@ -656,6 +692,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" s="3" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -682,9 +720,15 @@
       <c r="F12" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2914</t>
+      <c r="G12" t="n">
+        <v>2914</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3244</t>
         </is>
       </c>
     </row>
@@ -713,9 +757,15 @@
       <c r="F13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="G13" t="n">
+        <v>2856</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3112</t>
         </is>
       </c>
     </row>
@@ -744,9 +794,15 @@
       <c r="F14" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2836</t>
+      <c r="G14" t="n">
+        <v>2836</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3321</t>
         </is>
       </c>
     </row>
@@ -775,9 +831,15 @@
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="G15" t="n">
+        <v>2499</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2520</t>
         </is>
       </c>
     </row>
@@ -806,9 +868,15 @@
       <c r="F16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>3040</t>
+      <c r="G16" t="n">
+        <v>3040</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3543</t>
         </is>
       </c>
     </row>
@@ -832,6 +900,8 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" s="3" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" s="3" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -853,6 +923,8 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" s="3" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
+      <c r="H18" s="3" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -874,6 +946,8 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" s="3" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
+      <c r="H19" s="3" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -895,6 +969,8 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" s="3" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
+      <c r="H20" s="3" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -921,11 +997,11 @@
       <c r="F21" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>3032</t>
-        </is>
-      </c>
+      <c r="G21" t="n">
+        <v>3032</v>
+      </c>
+      <c r="H21" s="3" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -947,6 +1023,8 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" s="3" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
+      <c r="H22" s="3" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -968,6 +1046,8 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" s="3" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
+      <c r="H23" s="3" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -994,9 +1074,15 @@
       <c r="F24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="G24" t="n">
+        <v>2975</v>
+      </c>
+      <c r="H24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>3440</t>
         </is>
       </c>
     </row>
@@ -1020,6 +1106,8 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" s="3" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
+      <c r="H25" s="3" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1041,6 +1129,8 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" s="3" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
+      <c r="H26" s="3" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1062,6 +1152,8 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" s="3" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
+      <c r="H27" s="3" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1083,6 +1175,8 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" s="3" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" s="3" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1104,6 +1198,8 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" s="3" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
+      <c r="H29" s="3" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1125,6 +1221,8 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" s="3" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
+      <c r="H30" s="3" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1146,6 +1244,8 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" s="3" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
+      <c r="H31" s="3" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1167,6 +1267,8 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" s="3" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
+      <c r="H32" s="3" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1188,6 +1290,8 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" s="3" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" s="3" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1209,6 +1313,8 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" s="3" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
+      <c r="H34" s="3" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1235,7 +1341,13 @@
       <c r="F35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1266,9 +1378,15 @@
       <c r="F36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2877</t>
+      <c r="G36" t="n">
+        <v>2877</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -1292,6 +1410,8 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" s="3" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
+      <c r="H37" s="3" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1313,6 +1433,8 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" s="3" t="inlineStr"/>
       <c r="G38" t="inlineStr"/>
+      <c r="H38" s="3" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1339,9 +1461,15 @@
       <c r="F39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>2798</t>
+      <c r="G39" t="n">
+        <v>2798</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>3027</t>
         </is>
       </c>
     </row>
@@ -1370,9 +1498,15 @@
       <c r="F40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="G40" t="n">
+        <v>2840</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3188</t>
         </is>
       </c>
     </row>
@@ -1396,6 +1530,8 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" s="3" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
+      <c r="H41" s="3" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1422,9 +1558,15 @@
       <c r="F42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>2960</t>
+      <c r="G42" t="n">
+        <v>2960</v>
+      </c>
+      <c r="H42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>3355</t>
         </is>
       </c>
     </row>
@@ -1448,6 +1590,8 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" s="3" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" s="3" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1474,9 +1618,15 @@
       <c r="F44" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="G44" t="n">
+        <v>2819</v>
+      </c>
+      <c r="H44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>3139</t>
         </is>
       </c>
     </row>
@@ -1505,9 +1655,15 @@
       <c r="F45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2838</t>
+      <c r="G45" t="n">
+        <v>2838</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3138</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1692,13 @@
       <c r="F46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1567,9 +1729,15 @@
       <c r="F47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G47" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H47" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -1598,7 +1766,13 @@
       <c r="F48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1629,7 +1803,13 @@
       <c r="F49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1655,6 +1835,8 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" s="3" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
+      <c r="H50" s="3" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1676,6 +1858,8 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" s="3" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
+      <c r="H51" s="3" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1702,9 +1886,15 @@
       <c r="F52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="G52" t="n">
+        <v>2916</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>3298</t>
         </is>
       </c>
     </row>
@@ -1733,9 +1923,15 @@
       <c r="F53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="G53" t="n">
+        <v>2762</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>3073</t>
         </is>
       </c>
     </row>
@@ -1759,6 +1955,8 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" s="3" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
+      <c r="H54" s="3" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1785,9 +1983,15 @@
       <c r="F55" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2966</t>
+      <c r="G55" t="n">
+        <v>2966</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>3388</t>
         </is>
       </c>
     </row>
@@ -1816,9 +2020,15 @@
       <c r="F56" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>3063</t>
+      <c r="G56" t="n">
+        <v>3063</v>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>3597</t>
         </is>
       </c>
     </row>
@@ -1847,9 +2057,15 @@
       <c r="F57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="G57" t="n">
+        <v>3019</v>
+      </c>
+      <c r="H57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>3542</t>
         </is>
       </c>
     </row>
@@ -1878,9 +2094,15 @@
       <c r="F58" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="G58" t="n">
+        <v>3019</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>3520</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2131,15 @@
       <c r="F59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="G59" t="n">
+        <v>3065</v>
+      </c>
+      <c r="H59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3525</t>
         </is>
       </c>
     </row>
@@ -1940,9 +2168,15 @@
       <c r="F60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2945</t>
+      <c r="G60" t="n">
+        <v>2945</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -1971,9 +2205,15 @@
       <c r="F61" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2881</t>
+      <c r="G61" t="n">
+        <v>2881</v>
+      </c>
+      <c r="H61" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2242,15 @@
       <c r="F62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="G62" t="n">
+        <v>3009</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3525</t>
         </is>
       </c>
     </row>
@@ -2033,9 +2279,15 @@
       <c r="F63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="G63" t="n">
+        <v>2884</v>
+      </c>
+      <c r="H63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3296</t>
         </is>
       </c>
     </row>
@@ -2064,9 +2316,15 @@
       <c r="F64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>3042</t>
+      <c r="G64" t="n">
+        <v>3042</v>
+      </c>
+      <c r="H64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>3487</t>
         </is>
       </c>
     </row>
@@ -2090,6 +2348,8 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" s="3" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
+      <c r="H65" s="3" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2116,9 +2376,15 @@
       <c r="F66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>3020</t>
+      <c r="G66" t="n">
+        <v>3020</v>
+      </c>
+      <c r="H66" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>3677</t>
         </is>
       </c>
     </row>
@@ -2147,9 +2413,15 @@
       <c r="F67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="G67" t="n">
+        <v>2809</v>
+      </c>
+      <c r="H67" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>3092</t>
         </is>
       </c>
     </row>
@@ -2178,9 +2450,15 @@
       <c r="F68" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="G68" t="n">
+        <v>3067</v>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>3445</t>
         </is>
       </c>
     </row>
@@ -2209,9 +2487,15 @@
       <c r="F69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="G69" t="n">
+        <v>2885</v>
+      </c>
+      <c r="H69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -2240,9 +2524,15 @@
       <c r="F70" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="G70" t="n">
+        <v>2869</v>
+      </c>
+      <c r="H70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>3302</t>
         </is>
       </c>
     </row>
@@ -2271,9 +2561,15 @@
       <c r="F71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2922</t>
+      <c r="G71" t="n">
+        <v>2922</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2931</t>
         </is>
       </c>
     </row>
@@ -2302,9 +2598,15 @@
       <c r="F72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="G72" t="n">
+        <v>2984</v>
+      </c>
+      <c r="H72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>3381</t>
         </is>
       </c>
     </row>
@@ -2333,9 +2635,15 @@
       <c r="F73" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G73" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H73" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -2364,9 +2672,15 @@
       <c r="F74" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2709</t>
+      <c r="G74" t="n">
+        <v>2709</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -2395,9 +2709,15 @@
       <c r="F75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>2491</t>
+      <c r="G75" t="n">
+        <v>2491</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -2426,9 +2746,15 @@
       <c r="F76" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="G76" t="n">
+        <v>2800</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2843</t>
         </is>
       </c>
     </row>
@@ -2457,9 +2783,15 @@
       <c r="F77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="G77" t="n">
+        <v>2840</v>
+      </c>
+      <c r="H77" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>3222</t>
         </is>
       </c>
     </row>
@@ -2488,9 +2820,15 @@
       <c r="F78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="G78" t="n">
+        <v>2816</v>
+      </c>
+      <c r="H78" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -2519,9 +2857,15 @@
       <c r="F79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>2739</t>
+      <c r="G79" t="n">
+        <v>2739</v>
+      </c>
+      <c r="H79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2907</t>
         </is>
       </c>
     </row>
@@ -2550,9 +2894,15 @@
       <c r="F80" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>2735</t>
+      <c r="G80" t="n">
+        <v>2735</v>
+      </c>
+      <c r="H80" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -2581,9 +2931,15 @@
       <c r="F81" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>2697</t>
+      <c r="G81" t="n">
+        <v>2697</v>
+      </c>
+      <c r="H81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>2824</t>
         </is>
       </c>
     </row>
@@ -2612,9 +2968,15 @@
       <c r="F82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="G82" t="n">
+        <v>2618</v>
+      </c>
+      <c r="H82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>2885</t>
         </is>
       </c>
     </row>
@@ -2643,9 +3005,15 @@
       <c r="F83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2674,9 +3042,15 @@
       <c r="F84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="G84" t="n">
+        <v>2498</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -2705,11 +3079,11 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="3" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -2736,7 +3110,13 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2767,9 +3147,15 @@
       <c r="F87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>3149</t>
         </is>
       </c>
     </row>
@@ -2798,11 +3184,11 @@
       <c r="F88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="3" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2824,6 +3210,8 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" s="3" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
+      <c r="H89" s="3" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -2850,9 +3238,15 @@
       <c r="F90" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>3056</t>
+      <c r="G90" t="n">
+        <v>3056</v>
+      </c>
+      <c r="H90" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>3434</t>
         </is>
       </c>
     </row>
@@ -2881,7 +3275,13 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2912,9 +3312,15 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>2531</t>
+      <c r="G92" t="n">
+        <v>2531</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -2943,7 +3349,13 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2968,15 +3380,21 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="G94" t="n">
+        <v>2614</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -3005,9 +3423,15 @@
       <c r="F95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="G95" t="n">
+        <v>2807</v>
+      </c>
+      <c r="H95" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>3013</t>
         </is>
       </c>
     </row>
@@ -3036,9 +3460,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="G96" t="n">
+        <v>2494</v>
+      </c>
+      <c r="H96" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -3067,9 +3497,15 @@
       <c r="F97" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="G97" t="n">
+        <v>2851</v>
+      </c>
+      <c r="H97" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -3098,9 +3534,15 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>2672</t>
+      <c r="G98" t="n">
+        <v>2672</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -3123,15 +3565,21 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F99" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>2662</t>
+      <c r="G99" t="n">
+        <v>2662</v>
+      </c>
+      <c r="H99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2908</t>
         </is>
       </c>
     </row>
@@ -3160,9 +3608,15 @@
       <c r="F100" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="G100" t="n">
+        <v>2517</v>
+      </c>
+      <c r="H100" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2771</t>
         </is>
       </c>
     </row>
@@ -3191,9 +3645,15 @@
       <c r="F101" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="G101" t="n">
+        <v>2727</v>
+      </c>
+      <c r="H101" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>3054</t>
         </is>
       </c>
     </row>
@@ -3222,9 +3682,15 @@
       <c r="F102" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="G102" t="n">
+        <v>2786</v>
+      </c>
+      <c r="H102" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>3076</t>
         </is>
       </c>
     </row>
@@ -3247,15 +3713,21 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="G103" t="n">
+        <v>2712</v>
+      </c>
+      <c r="H103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2953</t>
         </is>
       </c>
     </row>
@@ -3284,9 +3756,15 @@
       <c r="F104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="G104" t="n">
+        <v>2821</v>
+      </c>
+      <c r="H104" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>3023</t>
         </is>
       </c>
     </row>
@@ -3315,7 +3793,13 @@
       <c r="F105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3346,9 +3830,15 @@
       <c r="F106" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="G106" t="n">
+        <v>2899</v>
+      </c>
+      <c r="H106" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -3377,9 +3867,15 @@
       <c r="F107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="G107" t="n">
+        <v>2879</v>
+      </c>
+      <c r="H107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>3140</t>
         </is>
       </c>
     </row>
@@ -3408,9 +3904,15 @@
       <c r="F108" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="G108" t="n">
+        <v>2777</v>
+      </c>
+      <c r="H108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>2929</t>
         </is>
       </c>
     </row>
@@ -3439,9 +3941,15 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="G109" t="n">
+        <v>2517</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -3464,15 +3972,21 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F110" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>2767</t>
+      <c r="G110" t="n">
+        <v>2767</v>
+      </c>
+      <c r="H110" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -3496,6 +4010,8 @@
       <c r="E111" t="inlineStr"/>
       <c r="F111" s="3" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
+      <c r="H111" s="3" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -3516,15 +4032,21 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F112" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>2654</t>
+      <c r="G112" t="n">
+        <v>2654</v>
+      </c>
+      <c r="H112" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2674</t>
         </is>
       </c>
     </row>
@@ -3553,9 +4075,15 @@
       <c r="F113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>2589</t>
+      <c r="G113" t="n">
+        <v>2589</v>
+      </c>
+      <c r="H113" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -3584,7 +4112,13 @@
       <c r="F114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="inlineStr">
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3609,15 +4143,21 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>2616</t>
+      <c r="G115" t="n">
+        <v>2616</v>
+      </c>
+      <c r="H115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>2714</t>
         </is>
       </c>
     </row>
@@ -3646,9 +4186,15 @@
       <c r="F116" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>2768</t>
+      <c r="G116" t="n">
+        <v>2768</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>2806</t>
         </is>
       </c>
     </row>
@@ -3677,11 +4223,11 @@
       <c r="F117" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>2537</t>
-        </is>
-      </c>
+      <c r="G117" t="n">
+        <v>2537</v>
+      </c>
+      <c r="H117" s="3" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -3703,6 +4249,8 @@
       <c r="E118" t="inlineStr"/>
       <c r="F118" s="3" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
+      <c r="H118" s="3" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -3729,9 +4277,15 @@
       <c r="F119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="G119" t="n">
+        <v>2499</v>
+      </c>
+      <c r="H119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -3760,9 +4314,15 @@
       <c r="F120" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="G120" t="n">
+        <v>2544</v>
+      </c>
+      <c r="H120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -3791,9 +4351,15 @@
       <c r="F121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3822,9 +4388,15 @@
       <c r="F122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="G122" t="n">
+        <v>2497</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -3853,9 +4425,15 @@
       <c r="F123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="G123" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -3884,9 +4462,15 @@
       <c r="F124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="G124" t="n">
+        <v>2484</v>
+      </c>
+      <c r="H124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -3915,7 +4499,13 @@
       <c r="F125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G125" t="inlineStr">
+      <c r="G125" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3946,9 +4536,15 @@
       <c r="F126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="G126" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>1497</t>
         </is>
       </c>
     </row>
@@ -3977,9 +4573,15 @@
       <c r="F127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>1527</t>
+      <c r="G127" t="n">
+        <v>1527</v>
+      </c>
+      <c r="H127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>1526</t>
         </is>
       </c>
     </row>
@@ -4008,9 +4610,15 @@
       <c r="F128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>1126</t>
+      <c r="G128" t="n">
+        <v>1126</v>
+      </c>
+      <c r="H128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>1141</t>
         </is>
       </c>
     </row>
@@ -4039,7 +4647,13 @@
       <c r="F129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G129" t="inlineStr">
+      <c r="G129" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4070,7 +4684,13 @@
       <c r="F130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G130" t="inlineStr">
+      <c r="G130" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4101,7 +4721,13 @@
       <c r="F131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="inlineStr">
+      <c r="G131" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4132,7 +4758,13 @@
       <c r="F132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G132" t="inlineStr">
+      <c r="G132" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4163,7 +4795,13 @@
       <c r="F133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G133" t="inlineStr">
+      <c r="G133" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4194,7 +4832,13 @@
       <c r="F134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="inlineStr">
+      <c r="G134" t="n">
+        <v>0</v>
+      </c>
+      <c r="H134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4225,9 +4869,15 @@
       <c r="F135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="G135" t="n">
+        <v>2536</v>
+      </c>
+      <c r="H135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>2630</t>
         </is>
       </c>
     </row>
@@ -4256,9 +4906,15 @@
       <c r="F136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G136" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>2793</t>
         </is>
       </c>
     </row>
@@ -4287,7 +4943,13 @@
       <c r="F137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G137" t="inlineStr">
+      <c r="G137" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4318,9 +4980,15 @@
       <c r="F138" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="G138" t="n">
+        <v>2565</v>
+      </c>
+      <c r="H138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -4349,7 +5017,13 @@
       <c r="F139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="inlineStr">
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4380,7 +5054,13 @@
       <c r="F140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G140" t="inlineStr">
+      <c r="G140" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4411,7 +5091,13 @@
       <c r="F141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="inlineStr">
+      <c r="G141" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4442,9 +5128,15 @@
       <c r="F142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G142" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>1570</t>
         </is>
       </c>
     </row>
@@ -4473,7 +5165,13 @@
       <c r="F143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G143" t="inlineStr">
+      <c r="G143" t="n">
+        <v>1400</v>
+      </c>
+      <c r="H143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" t="inlineStr">
         <is>
           <t>1400</t>
         </is>
@@ -4504,7 +5202,13 @@
       <c r="F144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="inlineStr">
+      <c r="G144" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4535,7 +5239,13 @@
       <c r="F145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="inlineStr">
+      <c r="G145" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4566,7 +5276,13 @@
       <c r="F146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="inlineStr">
+      <c r="G146" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4597,7 +5313,13 @@
       <c r="F147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="inlineStr">
+      <c r="G147" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4628,7 +5350,13 @@
       <c r="F148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G148" t="inlineStr">
+      <c r="G148" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4659,7 +5387,13 @@
       <c r="F149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G149" t="inlineStr">
+      <c r="G149" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4690,7 +5424,13 @@
       <c r="F150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G150" t="inlineStr">
+      <c r="G150" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4721,7 +5461,13 @@
       <c r="F151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G151" t="inlineStr">
+      <c r="G151" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4752,7 +5498,13 @@
       <c r="F152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G152" t="inlineStr">
+      <c r="G152" t="n">
+        <v>0</v>
+      </c>
+      <c r="H152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4783,7 +5535,13 @@
       <c r="F153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G153" t="inlineStr">
+      <c r="G153" t="n">
+        <v>0</v>
+      </c>
+      <c r="H153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4814,7 +5572,13 @@
       <c r="F154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G154" t="inlineStr">
+      <c r="G154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4845,7 +5609,13 @@
       <c r="F155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G155" t="inlineStr">
+      <c r="G155" t="n">
+        <v>0</v>
+      </c>
+      <c r="H155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4876,7 +5646,13 @@
       <c r="F156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G156" t="inlineStr">
+      <c r="G156" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4907,7 +5683,13 @@
       <c r="F157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G157" t="inlineStr">
+      <c r="G157" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4938,7 +5720,13 @@
       <c r="F158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G158" t="inlineStr">
+      <c r="G158" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4963,9 +5751,15 @@
       <c r="F159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="G159" t="n">
+        <v>2492</v>
+      </c>
+      <c r="H159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -4988,9 +5782,15 @@
       <c r="F160" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>1678</t>
+      <c r="G160" t="n">
+        <v>1678</v>
+      </c>
+      <c r="H160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>1727</t>
         </is>
       </c>
     </row>
@@ -5013,9 +5813,44 @@
       <c r="F161" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>1357</t>
+      <c r="G161" t="n">
+        <v>1357</v>
+      </c>
+      <c r="H161" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>1467</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>59093405</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>永恒不朽6</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F162" s="3" t="inlineStr"/>
+      <c r="G162" t="inlineStr"/>
+      <c r="H162" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>2288</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-28 12:30:57
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -5826,10 +5826,8 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>59093405</t>
-        </is>
+      <c r="A162" t="n">
+        <v>59093405</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-03-29 11:30:53
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:K163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>03-27_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>03-28_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>03-28_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="I2" t="n">
+        <v>2522</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -496,6 +512,8 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" s="3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" s="3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -519,6 +537,8 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" s="3" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
+      <c r="J4" s="3" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -542,6 +562,8 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="3" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
+      <c r="J5" s="3" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -565,6 +587,8 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" s="3" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
+      <c r="J6" s="3" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -588,6 +612,8 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -611,6 +637,8 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" s="3" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -634,6 +662,8 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" s="3" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -666,9 +696,15 @@
       <c r="H10" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>3589</t>
+      <c r="I10" t="n">
+        <v>3589</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>4188</t>
         </is>
       </c>
     </row>
@@ -694,6 +730,8 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" s="3" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -726,9 +764,15 @@
       <c r="H12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>3244</t>
+      <c r="I12" t="n">
+        <v>3244</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>3602</t>
         </is>
       </c>
     </row>
@@ -763,9 +807,15 @@
       <c r="H13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>3112</t>
+      <c r="I13" t="n">
+        <v>3112</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>3443</t>
         </is>
       </c>
     </row>
@@ -800,9 +850,15 @@
       <c r="H14" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3321</t>
+      <c r="I14" t="n">
+        <v>3321</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>3774</t>
         </is>
       </c>
     </row>
@@ -837,7 +893,13 @@
       <c r="H15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" t="n">
+        <v>2520</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>2520</t>
         </is>
@@ -874,11 +936,11 @@
       <c r="H16" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>3543</t>
-        </is>
-      </c>
+      <c r="I16" t="n">
+        <v>3543</v>
+      </c>
+      <c r="J16" s="3" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -902,6 +964,8 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
+      <c r="J17" s="3" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -925,6 +989,8 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" s="3" t="inlineStr"/>
       <c r="I18" t="inlineStr"/>
+      <c r="J18" s="3" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -948,6 +1014,8 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
+      <c r="J19" s="3" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -971,6 +1039,8 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" s="3" t="inlineStr"/>
       <c r="I20" t="inlineStr"/>
+      <c r="J20" s="3" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1002,6 +1072,8 @@
       </c>
       <c r="H21" s="3" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
+      <c r="J21" s="3" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1025,6 +1097,8 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" s="3" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
+      <c r="J22" s="3" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1048,6 +1122,8 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" s="3" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
+      <c r="J23" s="3" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1080,9 +1156,15 @@
       <c r="H24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="I24" t="n">
+        <v>3440</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -1108,6 +1190,8 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" s="3" t="inlineStr"/>
       <c r="I25" t="inlineStr"/>
+      <c r="J25" s="3" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1131,6 +1215,8 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" s="3" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
+      <c r="J26" s="3" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1154,6 +1240,8 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" s="3" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
+      <c r="J27" s="3" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1177,6 +1265,8 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" s="3" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
+      <c r="J28" s="3" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1200,6 +1290,8 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" s="3" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
+      <c r="J29" s="3" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1223,6 +1315,8 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" s="3" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
+      <c r="J30" s="3" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1246,6 +1340,8 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" s="3" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
+      <c r="J31" s="3" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1269,6 +1365,8 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" s="3" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
+      <c r="J32" s="3" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1292,6 +1390,8 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
+      <c r="J33" s="3" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1315,6 +1415,8 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" s="3" t="inlineStr"/>
       <c r="I34" t="inlineStr"/>
+      <c r="J34" s="3" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1347,9 +1449,15 @@
       <c r="H35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I35" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -1384,9 +1492,15 @@
       <c r="H36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="I36" t="n">
+        <v>3316</v>
+      </c>
+      <c r="J36" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>3398</t>
         </is>
       </c>
     </row>
@@ -1412,6 +1526,8 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" s="3" t="inlineStr"/>
       <c r="I37" t="inlineStr"/>
+      <c r="J37" s="3" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1435,6 +1551,8 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" s="3" t="inlineStr"/>
       <c r="I38" t="inlineStr"/>
+      <c r="J38" s="3" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1467,9 +1585,15 @@
       <c r="H39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>3027</t>
+      <c r="I39" t="n">
+        <v>3027</v>
+      </c>
+      <c r="J39" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1628,15 @@
       <c r="H40" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>3188</t>
+      <c r="I40" t="n">
+        <v>3188</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>3516</t>
         </is>
       </c>
     </row>
@@ -1532,6 +1662,8 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" s="3" t="inlineStr"/>
       <c r="I41" t="inlineStr"/>
+      <c r="J41" s="3" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1564,9 +1696,15 @@
       <c r="H42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>3355</t>
+      <c r="I42" t="n">
+        <v>3355</v>
+      </c>
+      <c r="J42" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3698</t>
         </is>
       </c>
     </row>
@@ -1592,6 +1730,8 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" s="3" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
+      <c r="J43" s="3" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1624,9 +1764,15 @@
       <c r="H44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>3139</t>
+      <c r="I44" t="n">
+        <v>3139</v>
+      </c>
+      <c r="J44" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3326</t>
         </is>
       </c>
     </row>
@@ -1661,9 +1807,15 @@
       <c r="H45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>3138</t>
+      <c r="I45" t="n">
+        <v>3138</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3504</t>
         </is>
       </c>
     </row>
@@ -1698,7 +1850,13 @@
       <c r="H46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="I46" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1735,7 +1893,13 @@
       <c r="H47" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="I47" t="n">
+        <v>2522</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>2522</t>
         </is>
@@ -1772,7 +1936,13 @@
       <c r="H48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1809,7 +1979,13 @@
       <c r="H49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1837,6 +2013,8 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" s="3" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
+      <c r="J50" s="3" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1860,6 +2038,8 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" s="3" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
+      <c r="J51" s="3" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1892,9 +2072,15 @@
       <c r="H52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>3298</t>
+      <c r="I52" t="n">
+        <v>3298</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>3636</t>
         </is>
       </c>
     </row>
@@ -1929,9 +2115,15 @@
       <c r="H53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>3073</t>
+      <c r="I53" t="n">
+        <v>3073</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>3421</t>
         </is>
       </c>
     </row>
@@ -1957,6 +2149,8 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" s="3" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
+      <c r="J54" s="3" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1989,9 +2183,15 @@
       <c r="H55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>3388</t>
+      <c r="I55" t="n">
+        <v>3388</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3811</t>
         </is>
       </c>
     </row>
@@ -2026,9 +2226,15 @@
       <c r="H56" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="I56" t="n">
+        <v>3597</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -2063,9 +2269,15 @@
       <c r="H57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>3542</t>
+      <c r="I57" t="n">
+        <v>3542</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2100,9 +2312,15 @@
       <c r="H58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>3520</t>
+      <c r="I58" t="n">
+        <v>3520</v>
+      </c>
+      <c r="J58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3769</t>
         </is>
       </c>
     </row>
@@ -2137,9 +2355,15 @@
       <c r="H59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3525</t>
+      <c r="I59" t="n">
+        <v>3525</v>
+      </c>
+      <c r="J59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3794</t>
         </is>
       </c>
     </row>
@@ -2174,9 +2398,15 @@
       <c r="H60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>3341</t>
+      <c r="I60" t="n">
+        <v>3341</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>3848</t>
         </is>
       </c>
     </row>
@@ -2211,9 +2441,15 @@
       <c r="H61" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="I61" t="n">
+        <v>3146</v>
+      </c>
+      <c r="J61" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>3191</t>
         </is>
       </c>
     </row>
@@ -2248,9 +2484,15 @@
       <c r="H62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3525</t>
+      <c r="I62" t="n">
+        <v>3525</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -2285,9 +2527,15 @@
       <c r="H63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3296</t>
+      <c r="I63" t="n">
+        <v>3296</v>
+      </c>
+      <c r="J63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -2322,9 +2570,15 @@
       <c r="H64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>3487</t>
+      <c r="I64" t="n">
+        <v>3487</v>
+      </c>
+      <c r="J64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -2350,6 +2604,8 @@
       <c r="G65" t="inlineStr"/>
       <c r="H65" s="3" t="inlineStr"/>
       <c r="I65" t="inlineStr"/>
+      <c r="J65" s="3" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2382,9 +2638,15 @@
       <c r="H66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>3677</t>
+      <c r="I66" t="n">
+        <v>3677</v>
+      </c>
+      <c r="J66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -2419,9 +2681,15 @@
       <c r="H67" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>3092</t>
+      <c r="I67" t="n">
+        <v>3092</v>
+      </c>
+      <c r="J67" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>3350</t>
         </is>
       </c>
     </row>
@@ -2456,9 +2724,15 @@
       <c r="H68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>3445</t>
+      <c r="I68" t="n">
+        <v>3445</v>
+      </c>
+      <c r="J68" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>3772</t>
         </is>
       </c>
     </row>
@@ -2493,9 +2767,15 @@
       <c r="H69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="I69" t="n">
+        <v>3206</v>
+      </c>
+      <c r="J69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>3517</t>
         </is>
       </c>
     </row>
@@ -2530,9 +2810,15 @@
       <c r="H70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>3302</t>
+      <c r="I70" t="n">
+        <v>3302</v>
+      </c>
+      <c r="J70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -2567,9 +2853,15 @@
       <c r="H71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>2931</t>
+      <c r="I71" t="n">
+        <v>2931</v>
+      </c>
+      <c r="J71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>3408</t>
         </is>
       </c>
     </row>
@@ -2604,9 +2896,15 @@
       <c r="H72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>3381</t>
+      <c r="I72" t="n">
+        <v>3381</v>
+      </c>
+      <c r="J72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>3723</t>
         </is>
       </c>
     </row>
@@ -2641,9 +2939,15 @@
       <c r="H73" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="I73" t="n">
+        <v>2826</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2823</t>
         </is>
       </c>
     </row>
@@ -2678,7 +2982,13 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I74" t="n">
+        <v>2712</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>2712</t>
         </is>
@@ -2715,9 +3025,15 @@
       <c r="H75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="I75" t="n">
+        <v>2516</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -2752,9 +3068,15 @@
       <c r="H76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>2843</t>
+      <c r="I76" t="n">
+        <v>2843</v>
+      </c>
+      <c r="J76" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3082</t>
         </is>
       </c>
     </row>
@@ -2789,9 +3111,15 @@
       <c r="H77" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>3222</t>
+      <c r="I77" t="n">
+        <v>3222</v>
+      </c>
+      <c r="J77" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>3491</t>
         </is>
       </c>
     </row>
@@ -2826,9 +3154,15 @@
       <c r="H78" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="I78" t="n">
+        <v>3045</v>
+      </c>
+      <c r="J78" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>3266</t>
         </is>
       </c>
     </row>
@@ -2863,9 +3197,15 @@
       <c r="H79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>2907</t>
+      <c r="I79" t="n">
+        <v>2907</v>
+      </c>
+      <c r="J79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -2900,9 +3240,15 @@
       <c r="H80" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>2888</t>
+      <c r="I80" t="n">
+        <v>2888</v>
+      </c>
+      <c r="J80" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -2937,9 +3283,15 @@
       <c r="H81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="I81" t="n">
+        <v>2824</v>
+      </c>
+      <c r="J81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>3008</t>
         </is>
       </c>
     </row>
@@ -2974,9 +3326,15 @@
       <c r="H82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="I82" t="n">
+        <v>2885</v>
+      </c>
+      <c r="J82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>3121</t>
         </is>
       </c>
     </row>
@@ -3011,9 +3369,15 @@
       <c r="H83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I83" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -3048,9 +3412,15 @@
       <c r="H84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="I84" t="n">
+        <v>2510</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2504</t>
         </is>
       </c>
     </row>
@@ -3084,6 +3454,8 @@
       </c>
       <c r="H85" s="3" t="inlineStr"/>
       <c r="I85" t="inlineStr"/>
+      <c r="J85" s="3" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3116,7 +3488,13 @@
       <c r="H86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="I86" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3153,9 +3531,15 @@
       <c r="H87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>3149</t>
+      <c r="I87" t="n">
+        <v>3149</v>
+      </c>
+      <c r="J87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>3679</t>
         </is>
       </c>
     </row>
@@ -3189,6 +3573,8 @@
       </c>
       <c r="H88" s="3" t="inlineStr"/>
       <c r="I88" t="inlineStr"/>
+      <c r="J88" s="3" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3212,6 +3598,8 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" s="3" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
+      <c r="J89" s="3" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3244,9 +3632,15 @@
       <c r="H90" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>3434</t>
+      <c r="I90" t="n">
+        <v>3434</v>
+      </c>
+      <c r="J90" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>3770</t>
         </is>
       </c>
     </row>
@@ -3281,7 +3675,13 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3318,9 +3718,15 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="I92" t="n">
+        <v>2586</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2630</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3761,13 @@
       <c r="H93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="I93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3392,9 +3804,15 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="I94" t="n">
+        <v>2624</v>
+      </c>
+      <c r="J94" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -3429,9 +3847,15 @@
       <c r="H95" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>3013</t>
+      <c r="I95" t="n">
+        <v>3013</v>
+      </c>
+      <c r="J95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>3258</t>
         </is>
       </c>
     </row>
@@ -3466,9 +3890,15 @@
       <c r="H96" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="I96" t="n">
+        <v>2561</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -3503,9 +3933,15 @@
       <c r="H97" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="I97" t="n">
+        <v>3159</v>
+      </c>
+      <c r="J97" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>3385</t>
         </is>
       </c>
     </row>
@@ -3540,9 +3976,15 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="I98" t="n">
+        <v>2803</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>2849</t>
         </is>
       </c>
     </row>
@@ -3577,9 +4019,15 @@
       <c r="H99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>2908</t>
+      <c r="I99" t="n">
+        <v>2908</v>
+      </c>
+      <c r="J99" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>3046</t>
         </is>
       </c>
     </row>
@@ -3614,9 +4062,15 @@
       <c r="H100" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>2771</t>
+      <c r="I100" t="n">
+        <v>2771</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -3651,9 +4105,15 @@
       <c r="H101" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>3054</t>
+      <c r="I101" t="n">
+        <v>3054</v>
+      </c>
+      <c r="J101" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>3288</t>
         </is>
       </c>
     </row>
@@ -3688,9 +4148,15 @@
       <c r="H102" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>3076</t>
+      <c r="I102" t="n">
+        <v>3076</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>3294</t>
         </is>
       </c>
     </row>
@@ -3700,7 +4166,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>Globalking1001</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3725,9 +4191,15 @@
       <c r="H103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>2953</t>
+      <c r="I103" t="n">
+        <v>2953</v>
+      </c>
+      <c r="J103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -3762,9 +4234,15 @@
       <c r="H104" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>3023</t>
+      <c r="I104" t="n">
+        <v>3023</v>
+      </c>
+      <c r="J104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>3190</t>
         </is>
       </c>
     </row>
@@ -3799,7 +4277,13 @@
       <c r="H105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3836,9 +4320,15 @@
       <c r="H106" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="I106" t="n">
+        <v>3206</v>
+      </c>
+      <c r="J106" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>3442</t>
         </is>
       </c>
     </row>
@@ -3873,9 +4363,15 @@
       <c r="H107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>3140</t>
+      <c r="I107" t="n">
+        <v>3140</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>3430</t>
         </is>
       </c>
     </row>
@@ -3910,9 +4406,15 @@
       <c r="H108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>2929</t>
+      <c r="I108" t="n">
+        <v>2929</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>3130</t>
         </is>
       </c>
     </row>
@@ -3947,9 +4449,15 @@
       <c r="H109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="I109" t="n">
+        <v>2528</v>
+      </c>
+      <c r="J109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -3984,9 +4492,15 @@
       <c r="H110" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="I110" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J110" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>3164</t>
         </is>
       </c>
     </row>
@@ -4012,6 +4526,8 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" s="3" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
+      <c r="J111" s="3" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4044,9 +4560,15 @@
       <c r="H112" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>2674</t>
+      <c r="I112" t="n">
+        <v>2674</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>2999</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4591,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F113" s="5" t="n">
@@ -4081,9 +4603,15 @@
       <c r="H113" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="I113" t="n">
+        <v>2668</v>
+      </c>
+      <c r="J113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>2730</t>
         </is>
       </c>
     </row>
@@ -4118,7 +4646,13 @@
       <c r="H114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I114" t="inlineStr">
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4155,9 +4689,15 @@
       <c r="H115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2714</t>
+      <c r="I115" t="n">
+        <v>2714</v>
+      </c>
+      <c r="J115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>2795</t>
         </is>
       </c>
     </row>
@@ -4192,9 +4732,15 @@
       <c r="H116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2806</t>
+      <c r="I116" t="n">
+        <v>2806</v>
+      </c>
+      <c r="J116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2848</t>
         </is>
       </c>
     </row>
@@ -4228,6 +4774,8 @@
       </c>
       <c r="H117" s="3" t="inlineStr"/>
       <c r="I117" t="inlineStr"/>
+      <c r="J117" s="3" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -4251,6 +4799,8 @@
       <c r="G118" t="inlineStr"/>
       <c r="H118" s="3" t="inlineStr"/>
       <c r="I118" t="inlineStr"/>
+      <c r="J118" s="3" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -4283,9 +4833,15 @@
       <c r="H119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="I119" t="n">
+        <v>2495</v>
+      </c>
+      <c r="J119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -4320,9 +4876,15 @@
       <c r="H120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="I120" t="n">
+        <v>2535</v>
+      </c>
+      <c r="J120" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -4357,9 +4919,15 @@
       <c r="H121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I121" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -4394,9 +4962,15 @@
       <c r="H122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="I122" t="n">
+        <v>2487</v>
+      </c>
+      <c r="J122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -4431,9 +5005,15 @@
       <c r="H123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="I123" t="n">
+        <v>2494</v>
+      </c>
+      <c r="J123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -4468,9 +5048,15 @@
       <c r="H124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="I124" t="n">
+        <v>2490</v>
+      </c>
+      <c r="J124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -4505,7 +5091,13 @@
       <c r="H125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I125" t="inlineStr">
+      <c r="I125" t="n">
+        <v>0</v>
+      </c>
+      <c r="J125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4542,9 +5134,15 @@
       <c r="H126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>1497</t>
+      <c r="I126" t="n">
+        <v>1497</v>
+      </c>
+      <c r="J126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>1492</t>
         </is>
       </c>
     </row>
@@ -4579,9 +5177,15 @@
       <c r="H127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>1526</t>
+      <c r="I127" t="n">
+        <v>1526</v>
+      </c>
+      <c r="J127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>1523</t>
         </is>
       </c>
     </row>
@@ -4616,9 +5220,15 @@
       <c r="H128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>1141</t>
+      <c r="I128" t="n">
+        <v>1141</v>
+      </c>
+      <c r="J128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>1171</t>
         </is>
       </c>
     </row>
@@ -4653,7 +5263,13 @@
       <c r="H129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I129" t="inlineStr">
+      <c r="I129" t="n">
+        <v>0</v>
+      </c>
+      <c r="J129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4690,7 +5306,13 @@
       <c r="H130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I130" t="inlineStr">
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4727,7 +5349,13 @@
       <c r="H131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I131" t="inlineStr">
+      <c r="I131" t="n">
+        <v>0</v>
+      </c>
+      <c r="J131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4764,7 +5392,13 @@
       <c r="H132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I132" t="inlineStr">
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4801,7 +5435,13 @@
       <c r="H133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I133" t="inlineStr">
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4838,7 +5478,13 @@
       <c r="H134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I134" t="inlineStr">
+      <c r="I134" t="n">
+        <v>0</v>
+      </c>
+      <c r="J134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4875,9 +5521,15 @@
       <c r="H135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="I135" t="n">
+        <v>2630</v>
+      </c>
+      <c r="J135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>2653</t>
         </is>
       </c>
     </row>
@@ -4912,9 +5564,15 @@
       <c r="H136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="I136" t="n">
+        <v>2793</v>
+      </c>
+      <c r="J136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -4949,7 +5607,13 @@
       <c r="H137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4986,9 +5650,15 @@
       <c r="H138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="I138" t="n">
+        <v>2556</v>
+      </c>
+      <c r="J138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -5023,7 +5693,13 @@
       <c r="H139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I139" t="inlineStr">
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5060,7 +5736,13 @@
       <c r="H140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I140" t="inlineStr">
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5097,7 +5779,13 @@
       <c r="H141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5134,9 +5822,15 @@
       <c r="H142" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>1570</t>
+      <c r="I142" t="n">
+        <v>1570</v>
+      </c>
+      <c r="J142" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>1623</t>
         </is>
       </c>
     </row>
@@ -5171,9 +5865,15 @@
       <c r="H143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>1400</t>
+      <c r="I143" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>1399</t>
         </is>
       </c>
     </row>
@@ -5208,7 +5908,13 @@
       <c r="H144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I144" t="inlineStr">
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5245,7 +5951,13 @@
       <c r="H145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5282,7 +5994,13 @@
       <c r="H146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5319,7 +6037,13 @@
       <c r="H147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="I147" t="n">
+        <v>0</v>
+      </c>
+      <c r="J147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5356,7 +6080,13 @@
       <c r="H148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="I148" t="n">
+        <v>0</v>
+      </c>
+      <c r="J148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5393,7 +6123,13 @@
       <c r="H149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5430,7 +6166,13 @@
       <c r="H150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I150" t="inlineStr">
+      <c r="I150" t="n">
+        <v>0</v>
+      </c>
+      <c r="J150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5467,7 +6209,13 @@
       <c r="H151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I151" t="inlineStr">
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5504,7 +6252,13 @@
       <c r="H152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I152" t="inlineStr">
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5541,7 +6295,13 @@
       <c r="H153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I153" t="inlineStr">
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5578,7 +6338,13 @@
       <c r="H154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5615,7 +6381,13 @@
       <c r="H155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I155" t="inlineStr">
+      <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5652,7 +6424,13 @@
       <c r="H156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I156" t="inlineStr">
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5689,7 +6467,13 @@
       <c r="H157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5726,7 +6510,13 @@
       <c r="H158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I158" t="inlineStr">
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5757,9 +6547,15 @@
       <c r="H159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="I159" t="n">
+        <v>2542</v>
+      </c>
+      <c r="J159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -5788,9 +6584,15 @@
       <c r="H160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>1727</t>
+      <c r="I160" t="n">
+        <v>1727</v>
+      </c>
+      <c r="J160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>1724</t>
         </is>
       </c>
     </row>
@@ -5819,9 +6621,15 @@
       <c r="H161" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>1467</t>
+      <c r="I161" t="n">
+        <v>1467</v>
+      </c>
+      <c r="J161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -5846,9 +6654,46 @@
       <c r="H162" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>2288</t>
+      <c r="I162" t="n">
+        <v>2288</v>
+      </c>
+      <c r="J162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>2283</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>59095922</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>xxxx7</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr"/>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F163" s="3" t="inlineStr"/>
+      <c r="G163" t="inlineStr"/>
+      <c r="H163" s="3" t="inlineStr"/>
+      <c r="I163" t="inlineStr"/>
+      <c r="J163" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-29 20:13:01
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -6667,10 +6667,8 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>59095922</t>
-        </is>
+      <c r="A163" t="n">
+        <v>59095922</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-03-30 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K163"/>
+  <dimension ref="A1:M163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>03-28_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>03-29_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>03-29_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="K2" t="n">
+        <v>2519</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2547</t>
         </is>
       </c>
     </row>
@@ -514,6 +530,8 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" s="3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
+      <c r="L3" s="3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -539,6 +557,8 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" s="3" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
+      <c r="L4" s="3" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -564,6 +584,8 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" s="3" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
+      <c r="L5" s="3" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -589,6 +611,8 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" s="3" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" s="3" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -614,6 +638,8 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" s="3" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" s="3" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -632,13 +658,25 @@
       <c r="D8" t="n">
         <v>7589</v>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F8" s="3" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" s="3" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" s="3" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>4591</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -664,6 +702,8 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" s="3" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" s="3" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -702,9 +742,15 @@
       <c r="J10" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>4188</t>
+      <c r="K10" t="n">
+        <v>4188</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>4454</t>
         </is>
       </c>
     </row>
@@ -732,6 +778,8 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" s="3" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" s="3" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -770,9 +818,15 @@
       <c r="J12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>3602</t>
+      <c r="K12" t="n">
+        <v>3602</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3981</t>
         </is>
       </c>
     </row>
@@ -813,9 +867,15 @@
       <c r="J13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>3443</t>
+      <c r="K13" t="n">
+        <v>3443</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>3811</t>
         </is>
       </c>
     </row>
@@ -856,9 +916,15 @@
       <c r="J14" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>3774</t>
+      <c r="K14" t="n">
+        <v>3774</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -899,9 +965,15 @@
       <c r="J15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>2520</t>
+      <c r="K15" t="n">
+        <v>2520</v>
+      </c>
+      <c r="L15" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -941,6 +1013,8 @@
       </c>
       <c r="J16" s="3" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" s="3" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -959,13 +1033,25 @@
       <c r="D17" t="n">
         <v>7362</v>
       </c>
-      <c r="E17" t="inlineStr"/>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F17" s="3" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
       <c r="J17" s="3" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>4459</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -991,6 +1077,8 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" s="3" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" s="3" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1016,6 +1104,8 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" s="3" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
+      <c r="L19" s="3" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1041,6 +1131,8 @@
       <c r="I20" t="inlineStr"/>
       <c r="J20" s="3" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
+      <c r="L20" s="3" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1074,6 +1166,14 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" s="3" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>4206</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1099,6 +1199,8 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" s="3" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" s="3" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1124,6 +1226,8 @@
       <c r="I23" t="inlineStr"/>
       <c r="J23" s="3" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
+      <c r="L23" s="3" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1162,9 +1266,15 @@
       <c r="J24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="K24" t="n">
+        <v>3875</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>4184</t>
         </is>
       </c>
     </row>
@@ -1192,6 +1302,8 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" s="3" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
+      <c r="L25" s="3" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1217,6 +1329,8 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" s="3" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
+      <c r="L26" s="3" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1242,6 +1356,8 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" s="3" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" s="3" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1267,6 +1383,8 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" s="3" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" s="3" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1292,6 +1410,8 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" s="3" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
+      <c r="L29" s="3" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1317,6 +1437,8 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" s="3" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" s="3" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1342,6 +1464,8 @@
       <c r="I31" t="inlineStr"/>
       <c r="J31" s="3" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
+      <c r="L31" s="3" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1367,6 +1491,8 @@
       <c r="I32" t="inlineStr"/>
       <c r="J32" s="3" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
+      <c r="L32" s="3" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1392,6 +1518,8 @@
       <c r="I33" t="inlineStr"/>
       <c r="J33" s="3" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
+      <c r="L33" s="3" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1417,6 +1545,8 @@
       <c r="I34" t="inlineStr"/>
       <c r="J34" s="3" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
+      <c r="L34" s="3" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1455,7 +1585,13 @@
       <c r="J35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="K35" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1498,11 +1634,11 @@
       <c r="J36" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>3398</t>
-        </is>
-      </c>
+      <c r="K36" t="n">
+        <v>3398</v>
+      </c>
+      <c r="L36" s="3" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1528,6 +1664,8 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" s="3" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
+      <c r="L37" s="3" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1553,6 +1691,8 @@
       <c r="I38" t="inlineStr"/>
       <c r="J38" s="3" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
+      <c r="L38" s="3" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1591,9 +1731,15 @@
       <c r="J39" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="K39" t="n">
+        <v>3339</v>
+      </c>
+      <c r="L39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>3610</t>
         </is>
       </c>
     </row>
@@ -1634,9 +1780,15 @@
       <c r="J40" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>3516</t>
+      <c r="K40" t="n">
+        <v>3516</v>
+      </c>
+      <c r="L40" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -1664,6 +1816,8 @@
       <c r="I41" t="inlineStr"/>
       <c r="J41" s="3" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
+      <c r="L41" s="3" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1702,9 +1856,15 @@
       <c r="J42" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="K42" t="n">
+        <v>3698</v>
+      </c>
+      <c r="L42" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>3986</t>
         </is>
       </c>
     </row>
@@ -1732,6 +1892,8 @@
       <c r="I43" t="inlineStr"/>
       <c r="J43" s="3" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
+      <c r="L43" s="3" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1770,9 +1932,15 @@
       <c r="J44" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>3326</t>
+      <c r="K44" t="n">
+        <v>3326</v>
+      </c>
+      <c r="L44" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>3660</t>
         </is>
       </c>
     </row>
@@ -1813,9 +1981,15 @@
       <c r="J45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3504</t>
+      <c r="K45" t="n">
+        <v>3504</v>
+      </c>
+      <c r="L45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3780</t>
         </is>
       </c>
     </row>
@@ -1856,9 +2030,15 @@
       <c r="J46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K46" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>2843</t>
         </is>
       </c>
     </row>
@@ -1899,9 +2079,15 @@
       <c r="J47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="K47" t="n">
+        <v>2522</v>
+      </c>
+      <c r="L47" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -1942,7 +2128,13 @@
       <c r="J48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1985,7 +2177,13 @@
       <c r="J49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2015,6 +2213,8 @@
       <c r="I50" t="inlineStr"/>
       <c r="J50" s="3" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
+      <c r="L50" s="3" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2040,6 +2240,8 @@
       <c r="I51" t="inlineStr"/>
       <c r="J51" s="3" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
+      <c r="L51" s="3" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2078,9 +2280,15 @@
       <c r="J52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>3636</t>
+      <c r="K52" t="n">
+        <v>3636</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>3729</t>
         </is>
       </c>
     </row>
@@ -2121,9 +2329,15 @@
       <c r="J53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>3421</t>
+      <c r="K53" t="n">
+        <v>3421</v>
+      </c>
+      <c r="L53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>3778</t>
         </is>
       </c>
     </row>
@@ -2151,6 +2365,8 @@
       <c r="I54" t="inlineStr"/>
       <c r="J54" s="3" t="inlineStr"/>
       <c r="K54" t="inlineStr"/>
+      <c r="L54" s="3" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2189,9 +2405,15 @@
       <c r="J55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3811</t>
+      <c r="K55" t="n">
+        <v>3811</v>
+      </c>
+      <c r="L55" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>4030</t>
         </is>
       </c>
     </row>
@@ -2232,9 +2454,15 @@
       <c r="J56" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="K56" t="n">
+        <v>3998</v>
+      </c>
+      <c r="L56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>4168</t>
         </is>
       </c>
     </row>
@@ -2275,9 +2503,15 @@
       <c r="J57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="K57" t="n">
+        <v>3989</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>4056</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2552,15 @@
       <c r="J58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="K58" t="n">
+        <v>3769</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -2361,9 +2601,15 @@
       <c r="J59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3794</t>
+      <c r="K59" t="n">
+        <v>3794</v>
+      </c>
+      <c r="L59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -2404,9 +2650,15 @@
       <c r="J60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>3848</t>
+      <c r="K60" t="n">
+        <v>3848</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>3981</t>
         </is>
       </c>
     </row>
@@ -2447,9 +2699,15 @@
       <c r="J61" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>3191</t>
+      <c r="K61" t="n">
+        <v>3191</v>
+      </c>
+      <c r="L61" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -2490,9 +2748,15 @@
       <c r="J62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="K62" t="n">
+        <v>3995</v>
+      </c>
+      <c r="L62" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>4359</t>
         </is>
       </c>
     </row>
@@ -2533,9 +2797,15 @@
       <c r="J63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="K63" t="n">
+        <v>3703</v>
+      </c>
+      <c r="L63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>4097</t>
         </is>
       </c>
     </row>
@@ -2576,9 +2846,15 @@
       <c r="J64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="K64" t="n">
+        <v>4027</v>
+      </c>
+      <c r="L64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>4283</t>
         </is>
       </c>
     </row>
@@ -2606,6 +2882,8 @@
       <c r="I65" t="inlineStr"/>
       <c r="J65" s="3" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
+      <c r="L65" s="3" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2644,9 +2922,15 @@
       <c r="J66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="K66" t="n">
+        <v>3995</v>
+      </c>
+      <c r="L66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>4005</t>
         </is>
       </c>
     </row>
@@ -2687,9 +2971,15 @@
       <c r="J67" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3350</t>
+      <c r="K67" t="n">
+        <v>3350</v>
+      </c>
+      <c r="L67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>3651</t>
         </is>
       </c>
     </row>
@@ -2730,9 +3020,15 @@
       <c r="J68" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>3772</t>
+      <c r="K68" t="n">
+        <v>3772</v>
+      </c>
+      <c r="L68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -2773,9 +3069,15 @@
       <c r="J69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>3517</t>
+      <c r="K69" t="n">
+        <v>3517</v>
+      </c>
+      <c r="L69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>3843</t>
         </is>
       </c>
     </row>
@@ -2816,9 +3118,15 @@
       <c r="J70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="K70" t="n">
+        <v>3638</v>
+      </c>
+      <c r="L70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>3963</t>
         </is>
       </c>
     </row>
@@ -2859,9 +3167,15 @@
       <c r="J71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>3408</t>
+      <c r="K71" t="n">
+        <v>3408</v>
+      </c>
+      <c r="L71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>3839</t>
         </is>
       </c>
     </row>
@@ -2902,9 +3216,15 @@
       <c r="J72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>3723</t>
+      <c r="K72" t="n">
+        <v>3723</v>
+      </c>
+      <c r="L72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -2945,7 +3265,13 @@
       <c r="J73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K73" t="inlineStr">
+      <c r="K73" t="n">
+        <v>2823</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="inlineStr">
         <is>
           <t>2823</t>
         </is>
@@ -2988,9 +3314,15 @@
       <c r="J74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="K74" t="n">
+        <v>2712</v>
+      </c>
+      <c r="L74" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>2816</t>
         </is>
       </c>
     </row>
@@ -3031,9 +3363,15 @@
       <c r="J75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="K75" t="n">
+        <v>2512</v>
+      </c>
+      <c r="L75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>2508</t>
         </is>
       </c>
     </row>
@@ -3074,9 +3412,15 @@
       <c r="J76" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3082</t>
+      <c r="K76" t="n">
+        <v>3082</v>
+      </c>
+      <c r="L76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3080</t>
         </is>
       </c>
     </row>
@@ -3117,9 +3461,15 @@
       <c r="J77" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>3491</t>
+      <c r="K77" t="n">
+        <v>3491</v>
+      </c>
+      <c r="L77" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -3160,9 +3510,15 @@
       <c r="J78" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>3266</t>
+      <c r="K78" t="n">
+        <v>3266</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -3203,9 +3559,15 @@
       <c r="J79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="K79" t="n">
+        <v>3014</v>
+      </c>
+      <c r="L79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -3246,9 +3608,15 @@
       <c r="J80" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="K80" t="n">
+        <v>2938</v>
+      </c>
+      <c r="L80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>3324</t>
         </is>
       </c>
     </row>
@@ -3289,9 +3657,15 @@
       <c r="J81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>3008</t>
+      <c r="K81" t="n">
+        <v>3008</v>
+      </c>
+      <c r="L81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -3332,9 +3706,15 @@
       <c r="J82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>3121</t>
+      <c r="K82" t="n">
+        <v>3121</v>
+      </c>
+      <c r="L82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>3255</t>
         </is>
       </c>
     </row>
@@ -3375,9 +3755,15 @@
       <c r="J83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="K83" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -3418,11 +3804,11 @@
       <c r="J84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>2504</t>
-        </is>
-      </c>
+      <c r="K84" t="n">
+        <v>2504</v>
+      </c>
+      <c r="L84" s="3" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3456,6 +3842,8 @@
       <c r="I85" t="inlineStr"/>
       <c r="J85" s="3" t="inlineStr"/>
       <c r="K85" t="inlineStr"/>
+      <c r="L85" s="3" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3494,11 +3882,11 @@
       <c r="J86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
+      <c r="K86" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L86" s="3" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -3537,9 +3925,15 @@
       <c r="J87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>3679</t>
+      <c r="K87" t="n">
+        <v>3679</v>
+      </c>
+      <c r="L87" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>4171</t>
         </is>
       </c>
     </row>
@@ -3575,6 +3969,8 @@
       <c r="I88" t="inlineStr"/>
       <c r="J88" s="3" t="inlineStr"/>
       <c r="K88" t="inlineStr"/>
+      <c r="L88" s="3" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3600,6 +3996,8 @@
       <c r="I89" t="inlineStr"/>
       <c r="J89" s="3" t="inlineStr"/>
       <c r="K89" t="inlineStr"/>
+      <c r="L89" s="3" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -3638,9 +4036,15 @@
       <c r="J90" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>3770</t>
+      <c r="K90" t="n">
+        <v>3770</v>
+      </c>
+      <c r="L90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>4045</t>
         </is>
       </c>
     </row>
@@ -3681,7 +4085,13 @@
       <c r="J91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3724,9 +4134,15 @@
       <c r="J92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>2630</t>
+      <c r="K92" t="n">
+        <v>2630</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -3767,7 +4183,13 @@
       <c r="J93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr">
+      <c r="K93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3810,9 +4232,15 @@
       <c r="J94" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="K94" t="n">
+        <v>3067</v>
+      </c>
+      <c r="L94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>3117</t>
         </is>
       </c>
     </row>
@@ -3853,9 +4281,15 @@
       <c r="J95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>3258</t>
+      <c r="K95" t="n">
+        <v>3258</v>
+      </c>
+      <c r="L95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>3577</t>
         </is>
       </c>
     </row>
@@ -3896,9 +4330,15 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="K96" t="n">
+        <v>2560</v>
+      </c>
+      <c r="L96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2576</t>
         </is>
       </c>
     </row>
@@ -3939,9 +4379,15 @@
       <c r="J97" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="K97" t="inlineStr">
-        <is>
-          <t>3385</t>
+      <c r="K97" t="n">
+        <v>3385</v>
+      </c>
+      <c r="L97" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>3721</t>
         </is>
       </c>
     </row>
@@ -3982,9 +4428,15 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
-        <is>
-          <t>2849</t>
+      <c r="K98" t="n">
+        <v>2849</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -4025,9 +4477,15 @@
       <c r="J99" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>3046</t>
+      <c r="K99" t="n">
+        <v>3046</v>
+      </c>
+      <c r="L99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>3043</t>
         </is>
       </c>
     </row>
@@ -4050,7 +4508,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F100" s="5" t="n">
@@ -4068,9 +4526,15 @@
       <c r="J100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="K100" t="n">
+        <v>2762</v>
+      </c>
+      <c r="L100" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>3104</t>
         </is>
       </c>
     </row>
@@ -4111,9 +4575,15 @@
       <c r="J101" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>3288</t>
+      <c r="K101" t="n">
+        <v>3288</v>
+      </c>
+      <c r="L101" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>3503</t>
         </is>
       </c>
     </row>
@@ -4154,9 +4624,15 @@
       <c r="J102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>3294</t>
+      <c r="K102" t="n">
+        <v>3294</v>
+      </c>
+      <c r="L102" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>3493</t>
         </is>
       </c>
     </row>
@@ -4197,9 +4673,15 @@
       <c r="J103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="K103" t="n">
+        <v>3237</v>
+      </c>
+      <c r="L103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>3511</t>
         </is>
       </c>
     </row>
@@ -4240,9 +4722,15 @@
       <c r="J104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>3190</t>
+      <c r="K104" t="n">
+        <v>3190</v>
+      </c>
+      <c r="L104" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>3460</t>
         </is>
       </c>
     </row>
@@ -4283,7 +4771,13 @@
       <c r="J105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K105" t="inlineStr">
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4326,9 +4820,15 @@
       <c r="J106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>3442</t>
+      <c r="K106" t="n">
+        <v>3442</v>
+      </c>
+      <c r="L106" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>3698</t>
         </is>
       </c>
     </row>
@@ -4369,9 +4869,15 @@
       <c r="J107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>3430</t>
+      <c r="K107" t="n">
+        <v>3430</v>
+      </c>
+      <c r="L107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>3576</t>
         </is>
       </c>
     </row>
@@ -4412,9 +4918,15 @@
       <c r="J108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K108" t="inlineStr">
-        <is>
-          <t>3130</t>
+      <c r="K108" t="n">
+        <v>3130</v>
+      </c>
+      <c r="L108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>3308</t>
         </is>
       </c>
     </row>
@@ -4455,9 +4967,15 @@
       <c r="J109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K109" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="K109" t="n">
+        <v>2525</v>
+      </c>
+      <c r="L109" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>2541</t>
         </is>
       </c>
     </row>
@@ -4498,9 +5016,15 @@
       <c r="J110" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K110" t="inlineStr">
-        <is>
-          <t>3164</t>
+      <c r="K110" t="n">
+        <v>3164</v>
+      </c>
+      <c r="L110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -4528,6 +5052,8 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" s="3" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
+      <c r="L111" s="3" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4566,9 +5092,15 @@
       <c r="J112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="K112" t="n">
+        <v>2999</v>
+      </c>
+      <c r="L112" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>3213</t>
         </is>
       </c>
     </row>
@@ -4609,9 +5141,15 @@
       <c r="J113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>2730</t>
+      <c r="K113" t="n">
+        <v>2730</v>
+      </c>
+      <c r="L113" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2883</t>
         </is>
       </c>
     </row>
@@ -4652,7 +5190,13 @@
       <c r="J114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K114" t="inlineStr">
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
+      <c r="L114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4695,9 +5239,15 @@
       <c r="J115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>2795</t>
+      <c r="K115" t="n">
+        <v>2795</v>
+      </c>
+      <c r="L115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -4738,9 +5288,15 @@
       <c r="J116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2848</t>
+      <c r="K116" t="n">
+        <v>2848</v>
+      </c>
+      <c r="L116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2883</t>
         </is>
       </c>
     </row>
@@ -4776,6 +5332,8 @@
       <c r="I117" t="inlineStr"/>
       <c r="J117" s="3" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
+      <c r="L117" s="3" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -4801,6 +5359,8 @@
       <c r="I118" t="inlineStr"/>
       <c r="J118" s="3" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
+      <c r="L118" s="3" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -4839,9 +5399,15 @@
       <c r="J119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="K119" t="n">
+        <v>2487</v>
+      </c>
+      <c r="L119" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -4882,9 +5448,15 @@
       <c r="J120" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="K120" t="n">
+        <v>2536</v>
+      </c>
+      <c r="L120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -4925,9 +5497,15 @@
       <c r="J121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="K121" t="n">
+        <v>2498</v>
+      </c>
+      <c r="L121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -4968,9 +5546,15 @@
       <c r="J122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="K122" t="n">
+        <v>2526</v>
+      </c>
+      <c r="L122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -5011,9 +5595,15 @@
       <c r="J123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K123" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K123" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -5054,9 +5644,15 @@
       <c r="J124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="K124" t="n">
+        <v>2487</v>
+      </c>
+      <c r="L124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -5097,7 +5693,13 @@
       <c r="J125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K125" t="inlineStr">
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
+      <c r="L125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5140,9 +5742,15 @@
       <c r="J126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K126" t="inlineStr">
-        <is>
-          <t>1492</t>
+      <c r="K126" t="n">
+        <v>1492</v>
+      </c>
+      <c r="L126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M126" t="inlineStr">
+        <is>
+          <t>1501</t>
         </is>
       </c>
     </row>
@@ -5183,9 +5791,15 @@
       <c r="J127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K127" t="inlineStr">
-        <is>
-          <t>1523</t>
+      <c r="K127" t="n">
+        <v>1523</v>
+      </c>
+      <c r="L127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" t="inlineStr">
+        <is>
+          <t>1550</t>
         </is>
       </c>
     </row>
@@ -5226,9 +5840,15 @@
       <c r="J128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K128" t="inlineStr">
-        <is>
-          <t>1171</t>
+      <c r="K128" t="n">
+        <v>1171</v>
+      </c>
+      <c r="L128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="inlineStr">
+        <is>
+          <t>1184</t>
         </is>
       </c>
     </row>
@@ -5269,7 +5889,13 @@
       <c r="J129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K129" t="inlineStr">
+      <c r="K129" t="n">
+        <v>0</v>
+      </c>
+      <c r="L129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5312,7 +5938,13 @@
       <c r="J130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K130" t="inlineStr">
+      <c r="K130" t="n">
+        <v>0</v>
+      </c>
+      <c r="L130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5355,7 +5987,13 @@
       <c r="J131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K131" t="inlineStr">
+      <c r="K131" t="n">
+        <v>0</v>
+      </c>
+      <c r="L131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5398,7 +6036,13 @@
       <c r="J132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K132" t="inlineStr">
+      <c r="K132" t="n">
+        <v>0</v>
+      </c>
+      <c r="L132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5441,7 +6085,13 @@
       <c r="J133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K133" t="inlineStr">
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
+      <c r="L133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5484,7 +6134,13 @@
       <c r="J134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K134" t="inlineStr">
+      <c r="K134" t="n">
+        <v>0</v>
+      </c>
+      <c r="L134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5527,9 +6183,15 @@
       <c r="J135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K135" t="inlineStr">
-        <is>
-          <t>2653</t>
+      <c r="K135" t="n">
+        <v>2653</v>
+      </c>
+      <c r="L135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M135" t="inlineStr">
+        <is>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -5570,9 +6232,15 @@
       <c r="J136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="K136" t="n">
+        <v>2773</v>
+      </c>
+      <c r="L136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -5613,7 +6281,13 @@
       <c r="J137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K137" t="inlineStr">
+      <c r="K137" t="n">
+        <v>0</v>
+      </c>
+      <c r="L137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5656,9 +6330,15 @@
       <c r="J138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K138" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="K138" t="n">
+        <v>2566</v>
+      </c>
+      <c r="L138" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -5699,7 +6379,13 @@
       <c r="J139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K139" t="inlineStr">
+      <c r="K139" t="n">
+        <v>0</v>
+      </c>
+      <c r="L139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5742,7 +6428,13 @@
       <c r="J140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K140" t="inlineStr">
+      <c r="K140" t="n">
+        <v>0</v>
+      </c>
+      <c r="L140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5785,7 +6477,13 @@
       <c r="J141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K141" t="inlineStr">
+      <c r="K141" t="n">
+        <v>0</v>
+      </c>
+      <c r="L141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5828,9 +6526,15 @@
       <c r="J142" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="K142" t="inlineStr">
-        <is>
-          <t>1623</t>
+      <c r="K142" t="n">
+        <v>1623</v>
+      </c>
+      <c r="L142" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>1642</t>
         </is>
       </c>
     </row>
@@ -5871,9 +6575,15 @@
       <c r="J143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K143" t="inlineStr">
-        <is>
-          <t>1399</t>
+      <c r="K143" t="n">
+        <v>1399</v>
+      </c>
+      <c r="L143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5914,7 +6624,13 @@
       <c r="J144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K144" t="inlineStr">
+      <c r="K144" t="n">
+        <v>0</v>
+      </c>
+      <c r="L144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5957,7 +6673,13 @@
       <c r="J145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K145" t="inlineStr">
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
+      <c r="L145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6000,7 +6722,13 @@
       <c r="J146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K146" t="inlineStr">
+      <c r="K146" t="n">
+        <v>0</v>
+      </c>
+      <c r="L146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6043,7 +6771,13 @@
       <c r="J147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K147" t="inlineStr">
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
+      <c r="L147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6086,7 +6820,13 @@
       <c r="J148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K148" t="inlineStr">
+      <c r="K148" t="n">
+        <v>0</v>
+      </c>
+      <c r="L148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6129,7 +6869,13 @@
       <c r="J149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K149" t="inlineStr">
+      <c r="K149" t="n">
+        <v>0</v>
+      </c>
+      <c r="L149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6172,7 +6918,13 @@
       <c r="J150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K150" t="inlineStr">
+      <c r="K150" t="n">
+        <v>0</v>
+      </c>
+      <c r="L150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6215,7 +6967,13 @@
       <c r="J151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K151" t="inlineStr">
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6258,7 +7016,13 @@
       <c r="J152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K152" t="inlineStr">
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6301,7 +7065,13 @@
       <c r="J153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K153" t="inlineStr">
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6344,7 +7114,13 @@
       <c r="J154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K154" t="inlineStr">
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6387,7 +7163,13 @@
       <c r="J155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K155" t="inlineStr">
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6430,7 +7212,13 @@
       <c r="J156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K156" t="inlineStr">
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6473,7 +7261,13 @@
       <c r="J157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K157" t="inlineStr">
+      <c r="K157" t="n">
+        <v>0</v>
+      </c>
+      <c r="L157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6516,7 +7310,13 @@
       <c r="J158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K158" t="inlineStr">
+      <c r="K158" t="n">
+        <v>0</v>
+      </c>
+      <c r="L158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6553,9 +7353,15 @@
       <c r="J159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K159" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="K159" t="n">
+        <v>2556</v>
+      </c>
+      <c r="L159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M159" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -6590,9 +7396,15 @@
       <c r="J160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K160" t="inlineStr">
-        <is>
-          <t>1724</t>
+      <c r="K160" t="n">
+        <v>1724</v>
+      </c>
+      <c r="L160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M160" t="inlineStr">
+        <is>
+          <t>1719</t>
         </is>
       </c>
     </row>
@@ -6627,7 +7439,13 @@
       <c r="J161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K161" t="inlineStr">
+      <c r="K161" t="n">
+        <v>1500</v>
+      </c>
+      <c r="L161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -6660,9 +7478,15 @@
       <c r="J162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K162" t="inlineStr">
-        <is>
-          <t>2283</t>
+      <c r="K162" t="n">
+        <v>2283</v>
+      </c>
+      <c r="L162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>2274</t>
         </is>
       </c>
     </row>
@@ -6689,9 +7513,15 @@
       <c r="J163" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K163" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="K163" t="n">
+        <v>2498</v>
+      </c>
+      <c r="L163" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-31 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M163"/>
+  <dimension ref="A1:O165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>03-29_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>03-30_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>03-30_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,9 +510,15 @@
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>2547</t>
+      <c r="M2" t="n">
+        <v>2547</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -532,6 +548,8 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" s="3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
+      <c r="N3" s="3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -559,6 +577,8 @@
       <c r="K4" t="inlineStr"/>
       <c r="L4" s="3" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+      <c r="N4" s="3" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -577,7 +597,11 @@
       <c r="D5" t="n">
         <v>7383</v>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F5" s="3" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" s="3" t="inlineStr"/>
@@ -586,6 +610,14 @@
       <c r="K5" t="inlineStr"/>
       <c r="L5" s="3" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
+      <c r="N5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>4594</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -613,6 +645,8 @@
       <c r="K6" t="inlineStr"/>
       <c r="L6" s="3" t="inlineStr"/>
       <c r="M6" t="inlineStr"/>
+      <c r="N6" s="3" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -640,6 +674,8 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" s="3" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" s="3" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -672,9 +708,15 @@
       <c r="L8" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>4591</t>
+      <c r="M8" t="n">
+        <v>4591</v>
+      </c>
+      <c r="N8" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>5007</t>
         </is>
       </c>
     </row>
@@ -704,6 +746,8 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" s="3" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" s="3" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -748,9 +792,15 @@
       <c r="L10" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>4454</t>
+      <c r="M10" t="n">
+        <v>4454</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>4677</t>
         </is>
       </c>
     </row>
@@ -780,6 +830,8 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" s="3" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" s="3" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -824,9 +876,15 @@
       <c r="L12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>3981</t>
+      <c r="M12" t="n">
+        <v>3981</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>4276</t>
         </is>
       </c>
     </row>
@@ -873,9 +931,15 @@
       <c r="L13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>3811</t>
+      <c r="M13" t="n">
+        <v>3811</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -922,9 +986,15 @@
       <c r="L14" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="M14" t="n">
+        <v>4098</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>4387</t>
         </is>
       </c>
     </row>
@@ -971,9 +1041,15 @@
       <c r="L15" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="M15" t="n">
+        <v>2746</v>
+      </c>
+      <c r="N15" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -1015,6 +1091,8 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" s="3" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" s="3" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1047,9 +1125,15 @@
       <c r="L17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>4459</t>
+      <c r="M17" t="n">
+        <v>4459</v>
+      </c>
+      <c r="N17" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4840</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1154,11 @@
       <c r="D18" t="n">
         <v>7232</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F18" s="3" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" s="3" t="inlineStr"/>
@@ -1079,6 +1167,14 @@
       <c r="K18" t="inlineStr"/>
       <c r="L18" s="3" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
+      <c r="N18" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>5159</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1097,7 +1193,11 @@
       <c r="D19" t="n">
         <v>7103</v>
       </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F19" s="3" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" s="3" t="inlineStr"/>
@@ -1106,6 +1206,14 @@
       <c r="K19" t="inlineStr"/>
       <c r="L19" s="3" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
+      <c r="N19" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4596</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1133,6 +1241,8 @@
       <c r="K20" t="inlineStr"/>
       <c r="L20" s="3" t="inlineStr"/>
       <c r="M20" t="inlineStr"/>
+      <c r="N20" s="3" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1169,9 +1279,15 @@
       <c r="L21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>4206</t>
+      <c r="M21" t="n">
+        <v>4206</v>
+      </c>
+      <c r="N21" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>4670</t>
         </is>
       </c>
     </row>
@@ -1201,6 +1317,8 @@
       <c r="K22" t="inlineStr"/>
       <c r="L22" s="3" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
+      <c r="N22" s="3" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1219,7 +1337,11 @@
       <c r="D23" t="n">
         <v>6909</v>
       </c>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F23" s="3" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" s="3" t="inlineStr"/>
@@ -1228,6 +1350,14 @@
       <c r="K23" t="inlineStr"/>
       <c r="L23" s="3" t="inlineStr"/>
       <c r="M23" t="inlineStr"/>
+      <c r="N23" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>4883</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1272,9 +1402,15 @@
       <c r="L24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>4184</t>
+      <c r="M24" t="n">
+        <v>4184</v>
+      </c>
+      <c r="N24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>4439</t>
         </is>
       </c>
     </row>
@@ -1304,6 +1440,8 @@
       <c r="K25" t="inlineStr"/>
       <c r="L25" s="3" t="inlineStr"/>
       <c r="M25" t="inlineStr"/>
+      <c r="N25" s="3" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1331,6 +1469,8 @@
       <c r="K26" t="inlineStr"/>
       <c r="L26" s="3" t="inlineStr"/>
       <c r="M26" t="inlineStr"/>
+      <c r="N26" s="3" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1358,6 +1498,8 @@
       <c r="K27" t="inlineStr"/>
       <c r="L27" s="3" t="inlineStr"/>
       <c r="M27" t="inlineStr"/>
+      <c r="N27" s="3" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1385,6 +1527,8 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" s="3" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" s="3" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1412,6 +1556,8 @@
       <c r="K29" t="inlineStr"/>
       <c r="L29" s="3" t="inlineStr"/>
       <c r="M29" t="inlineStr"/>
+      <c r="N29" s="3" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1439,6 +1585,8 @@
       <c r="K30" t="inlineStr"/>
       <c r="L30" s="3" t="inlineStr"/>
       <c r="M30" t="inlineStr"/>
+      <c r="N30" s="3" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1466,6 +1614,8 @@
       <c r="K31" t="inlineStr"/>
       <c r="L31" s="3" t="inlineStr"/>
       <c r="M31" t="inlineStr"/>
+      <c r="N31" s="3" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1493,6 +1643,8 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" s="3" t="inlineStr"/>
       <c r="M32" t="inlineStr"/>
+      <c r="N32" s="3" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1520,6 +1672,8 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" s="3" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
+      <c r="N33" s="3" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1547,6 +1701,8 @@
       <c r="K34" t="inlineStr"/>
       <c r="L34" s="3" t="inlineStr"/>
       <c r="M34" t="inlineStr"/>
+      <c r="N34" s="3" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1591,7 +1747,13 @@
       <c r="L35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="M35" t="n">
+        <v>2516</v>
+      </c>
+      <c r="N35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1639,6 +1801,8 @@
       </c>
       <c r="L36" s="3" t="inlineStr"/>
       <c r="M36" t="inlineStr"/>
+      <c r="N36" s="3" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1666,6 +1830,8 @@
       <c r="K37" t="inlineStr"/>
       <c r="L37" s="3" t="inlineStr"/>
       <c r="M37" t="inlineStr"/>
+      <c r="N37" s="3" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1693,6 +1859,8 @@
       <c r="K38" t="inlineStr"/>
       <c r="L38" s="3" t="inlineStr"/>
       <c r="M38" t="inlineStr"/>
+      <c r="N38" s="3" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1737,9 +1905,15 @@
       <c r="L39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>3610</t>
+      <c r="M39" t="n">
+        <v>3610</v>
+      </c>
+      <c r="N39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>3885</t>
         </is>
       </c>
     </row>
@@ -1786,9 +1960,15 @@
       <c r="L40" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="M40" t="n">
+        <v>3635</v>
+      </c>
+      <c r="N40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -1818,6 +1998,8 @@
       <c r="K41" t="inlineStr"/>
       <c r="L41" s="3" t="inlineStr"/>
       <c r="M41" t="inlineStr"/>
+      <c r="N41" s="3" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1862,9 +2044,15 @@
       <c r="L42" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>3986</t>
+      <c r="M42" t="n">
+        <v>3986</v>
+      </c>
+      <c r="N42" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -1894,6 +2082,8 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" s="3" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" s="3" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1938,9 +2128,15 @@
       <c r="L44" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>3660</t>
+      <c r="M44" t="n">
+        <v>3660</v>
+      </c>
+      <c r="N44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>3659</t>
         </is>
       </c>
     </row>
@@ -1987,9 +2183,15 @@
       <c r="L45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3780</t>
+      <c r="M45" t="n">
+        <v>3780</v>
+      </c>
+      <c r="N45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -2036,7 +2238,13 @@
       <c r="L46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M46" t="inlineStr">
+      <c r="M46" t="n">
+        <v>2843</v>
+      </c>
+      <c r="N46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O46" t="inlineStr">
         <is>
           <t>2843</t>
         </is>
@@ -2085,9 +2293,15 @@
       <c r="L47" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="M47" t="n">
+        <v>2521</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2348,13 @@
       <c r="L48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M48" t="inlineStr">
+      <c r="M48" t="n">
+        <v>0</v>
+      </c>
+      <c r="N48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2183,7 +2403,13 @@
       <c r="L49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="M49" t="n">
+        <v>0</v>
+      </c>
+      <c r="N49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2206,7 +2432,11 @@
       <c r="D50" t="n">
         <v>6585</v>
       </c>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F50" s="3" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" s="3" t="inlineStr"/>
@@ -2215,6 +2445,14 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" s="3" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
+      <c r="N50" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>4338</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2242,6 +2480,8 @@
       <c r="K51" t="inlineStr"/>
       <c r="L51" s="3" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
+      <c r="N51" s="3" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2286,9 +2526,15 @@
       <c r="L52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>3729</t>
+      <c r="M52" t="n">
+        <v>3729</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>4033</t>
         </is>
       </c>
     </row>
@@ -2335,9 +2581,15 @@
       <c r="L53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>3778</t>
+      <c r="M53" t="n">
+        <v>3778</v>
+      </c>
+      <c r="N53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>4023</t>
         </is>
       </c>
     </row>
@@ -2367,6 +2619,8 @@
       <c r="K54" t="inlineStr"/>
       <c r="L54" s="3" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
+      <c r="N54" s="3" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2411,9 +2665,15 @@
       <c r="L55" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>4030</t>
+      <c r="M55" t="n">
+        <v>4030</v>
+      </c>
+      <c r="N55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>4252</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2720,15 @@
       <c r="L56" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>4168</t>
+      <c r="M56" t="n">
+        <v>4168</v>
+      </c>
+      <c r="N56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>4336</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2775,15 @@
       <c r="L57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="M57" t="n">
+        <v>4056</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>4212</t>
         </is>
       </c>
     </row>
@@ -2558,9 +2830,15 @@
       <c r="L58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="M58" t="n">
+        <v>3993</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>4187</t>
         </is>
       </c>
     </row>
@@ -2607,9 +2885,15 @@
       <c r="L59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="M59" t="n">
+        <v>3991</v>
+      </c>
+      <c r="N59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -2656,9 +2940,15 @@
       <c r="L60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>3981</t>
+      <c r="M60" t="n">
+        <v>3981</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>4054</t>
         </is>
       </c>
     </row>
@@ -2705,9 +2995,15 @@
       <c r="L61" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="M61" t="n">
+        <v>3320</v>
+      </c>
+      <c r="N61" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -2754,9 +3050,15 @@
       <c r="L62" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>4359</t>
+      <c r="M62" t="n">
+        <v>4359</v>
+      </c>
+      <c r="N62" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -2803,9 +3105,15 @@
       <c r="L63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>4097</t>
+      <c r="M63" t="n">
+        <v>4097</v>
+      </c>
+      <c r="N63" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>4300</t>
         </is>
       </c>
     </row>
@@ -2852,9 +3160,15 @@
       <c r="L64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>4283</t>
+      <c r="M64" t="n">
+        <v>4283</v>
+      </c>
+      <c r="N64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>4513</t>
         </is>
       </c>
     </row>
@@ -2884,6 +3198,8 @@
       <c r="K65" t="inlineStr"/>
       <c r="L65" s="3" t="inlineStr"/>
       <c r="M65" t="inlineStr"/>
+      <c r="N65" s="3" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -2928,9 +3244,15 @@
       <c r="L66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>4005</t>
+      <c r="M66" t="n">
+        <v>4005</v>
+      </c>
+      <c r="N66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>4483</t>
         </is>
       </c>
     </row>
@@ -2977,9 +3299,15 @@
       <c r="L67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3651</t>
+      <c r="M67" t="n">
+        <v>3651</v>
+      </c>
+      <c r="N67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>3919</t>
         </is>
       </c>
     </row>
@@ -3026,9 +3354,15 @@
       <c r="L68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="M68" t="n">
+        <v>3984</v>
+      </c>
+      <c r="N68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -3075,9 +3409,15 @@
       <c r="L69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M69" t="inlineStr">
-        <is>
-          <t>3843</t>
+      <c r="M69" t="n">
+        <v>3843</v>
+      </c>
+      <c r="N69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -3124,9 +3464,15 @@
       <c r="L70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>3963</t>
+      <c r="M70" t="n">
+        <v>3963</v>
+      </c>
+      <c r="N70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>4067</t>
         </is>
       </c>
     </row>
@@ -3173,9 +3519,15 @@
       <c r="L71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>3839</t>
+      <c r="M71" t="n">
+        <v>3839</v>
+      </c>
+      <c r="N71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>4202</t>
         </is>
       </c>
     </row>
@@ -3222,9 +3574,15 @@
       <c r="L72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>4071</t>
+      <c r="M72" t="n">
+        <v>4071</v>
+      </c>
+      <c r="N72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -3271,9 +3629,15 @@
       <c r="L73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="M73" t="n">
+        <v>2823</v>
+      </c>
+      <c r="N73" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -3320,9 +3684,15 @@
       <c r="L74" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>2816</t>
+      <c r="M74" t="n">
+        <v>2816</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>2810</t>
         </is>
       </c>
     </row>
@@ -3369,9 +3739,15 @@
       <c r="L75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>2508</t>
+      <c r="M75" t="n">
+        <v>2508</v>
+      </c>
+      <c r="N75" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -3418,9 +3794,15 @@
       <c r="L76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>3080</t>
+      <c r="M76" t="n">
+        <v>3080</v>
+      </c>
+      <c r="N76" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -3467,9 +3849,15 @@
       <c r="L77" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="M77" t="n">
+        <v>3779</v>
+      </c>
+      <c r="N77" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -3516,9 +3904,15 @@
       <c r="L78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="M78" t="n">
+        <v>3312</v>
+      </c>
+      <c r="N78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>3512</t>
         </is>
       </c>
     </row>
@@ -3565,9 +3959,15 @@
       <c r="L79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="M79" t="n">
+        <v>3233</v>
+      </c>
+      <c r="N79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>3447</t>
         </is>
       </c>
     </row>
@@ -3614,9 +4014,15 @@
       <c r="L80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>3324</t>
+      <c r="M80" t="n">
+        <v>3324</v>
+      </c>
+      <c r="N80" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>3559</t>
         </is>
       </c>
     </row>
@@ -3663,9 +4069,15 @@
       <c r="L81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>3135</t>
+      <c r="M81" t="n">
+        <v>3135</v>
+      </c>
+      <c r="N81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>3293</t>
         </is>
       </c>
     </row>
@@ -3712,9 +4124,15 @@
       <c r="L82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>3255</t>
+      <c r="M82" t="n">
+        <v>3255</v>
+      </c>
+      <c r="N82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -3761,9 +4179,15 @@
       <c r="L83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="M83" t="n">
+        <v>2532</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>2531</t>
         </is>
       </c>
     </row>
@@ -3809,6 +4233,8 @@
       </c>
       <c r="L84" s="3" t="inlineStr"/>
       <c r="M84" t="inlineStr"/>
+      <c r="N84" s="3" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -3844,6 +4270,8 @@
       <c r="K85" t="inlineStr"/>
       <c r="L85" s="3" t="inlineStr"/>
       <c r="M85" t="inlineStr"/>
+      <c r="N85" s="3" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -3887,6 +4315,8 @@
       </c>
       <c r="L86" s="3" t="inlineStr"/>
       <c r="M86" t="inlineStr"/>
+      <c r="N86" s="3" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -3931,7 +4361,13 @@
       <c r="L87" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M87" t="inlineStr">
+      <c r="M87" t="n">
+        <v>4171</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
         <is>
           <t>4171</t>
         </is>
@@ -3971,6 +4407,8 @@
       <c r="K88" t="inlineStr"/>
       <c r="L88" s="3" t="inlineStr"/>
       <c r="M88" t="inlineStr"/>
+      <c r="N88" s="3" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -3998,6 +4436,8 @@
       <c r="K89" t="inlineStr"/>
       <c r="L89" s="3" t="inlineStr"/>
       <c r="M89" t="inlineStr"/>
+      <c r="N89" s="3" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4042,9 +4482,15 @@
       <c r="L90" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>4045</t>
+      <c r="M90" t="n">
+        <v>4045</v>
+      </c>
+      <c r="N90" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>4270</t>
         </is>
       </c>
     </row>
@@ -4091,7 +4537,13 @@
       <c r="L91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4140,9 +4592,15 @@
       <c r="L92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="M92" t="n">
+        <v>2624</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -4189,7 +4647,13 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
+      <c r="M93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4238,9 +4702,15 @@
       <c r="L94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>3117</t>
+      <c r="M94" t="n">
+        <v>3117</v>
+      </c>
+      <c r="N94" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -4287,9 +4757,15 @@
       <c r="L95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M95" t="inlineStr">
-        <is>
-          <t>3577</t>
+      <c r="M95" t="n">
+        <v>3577</v>
+      </c>
+      <c r="N95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>3806</t>
         </is>
       </c>
     </row>
@@ -4336,9 +4812,15 @@
       <c r="L96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2576</t>
+      <c r="M96" t="n">
+        <v>2576</v>
+      </c>
+      <c r="N96" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>2869</t>
         </is>
       </c>
     </row>
@@ -4385,9 +4867,15 @@
       <c r="L97" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="M97" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="M97" t="n">
+        <v>3721</v>
+      </c>
+      <c r="N97" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>3887</t>
         </is>
       </c>
     </row>
@@ -4434,9 +4922,15 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="M98" t="n">
+        <v>2899</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>2911</t>
         </is>
       </c>
     </row>
@@ -4483,9 +4977,15 @@
       <c r="L99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>3043</t>
+      <c r="M99" t="n">
+        <v>3043</v>
+      </c>
+      <c r="N99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>3086</t>
         </is>
       </c>
     </row>
@@ -4532,9 +5032,15 @@
       <c r="L100" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>3104</t>
+      <c r="M100" t="n">
+        <v>3104</v>
+      </c>
+      <c r="N100" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>3459</t>
         </is>
       </c>
     </row>
@@ -4581,9 +5087,15 @@
       <c r="L101" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>3503</t>
+      <c r="M101" t="n">
+        <v>3503</v>
+      </c>
+      <c r="N101" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O101" t="inlineStr">
+        <is>
+          <t>3937</t>
         </is>
       </c>
     </row>
@@ -4630,9 +5142,15 @@
       <c r="L102" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>3493</t>
+      <c r="M102" t="n">
+        <v>3493</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="inlineStr">
+        <is>
+          <t>3670</t>
         </is>
       </c>
     </row>
@@ -4679,9 +5197,15 @@
       <c r="L103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>3511</t>
+      <c r="M103" t="n">
+        <v>3511</v>
+      </c>
+      <c r="N103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O103" t="inlineStr">
+        <is>
+          <t>3756</t>
         </is>
       </c>
     </row>
@@ -4728,9 +5252,15 @@
       <c r="L104" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M104" t="inlineStr">
-        <is>
-          <t>3460</t>
+      <c r="M104" t="n">
+        <v>3460</v>
+      </c>
+      <c r="N104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -4777,7 +5307,13 @@
       <c r="L105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4826,9 +5362,15 @@
       <c r="L106" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M106" t="inlineStr">
-        <is>
-          <t>3698</t>
+      <c r="M106" t="n">
+        <v>3698</v>
+      </c>
+      <c r="N106" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>3933</t>
         </is>
       </c>
     </row>
@@ -4875,9 +5417,15 @@
       <c r="L107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M107" t="inlineStr">
-        <is>
-          <t>3576</t>
+      <c r="M107" t="n">
+        <v>3576</v>
+      </c>
+      <c r="N107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>3874</t>
         </is>
       </c>
     </row>
@@ -4924,9 +5472,15 @@
       <c r="L108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M108" t="inlineStr">
-        <is>
-          <t>3308</t>
+      <c r="M108" t="n">
+        <v>3308</v>
+      </c>
+      <c r="N108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>3589</t>
         </is>
       </c>
     </row>
@@ -4973,9 +5527,15 @@
       <c r="L109" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>2541</t>
+      <c r="M109" t="n">
+        <v>2541</v>
+      </c>
+      <c r="N109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -5022,9 +5582,15 @@
       <c r="L110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>3428</t>
+      <c r="M110" t="n">
+        <v>3428</v>
+      </c>
+      <c r="N110" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O110" t="inlineStr">
+        <is>
+          <t>3649</t>
         </is>
       </c>
     </row>
@@ -5054,6 +5620,8 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" s="3" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
+      <c r="N111" s="3" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5098,9 +5666,15 @@
       <c r="L112" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>3213</t>
+      <c r="M112" t="n">
+        <v>3213</v>
+      </c>
+      <c r="N112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -5147,9 +5721,15 @@
       <c r="L113" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>2883</t>
+      <c r="M113" t="n">
+        <v>2883</v>
+      </c>
+      <c r="N113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -5196,7 +5776,13 @@
       <c r="L114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M114" t="inlineStr">
+      <c r="M114" t="n">
+        <v>0</v>
+      </c>
+      <c r="N114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5245,9 +5831,15 @@
       <c r="L115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="M115" t="n">
+        <v>2856</v>
+      </c>
+      <c r="N115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -5294,9 +5886,15 @@
       <c r="L116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2883</t>
+      <c r="M116" t="n">
+        <v>2883</v>
+      </c>
+      <c r="N116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -5334,6 +5932,8 @@
       <c r="K117" t="inlineStr"/>
       <c r="L117" s="3" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
+      <c r="N117" s="3" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -5361,6 +5961,8 @@
       <c r="K118" t="inlineStr"/>
       <c r="L118" s="3" t="inlineStr"/>
       <c r="M118" t="inlineStr"/>
+      <c r="N118" s="3" t="inlineStr"/>
+      <c r="O118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -5405,9 +6007,15 @@
       <c r="L119" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>2796</t>
+      <c r="M119" t="n">
+        <v>2796</v>
+      </c>
+      <c r="N119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -5454,9 +6062,15 @@
       <c r="L120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="M120" t="n">
+        <v>2528</v>
+      </c>
+      <c r="N120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -5503,9 +6117,15 @@
       <c r="L121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>2513</t>
+      <c r="M121" t="n">
+        <v>2513</v>
+      </c>
+      <c r="N121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -5552,9 +6172,15 @@
       <c r="L122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="M122" t="n">
+        <v>2550</v>
+      </c>
+      <c r="N122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -5601,11 +6227,11 @@
       <c r="L123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M123" t="inlineStr">
-        <is>
-          <t>2497</t>
-        </is>
-      </c>
+      <c r="M123" t="n">
+        <v>2497</v>
+      </c>
+      <c r="N123" s="3" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -5650,9 +6276,15 @@
       <c r="L124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="M124" t="n">
+        <v>2484</v>
+      </c>
+      <c r="N124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -5699,7 +6331,13 @@
       <c r="L125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M125" t="inlineStr">
+      <c r="M125" t="n">
+        <v>0</v>
+      </c>
+      <c r="N125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5748,9 +6386,15 @@
       <c r="L126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M126" t="inlineStr">
-        <is>
-          <t>1501</t>
+      <c r="M126" t="n">
+        <v>1501</v>
+      </c>
+      <c r="N126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O126" t="inlineStr">
+        <is>
+          <t>1496</t>
         </is>
       </c>
     </row>
@@ -5797,9 +6441,15 @@
       <c r="L127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M127" t="inlineStr">
-        <is>
-          <t>1550</t>
+      <c r="M127" t="n">
+        <v>1550</v>
+      </c>
+      <c r="N127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>1576</t>
         </is>
       </c>
     </row>
@@ -5846,9 +6496,15 @@
       <c r="L128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M128" t="inlineStr">
-        <is>
-          <t>1184</t>
+      <c r="M128" t="n">
+        <v>1184</v>
+      </c>
+      <c r="N128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O128" t="inlineStr">
+        <is>
+          <t>1181</t>
         </is>
       </c>
     </row>
@@ -5895,7 +6551,13 @@
       <c r="L129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M129" t="inlineStr">
+      <c r="M129" t="n">
+        <v>0</v>
+      </c>
+      <c r="N129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5944,7 +6606,13 @@
       <c r="L130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M130" t="inlineStr">
+      <c r="M130" t="n">
+        <v>0</v>
+      </c>
+      <c r="N130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5993,7 +6661,13 @@
       <c r="L131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M131" t="inlineStr">
+      <c r="M131" t="n">
+        <v>0</v>
+      </c>
+      <c r="N131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6042,7 +6716,13 @@
       <c r="L132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M132" t="inlineStr">
+      <c r="M132" t="n">
+        <v>0</v>
+      </c>
+      <c r="N132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6091,7 +6771,13 @@
       <c r="L133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M133" t="inlineStr">
+      <c r="M133" t="n">
+        <v>0</v>
+      </c>
+      <c r="N133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6140,7 +6826,13 @@
       <c r="L134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M134" t="inlineStr">
+      <c r="M134" t="n">
+        <v>0</v>
+      </c>
+      <c r="N134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6189,9 +6881,15 @@
       <c r="L135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M135" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="M135" t="n">
+        <v>2647</v>
+      </c>
+      <c r="N135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -6238,9 +6936,15 @@
       <c r="L136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>2981</t>
+      <c r="M136" t="n">
+        <v>2981</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6991,13 @@
       <c r="L137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M137" t="inlineStr">
+      <c r="M137" t="n">
+        <v>0</v>
+      </c>
+      <c r="N137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6336,9 +7046,15 @@
       <c r="L138" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="M138" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="M138" t="n">
+        <v>2587</v>
+      </c>
+      <c r="N138" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -6385,7 +7101,13 @@
       <c r="L139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M139" t="inlineStr">
+      <c r="M139" t="n">
+        <v>0</v>
+      </c>
+      <c r="N139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6434,7 +7156,13 @@
       <c r="L140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M140" t="inlineStr">
+      <c r="M140" t="n">
+        <v>0</v>
+      </c>
+      <c r="N140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6483,9 +7211,15 @@
       <c r="L141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M141" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M141" t="n">
+        <v>0</v>
+      </c>
+      <c r="N141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -6532,9 +7266,15 @@
       <c r="L142" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="M142" t="inlineStr">
-        <is>
-          <t>1642</t>
+      <c r="M142" t="n">
+        <v>1642</v>
+      </c>
+      <c r="N142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>1658</t>
         </is>
       </c>
     </row>
@@ -6581,7 +7321,13 @@
       <c r="L143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M143" t="inlineStr">
+      <c r="M143" t="n">
+        <v>0</v>
+      </c>
+      <c r="N143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6630,7 +7376,13 @@
       <c r="L144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M144" t="inlineStr">
+      <c r="M144" t="n">
+        <v>0</v>
+      </c>
+      <c r="N144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6679,7 +7431,13 @@
       <c r="L145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M145" t="inlineStr">
+      <c r="M145" t="n">
+        <v>0</v>
+      </c>
+      <c r="N145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6728,7 +7486,13 @@
       <c r="L146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M146" t="inlineStr">
+      <c r="M146" t="n">
+        <v>0</v>
+      </c>
+      <c r="N146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6777,7 +7541,13 @@
       <c r="L147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M147" t="inlineStr">
+      <c r="M147" t="n">
+        <v>0</v>
+      </c>
+      <c r="N147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6826,7 +7596,13 @@
       <c r="L148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M148" t="inlineStr">
+      <c r="M148" t="n">
+        <v>0</v>
+      </c>
+      <c r="N148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6875,7 +7651,13 @@
       <c r="L149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M149" t="inlineStr">
+      <c r="M149" t="n">
+        <v>0</v>
+      </c>
+      <c r="N149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6924,7 +7706,13 @@
       <c r="L150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M150" t="inlineStr">
+      <c r="M150" t="n">
+        <v>0</v>
+      </c>
+      <c r="N150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6973,7 +7761,13 @@
       <c r="L151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M151" t="inlineStr">
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7022,7 +7816,13 @@
       <c r="L152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M152" t="inlineStr">
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7071,7 +7871,13 @@
       <c r="L153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M153" t="inlineStr">
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7120,7 +7926,13 @@
       <c r="L154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M154" t="inlineStr">
+      <c r="M154" t="n">
+        <v>0</v>
+      </c>
+      <c r="N154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7169,7 +7981,13 @@
       <c r="L155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M155" t="inlineStr">
+      <c r="M155" t="n">
+        <v>0</v>
+      </c>
+      <c r="N155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7218,7 +8036,13 @@
       <c r="L156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M156" t="inlineStr">
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7267,7 +8091,13 @@
       <c r="L157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M157" t="inlineStr">
+      <c r="M157" t="n">
+        <v>0</v>
+      </c>
+      <c r="N157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7316,7 +8146,13 @@
       <c r="L158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M158" t="inlineStr">
+      <c r="M158" t="n">
+        <v>0</v>
+      </c>
+      <c r="N158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7359,9 +8195,15 @@
       <c r="L159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M159" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="M159" t="n">
+        <v>2552</v>
+      </c>
+      <c r="N159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O159" t="inlineStr">
+        <is>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -7402,9 +8244,15 @@
       <c r="L160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M160" t="inlineStr">
-        <is>
-          <t>1719</t>
+      <c r="M160" t="n">
+        <v>1719</v>
+      </c>
+      <c r="N160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>1717</t>
         </is>
       </c>
     </row>
@@ -7445,7 +8293,13 @@
       <c r="L161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M161" t="inlineStr">
+      <c r="M161" t="n">
+        <v>1500</v>
+      </c>
+      <c r="N161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O161" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -7484,9 +8338,15 @@
       <c r="L162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M162" t="inlineStr">
-        <is>
-          <t>2274</t>
+      <c r="M162" t="n">
+        <v>2274</v>
+      </c>
+      <c r="N162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>2264</t>
         </is>
       </c>
     </row>
@@ -7519,9 +8379,85 @@
       <c r="L163" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M163" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="M163" t="n">
+        <v>2592</v>
+      </c>
+      <c r="N163" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>2766</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>59083984</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>战神哥606</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr"/>
+      <c r="D164" t="inlineStr"/>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F164" s="3" t="inlineStr"/>
+      <c r="G164" t="inlineStr"/>
+      <c r="H164" s="3" t="inlineStr"/>
+      <c r="I164" t="inlineStr"/>
+      <c r="J164" s="3" t="inlineStr"/>
+      <c r="K164" t="inlineStr"/>
+      <c r="L164" s="3" t="inlineStr"/>
+      <c r="M164" t="inlineStr"/>
+      <c r="N164" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O164" t="inlineStr">
+        <is>
+          <t>1638</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>27484940</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>66666zgx</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr"/>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F165" s="3" t="inlineStr"/>
+      <c r="G165" t="inlineStr"/>
+      <c r="H165" s="3" t="inlineStr"/>
+      <c r="I165" t="inlineStr"/>
+      <c r="J165" s="3" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" s="3" t="inlineStr"/>
+      <c r="M165" t="inlineStr"/>
+      <c r="N165" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="O165" t="inlineStr">
+        <is>
+          <t>4922</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-03-31 16:49:25
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -8392,10 +8392,8 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>59083984</t>
-        </is>
+      <c r="A164" t="n">
+        <v>59083984</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -8427,10 +8425,8 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>27484940</t>
-        </is>
+      <c r="A165" t="n">
+        <v>27484940</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-04-01 11:31:02
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O165"/>
+  <dimension ref="A1:Q166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>03-30_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>03-31_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>03-31_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,9 +526,15 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="O2" t="n">
+        <v>2561</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>2558</t>
         </is>
       </c>
     </row>
@@ -550,6 +566,8 @@
       <c r="M3" t="inlineStr"/>
       <c r="N3" s="3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
+      <c r="P3" s="3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -579,6 +597,8 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" s="3" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" s="3" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -613,9 +633,15 @@
       <c r="N5" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="O5" t="n">
+        <v>4594</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>4901</t>
         </is>
       </c>
     </row>
@@ -647,6 +673,8 @@
       <c r="M6" t="inlineStr"/>
       <c r="N6" s="3" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
+      <c r="P6" s="3" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -676,6 +704,8 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" s="3" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" s="3" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -714,9 +744,15 @@
       <c r="N8" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>5007</t>
+      <c r="O8" t="n">
+        <v>5007</v>
+      </c>
+      <c r="P8" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>5453</t>
         </is>
       </c>
     </row>
@@ -748,6 +784,8 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" s="3" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" s="3" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -798,9 +836,15 @@
       <c r="N10" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>4677</t>
+      <c r="O10" t="n">
+        <v>4677</v>
+      </c>
+      <c r="P10" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>5050</t>
         </is>
       </c>
     </row>
@@ -832,6 +876,8 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" s="3" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" s="3" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -882,9 +928,15 @@
       <c r="N12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>4276</t>
+      <c r="O12" t="n">
+        <v>4276</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>4476</t>
         </is>
       </c>
     </row>
@@ -937,9 +989,15 @@
       <c r="N13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>4152</t>
+      <c r="O13" t="n">
+        <v>4152</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>4479</t>
         </is>
       </c>
     </row>
@@ -992,9 +1050,15 @@
       <c r="N14" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>4387</t>
+      <c r="O14" t="n">
+        <v>4387</v>
+      </c>
+      <c r="P14" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>4599</t>
         </is>
       </c>
     </row>
@@ -1047,9 +1111,15 @@
       <c r="N15" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>3659</t>
+      <c r="O15" t="n">
+        <v>3659</v>
+      </c>
+      <c r="P15" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -1093,6 +1163,8 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" s="3" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1131,9 +1203,15 @@
       <c r="N17" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>4840</t>
+      <c r="O17" t="n">
+        <v>4840</v>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>5213</t>
         </is>
       </c>
     </row>
@@ -1170,9 +1248,15 @@
       <c r="N18" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>5159</t>
+      <c r="O18" t="n">
+        <v>5159</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>5382</t>
         </is>
       </c>
     </row>
@@ -1209,9 +1293,15 @@
       <c r="N19" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>4596</t>
+      <c r="O19" t="n">
+        <v>4596</v>
+      </c>
+      <c r="P19" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>4871</t>
         </is>
       </c>
     </row>
@@ -1243,6 +1333,8 @@
       <c r="M20" t="inlineStr"/>
       <c r="N20" s="3" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
+      <c r="P20" s="3" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1285,9 +1377,15 @@
       <c r="N21" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>4670</t>
+      <c r="O21" t="n">
+        <v>4670</v>
+      </c>
+      <c r="P21" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>5041</t>
         </is>
       </c>
     </row>
@@ -1319,6 +1417,8 @@
       <c r="M22" t="inlineStr"/>
       <c r="N22" s="3" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
+      <c r="P22" s="3" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1353,9 +1453,15 @@
       <c r="N23" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>4883</t>
+      <c r="O23" t="n">
+        <v>4883</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>5202</t>
         </is>
       </c>
     </row>
@@ -1408,9 +1514,15 @@
       <c r="N24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>4439</t>
+      <c r="O24" t="n">
+        <v>4439</v>
+      </c>
+      <c r="P24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4693</t>
         </is>
       </c>
     </row>
@@ -1442,6 +1554,8 @@
       <c r="M25" t="inlineStr"/>
       <c r="N25" s="3" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
+      <c r="P25" s="3" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1471,6 +1585,8 @@
       <c r="M26" t="inlineStr"/>
       <c r="N26" s="3" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
+      <c r="P26" s="3" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1500,6 +1616,8 @@
       <c r="M27" t="inlineStr"/>
       <c r="N27" s="3" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
+      <c r="P27" s="3" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1529,6 +1647,8 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" s="3" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
+      <c r="P28" s="3" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1558,6 +1678,8 @@
       <c r="M29" t="inlineStr"/>
       <c r="N29" s="3" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
+      <c r="P29" s="3" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1587,6 +1709,8 @@
       <c r="M30" t="inlineStr"/>
       <c r="N30" s="3" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
+      <c r="P30" s="3" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1616,6 +1740,8 @@
       <c r="M31" t="inlineStr"/>
       <c r="N31" s="3" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
+      <c r="P31" s="3" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1645,6 +1771,8 @@
       <c r="M32" t="inlineStr"/>
       <c r="N32" s="3" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
+      <c r="P32" s="3" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1674,6 +1802,8 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" s="3" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" s="3" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1703,6 +1833,8 @@
       <c r="M34" t="inlineStr"/>
       <c r="N34" s="3" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
+      <c r="P34" s="3" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1753,7 +1885,13 @@
       <c r="N35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O35" t="inlineStr">
+      <c r="O35" t="n">
+        <v>2516</v>
+      </c>
+      <c r="P35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1803,6 +1941,8 @@
       <c r="M36" t="inlineStr"/>
       <c r="N36" s="3" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
+      <c r="P36" s="3" t="inlineStr"/>
+      <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1832,6 +1972,8 @@
       <c r="M37" t="inlineStr"/>
       <c r="N37" s="3" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
+      <c r="P37" s="3" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1861,6 +2003,8 @@
       <c r="M38" t="inlineStr"/>
       <c r="N38" s="3" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
+      <c r="P38" s="3" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1911,9 +2055,15 @@
       <c r="N39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>3885</t>
+      <c r="O39" t="n">
+        <v>3885</v>
+      </c>
+      <c r="P39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -1966,9 +2116,15 @@
       <c r="N40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>3949</t>
+      <c r="O40" t="n">
+        <v>3949</v>
+      </c>
+      <c r="P40" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>4096</t>
         </is>
       </c>
     </row>
@@ -2000,6 +2156,8 @@
       <c r="M41" t="inlineStr"/>
       <c r="N41" s="3" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
+      <c r="P41" s="3" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2050,9 +2208,15 @@
       <c r="N42" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="O42" t="n">
+        <v>4106</v>
+      </c>
+      <c r="P42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -2084,6 +2248,8 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" s="3" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
+      <c r="P43" s="3" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2134,9 +2300,15 @@
       <c r="N44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>3659</t>
+      <c r="O44" t="n">
+        <v>3659</v>
+      </c>
+      <c r="P44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>4043</t>
         </is>
       </c>
     </row>
@@ -2189,9 +2361,15 @@
       <c r="N45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="O45" t="n">
+        <v>3991</v>
+      </c>
+      <c r="P45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>4171</t>
         </is>
       </c>
     </row>
@@ -2244,7 +2422,13 @@
       <c r="N46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O46" t="inlineStr">
+      <c r="O46" t="n">
+        <v>2843</v>
+      </c>
+      <c r="P46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="inlineStr">
         <is>
           <t>2843</t>
         </is>
@@ -2299,9 +2483,15 @@
       <c r="N47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="O47" t="n">
+        <v>2537</v>
+      </c>
+      <c r="P47" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -2354,7 +2544,13 @@
       <c r="N48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O48" t="inlineStr">
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2409,7 +2605,13 @@
       <c r="N49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O49" t="inlineStr">
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2448,9 +2650,15 @@
       <c r="N50" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>4338</t>
+      <c r="O50" t="n">
+        <v>4338</v>
+      </c>
+      <c r="P50" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>4550</t>
         </is>
       </c>
     </row>
@@ -2482,6 +2690,8 @@
       <c r="M51" t="inlineStr"/>
       <c r="N51" s="3" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
+      <c r="P51" s="3" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2532,9 +2742,15 @@
       <c r="N52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>4033</t>
+      <c r="O52" t="n">
+        <v>4033</v>
+      </c>
+      <c r="P52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>4345</t>
         </is>
       </c>
     </row>
@@ -2587,9 +2803,15 @@
       <c r="N53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>4023</t>
+      <c r="O53" t="n">
+        <v>4023</v>
+      </c>
+      <c r="P53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>4196</t>
         </is>
       </c>
     </row>
@@ -2621,6 +2843,8 @@
       <c r="M54" t="inlineStr"/>
       <c r="N54" s="3" t="inlineStr"/>
       <c r="O54" t="inlineStr"/>
+      <c r="P54" s="3" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2671,9 +2895,15 @@
       <c r="N55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>4252</t>
+      <c r="O55" t="n">
+        <v>4252</v>
+      </c>
+      <c r="P55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>4503</t>
         </is>
       </c>
     </row>
@@ -2726,9 +2956,15 @@
       <c r="N56" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>4336</t>
+      <c r="O56" t="n">
+        <v>4336</v>
+      </c>
+      <c r="P56" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>4600</t>
         </is>
       </c>
     </row>
@@ -2781,9 +3017,15 @@
       <c r="N57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>4212</t>
+      <c r="O57" t="n">
+        <v>4212</v>
+      </c>
+      <c r="P57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>4302</t>
         </is>
       </c>
     </row>
@@ -2836,9 +3078,15 @@
       <c r="N58" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>4187</t>
+      <c r="O58" t="n">
+        <v>4187</v>
+      </c>
+      <c r="P58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -2891,9 +3139,15 @@
       <c r="N59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>4152</t>
+      <c r="O59" t="n">
+        <v>4152</v>
+      </c>
+      <c r="P59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>4150</t>
         </is>
       </c>
     </row>
@@ -2946,9 +3200,15 @@
       <c r="N60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>4054</t>
+      <c r="O60" t="n">
+        <v>4054</v>
+      </c>
+      <c r="P60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>4324</t>
         </is>
       </c>
     </row>
@@ -3001,9 +3261,15 @@
       <c r="N61" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="O61" t="n">
+        <v>3451</v>
+      </c>
+      <c r="P61" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>3583</t>
         </is>
       </c>
     </row>
@@ -3056,9 +3322,15 @@
       <c r="N62" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>4627</t>
+      <c r="O62" t="n">
+        <v>4627</v>
+      </c>
+      <c r="P62" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>4856</t>
         </is>
       </c>
     </row>
@@ -3111,9 +3383,15 @@
       <c r="N63" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>4300</t>
+      <c r="O63" t="n">
+        <v>4300</v>
+      </c>
+      <c r="P63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>4593</t>
         </is>
       </c>
     </row>
@@ -3166,9 +3444,15 @@
       <c r="N64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>4513</t>
+      <c r="O64" t="n">
+        <v>4513</v>
+      </c>
+      <c r="P64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>4728</t>
         </is>
       </c>
     </row>
@@ -3200,6 +3484,8 @@
       <c r="M65" t="inlineStr"/>
       <c r="N65" s="3" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" s="3" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3250,9 +3536,15 @@
       <c r="N66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>4483</t>
+      <c r="O66" t="n">
+        <v>4483</v>
+      </c>
+      <c r="P66" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>4429</t>
         </is>
       </c>
     </row>
@@ -3305,9 +3597,15 @@
       <c r="N67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>3919</t>
+      <c r="O67" t="n">
+        <v>3919</v>
+      </c>
+      <c r="P67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -3360,9 +3658,15 @@
       <c r="N68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>4082</t>
+      <c r="O68" t="n">
+        <v>4082</v>
+      </c>
+      <c r="P68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>4286</t>
         </is>
       </c>
     </row>
@@ -3415,9 +3719,15 @@
       <c r="N69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="O69" t="n">
+        <v>3987</v>
+      </c>
+      <c r="P69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>4121</t>
         </is>
       </c>
     </row>
@@ -3470,9 +3780,15 @@
       <c r="N70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>4067</t>
+      <c r="O70" t="n">
+        <v>4067</v>
+      </c>
+      <c r="P70" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>4182</t>
         </is>
       </c>
     </row>
@@ -3525,9 +3841,15 @@
       <c r="N71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>4202</t>
+      <c r="O71" t="n">
+        <v>4202</v>
+      </c>
+      <c r="P71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -3580,9 +3902,15 @@
       <c r="N72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="O72" t="n">
+        <v>4050</v>
+      </c>
+      <c r="P72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>4224</t>
         </is>
       </c>
     </row>
@@ -3635,9 +3963,15 @@
       <c r="N73" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>2870</t>
+      <c r="O73" t="n">
+        <v>2870</v>
+      </c>
+      <c r="P73" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>3205</t>
         </is>
       </c>
     </row>
@@ -3690,9 +4024,15 @@
       <c r="N74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>2810</t>
+      <c r="O74" t="n">
+        <v>2810</v>
+      </c>
+      <c r="P74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -3745,9 +4085,15 @@
       <c r="N75" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="O75" t="n">
+        <v>2609</v>
+      </c>
+      <c r="P75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>3089</t>
         </is>
       </c>
     </row>
@@ -3800,9 +4146,15 @@
       <c r="N76" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="O76" t="n">
+        <v>3369</v>
+      </c>
+      <c r="P76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -3855,9 +4207,15 @@
       <c r="N77" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="O77" t="n">
+        <v>3991</v>
+      </c>
+      <c r="P77" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>4087</t>
         </is>
       </c>
     </row>
@@ -3910,9 +4268,15 @@
       <c r="N78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>3512</t>
+      <c r="O78" t="n">
+        <v>3512</v>
+      </c>
+      <c r="P78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>3692</t>
         </is>
       </c>
     </row>
@@ -3965,9 +4329,15 @@
       <c r="N79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>3447</t>
+      <c r="O79" t="n">
+        <v>3447</v>
+      </c>
+      <c r="P79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>3571</t>
         </is>
       </c>
     </row>
@@ -4020,9 +4390,15 @@
       <c r="N80" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>3559</t>
+      <c r="O80" t="n">
+        <v>3559</v>
+      </c>
+      <c r="P80" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>3710</t>
         </is>
       </c>
     </row>
@@ -4075,9 +4451,15 @@
       <c r="N81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>3293</t>
+      <c r="O81" t="n">
+        <v>3293</v>
+      </c>
+      <c r="P81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>3482</t>
         </is>
       </c>
     </row>
@@ -4130,9 +4512,15 @@
       <c r="N82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>3394</t>
+      <c r="O82" t="n">
+        <v>3394</v>
+      </c>
+      <c r="P82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>3566</t>
         </is>
       </c>
     </row>
@@ -4185,9 +4573,15 @@
       <c r="N83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>2531</t>
+      <c r="O83" t="n">
+        <v>2531</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -4235,6 +4629,8 @@
       <c r="M84" t="inlineStr"/>
       <c r="N84" s="3" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
+      <c r="P84" s="3" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4272,6 +4668,8 @@
       <c r="M85" t="inlineStr"/>
       <c r="N85" s="3" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
+      <c r="P85" s="3" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4317,6 +4715,8 @@
       <c r="M86" t="inlineStr"/>
       <c r="N86" s="3" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
+      <c r="P86" s="3" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4367,9 +4767,15 @@
       <c r="N87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>4171</t>
+      <c r="O87" t="n">
+        <v>4171</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>4187</t>
         </is>
       </c>
     </row>
@@ -4409,6 +4815,8 @@
       <c r="M88" t="inlineStr"/>
       <c r="N88" s="3" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
+      <c r="P88" s="3" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4438,6 +4846,8 @@
       <c r="M89" t="inlineStr"/>
       <c r="N89" s="3" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
+      <c r="P89" s="3" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4488,9 +4898,15 @@
       <c r="N90" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>4270</t>
+      <c r="O90" t="n">
+        <v>4270</v>
+      </c>
+      <c r="P90" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>4491</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4959,13 @@
       <c r="N91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O91" t="inlineStr">
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4598,9 +5020,15 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="O92" t="n">
+        <v>2619</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -4653,7 +5081,13 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
+      <c r="O93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4708,9 +5142,15 @@
       <c r="N94" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="O94" t="n">
+        <v>3623</v>
+      </c>
+      <c r="P94" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>4079</t>
         </is>
       </c>
     </row>
@@ -4763,9 +5203,15 @@
       <c r="N95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>3806</t>
+      <c r="O95" t="n">
+        <v>3806</v>
+      </c>
+      <c r="P95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>4058</t>
         </is>
       </c>
     </row>
@@ -4818,9 +5264,15 @@
       <c r="N96" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>2869</t>
+      <c r="O96" t="n">
+        <v>2869</v>
+      </c>
+      <c r="P96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -4873,9 +5325,15 @@
       <c r="N97" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>3887</t>
+      <c r="O97" t="n">
+        <v>3887</v>
+      </c>
+      <c r="P97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>3939</t>
         </is>
       </c>
     </row>
@@ -4928,9 +5386,15 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="O98" t="n">
+        <v>2911</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>2940</t>
         </is>
       </c>
     </row>
@@ -4983,9 +5447,15 @@
       <c r="N99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>3086</t>
+      <c r="O99" t="n">
+        <v>3086</v>
+      </c>
+      <c r="P99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>3207</t>
         </is>
       </c>
     </row>
@@ -5038,9 +5508,15 @@
       <c r="N100" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>3459</t>
+      <c r="O100" t="n">
+        <v>3459</v>
+      </c>
+      <c r="P100" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>3655</t>
         </is>
       </c>
     </row>
@@ -5093,9 +5569,15 @@
       <c r="N101" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>3937</t>
+      <c r="O101" t="n">
+        <v>3937</v>
+      </c>
+      <c r="P101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>4130</t>
         </is>
       </c>
     </row>
@@ -5148,9 +5630,15 @@
       <c r="N102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>3670</t>
+      <c r="O102" t="n">
+        <v>3670</v>
+      </c>
+      <c r="P102" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -5203,9 +5691,15 @@
       <c r="N103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>3756</t>
+      <c r="O103" t="n">
+        <v>3756</v>
+      </c>
+      <c r="P103" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>3980</t>
         </is>
       </c>
     </row>
@@ -5258,9 +5752,15 @@
       <c r="N104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="O104" t="n">
+        <v>3635</v>
+      </c>
+      <c r="P104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>3951</t>
         </is>
       </c>
     </row>
@@ -5313,7 +5813,13 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5368,9 +5874,15 @@
       <c r="N106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>3933</t>
+      <c r="O106" t="n">
+        <v>3933</v>
+      </c>
+      <c r="P106" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -5423,9 +5935,15 @@
       <c r="N107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>3874</t>
+      <c r="O107" t="n">
+        <v>3874</v>
+      </c>
+      <c r="P107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>3981</t>
         </is>
       </c>
     </row>
@@ -5478,9 +5996,15 @@
       <c r="N108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>3589</t>
+      <c r="O108" t="n">
+        <v>3589</v>
+      </c>
+      <c r="P108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>3894</t>
         </is>
       </c>
     </row>
@@ -5533,7 +6057,13 @@
       <c r="N109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O109" t="inlineStr">
+      <c r="O109" t="n">
+        <v>2540</v>
+      </c>
+      <c r="P109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
         <is>
           <t>2540</t>
         </is>
@@ -5588,9 +6118,15 @@
       <c r="N110" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O110" t="inlineStr">
-        <is>
-          <t>3649</t>
+      <c r="O110" t="n">
+        <v>3649</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>3821</t>
         </is>
       </c>
     </row>
@@ -5622,6 +6158,8 @@
       <c r="M111" t="inlineStr"/>
       <c r="N111" s="3" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
+      <c r="P111" s="3" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5672,9 +6210,15 @@
       <c r="N112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>3469</t>
+      <c r="O112" t="n">
+        <v>3469</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>3696</t>
         </is>
       </c>
     </row>
@@ -5727,9 +6271,15 @@
       <c r="N113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="O113" t="n">
+        <v>2990</v>
+      </c>
+      <c r="P113" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>3119</t>
         </is>
       </c>
     </row>
@@ -5782,7 +6332,13 @@
       <c r="N114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
+      <c r="O114" t="n">
+        <v>0</v>
+      </c>
+      <c r="P114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5837,9 +6393,15 @@
       <c r="N115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="O115" t="n">
+        <v>2916</v>
+      </c>
+      <c r="P115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -5892,9 +6454,15 @@
       <c r="N116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="O116" t="n">
+        <v>2928</v>
+      </c>
+      <c r="P116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2941</t>
         </is>
       </c>
     </row>
@@ -5934,6 +6502,8 @@
       <c r="M117" t="inlineStr"/>
       <c r="N117" s="3" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
+      <c r="P117" s="3" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -5963,6 +6533,8 @@
       <c r="M118" t="inlineStr"/>
       <c r="N118" s="3" t="inlineStr"/>
       <c r="O118" t="inlineStr"/>
+      <c r="P118" s="3" t="inlineStr"/>
+      <c r="Q118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -6013,9 +6585,15 @@
       <c r="N119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>2786</t>
+      <c r="O119" t="n">
+        <v>2786</v>
+      </c>
+      <c r="P119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -6068,9 +6646,15 @@
       <c r="N120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="O120" t="n">
+        <v>2524</v>
+      </c>
+      <c r="P120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2824</t>
         </is>
       </c>
     </row>
@@ -6123,9 +6707,15 @@
       <c r="N121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="O121" t="n">
+        <v>2579</v>
+      </c>
+      <c r="P121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -6178,9 +6768,15 @@
       <c r="N122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="O122" t="n">
+        <v>2544</v>
+      </c>
+      <c r="P122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>2617</t>
         </is>
       </c>
     </row>
@@ -6232,6 +6828,8 @@
       </c>
       <c r="N123" s="3" t="inlineStr"/>
       <c r="O123" t="inlineStr"/>
+      <c r="P123" s="3" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -6282,9 +6880,15 @@
       <c r="N124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="O124" t="n">
+        <v>2497</v>
+      </c>
+      <c r="P124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6941,13 @@
       <c r="N125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O125" t="inlineStr">
+      <c r="O125" t="n">
+        <v>0</v>
+      </c>
+      <c r="P125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6392,9 +7002,15 @@
       <c r="N126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O126" t="inlineStr">
-        <is>
-          <t>1496</t>
+      <c r="O126" t="n">
+        <v>1496</v>
+      </c>
+      <c r="P126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>1490</t>
         </is>
       </c>
     </row>
@@ -6447,9 +7063,15 @@
       <c r="N127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O127" t="inlineStr">
-        <is>
-          <t>1576</t>
+      <c r="O127" t="n">
+        <v>1576</v>
+      </c>
+      <c r="P127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>1574</t>
         </is>
       </c>
     </row>
@@ -6502,9 +7124,15 @@
       <c r="N128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O128" t="inlineStr">
-        <is>
-          <t>1181</t>
+      <c r="O128" t="n">
+        <v>1181</v>
+      </c>
+      <c r="P128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q128" t="inlineStr">
+        <is>
+          <t>1180</t>
         </is>
       </c>
     </row>
@@ -6557,7 +7185,13 @@
       <c r="N129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O129" t="inlineStr">
+      <c r="O129" t="n">
+        <v>0</v>
+      </c>
+      <c r="P129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6612,7 +7246,13 @@
       <c r="N130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O130" t="inlineStr">
+      <c r="O130" t="n">
+        <v>0</v>
+      </c>
+      <c r="P130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6667,7 +7307,13 @@
       <c r="N131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O131" t="inlineStr">
+      <c r="O131" t="n">
+        <v>0</v>
+      </c>
+      <c r="P131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6722,7 +7368,13 @@
       <c r="N132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O132" t="inlineStr">
+      <c r="O132" t="n">
+        <v>0</v>
+      </c>
+      <c r="P132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6777,7 +7429,13 @@
       <c r="N133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O133" t="inlineStr">
+      <c r="O133" t="n">
+        <v>0</v>
+      </c>
+      <c r="P133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6832,7 +7490,13 @@
       <c r="N134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O134" t="inlineStr">
+      <c r="O134" t="n">
+        <v>0</v>
+      </c>
+      <c r="P134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6887,9 +7551,15 @@
       <c r="N135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O135" t="inlineStr">
-        <is>
-          <t>2656</t>
+      <c r="O135" t="n">
+        <v>2656</v>
+      </c>
+      <c r="P135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -6942,9 +7612,15 @@
       <c r="N136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="O136" t="n">
+        <v>2963</v>
+      </c>
+      <c r="P136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -6997,7 +7673,13 @@
       <c r="N137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O137" t="inlineStr">
+      <c r="O137" t="n">
+        <v>0</v>
+      </c>
+      <c r="P137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7052,9 +7734,15 @@
       <c r="N138" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="O138" t="inlineStr">
-        <is>
-          <t>2712</t>
+      <c r="O138" t="n">
+        <v>2712</v>
+      </c>
+      <c r="P138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -7107,7 +7795,13 @@
       <c r="N139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O139" t="inlineStr">
+      <c r="O139" t="n">
+        <v>0</v>
+      </c>
+      <c r="P139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7162,7 +7856,13 @@
       <c r="N140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O140" t="inlineStr">
+      <c r="O140" t="n">
+        <v>0</v>
+      </c>
+      <c r="P140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7217,7 +7917,13 @@
       <c r="N141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O141" t="inlineStr">
+      <c r="O141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -7272,9 +7978,15 @@
       <c r="N142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O142" t="inlineStr">
-        <is>
-          <t>1658</t>
+      <c r="O142" t="n">
+        <v>1658</v>
+      </c>
+      <c r="P142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>1657</t>
         </is>
       </c>
     </row>
@@ -7327,7 +8039,13 @@
       <c r="N143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O143" t="inlineStr">
+      <c r="O143" t="n">
+        <v>0</v>
+      </c>
+      <c r="P143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7382,7 +8100,13 @@
       <c r="N144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O144" t="inlineStr">
+      <c r="O144" t="n">
+        <v>0</v>
+      </c>
+      <c r="P144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7437,7 +8161,13 @@
       <c r="N145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O145" t="inlineStr">
+      <c r="O145" t="n">
+        <v>0</v>
+      </c>
+      <c r="P145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7492,7 +8222,13 @@
       <c r="N146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O146" t="inlineStr">
+      <c r="O146" t="n">
+        <v>0</v>
+      </c>
+      <c r="P146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7547,7 +8283,13 @@
       <c r="N147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O147" t="inlineStr">
+      <c r="O147" t="n">
+        <v>0</v>
+      </c>
+      <c r="P147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7602,7 +8344,13 @@
       <c r="N148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O148" t="inlineStr">
+      <c r="O148" t="n">
+        <v>0</v>
+      </c>
+      <c r="P148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7657,7 +8405,13 @@
       <c r="N149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O149" t="inlineStr">
+      <c r="O149" t="n">
+        <v>0</v>
+      </c>
+      <c r="P149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7712,7 +8466,13 @@
       <c r="N150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O150" t="inlineStr">
+      <c r="O150" t="n">
+        <v>0</v>
+      </c>
+      <c r="P150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7767,9 +8527,15 @@
       <c r="N151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O151" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q151" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -7822,7 +8588,13 @@
       <c r="N152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O152" t="inlineStr">
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7877,7 +8649,13 @@
       <c r="N153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O153" t="inlineStr">
+      <c r="O153" t="n">
+        <v>0</v>
+      </c>
+      <c r="P153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7932,7 +8710,13 @@
       <c r="N154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O154" t="inlineStr">
+      <c r="O154" t="n">
+        <v>0</v>
+      </c>
+      <c r="P154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7987,7 +8771,13 @@
       <c r="N155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O155" t="inlineStr">
+      <c r="O155" t="n">
+        <v>0</v>
+      </c>
+      <c r="P155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8042,7 +8832,13 @@
       <c r="N156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O156" t="inlineStr">
+      <c r="O156" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8097,7 +8893,13 @@
       <c r="N157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O157" t="inlineStr">
+      <c r="O157" t="n">
+        <v>0</v>
+      </c>
+      <c r="P157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8152,7 +8954,13 @@
       <c r="N158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O158" t="inlineStr">
+      <c r="O158" t="n">
+        <v>0</v>
+      </c>
+      <c r="P158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8201,9 +9009,15 @@
       <c r="N159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O159" t="inlineStr">
-        <is>
-          <t>2575</t>
+      <c r="O159" t="n">
+        <v>2575</v>
+      </c>
+      <c r="P159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -8250,9 +9064,15 @@
       <c r="N160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O160" t="inlineStr">
-        <is>
-          <t>1717</t>
+      <c r="O160" t="n">
+        <v>1717</v>
+      </c>
+      <c r="P160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" t="inlineStr">
+        <is>
+          <t>1728</t>
         </is>
       </c>
     </row>
@@ -8299,9 +9119,15 @@
       <c r="N161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O161" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="O161" t="n">
+        <v>1500</v>
+      </c>
+      <c r="P161" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q161" t="inlineStr">
+        <is>
+          <t>1556</t>
         </is>
       </c>
     </row>
@@ -8344,9 +9170,15 @@
       <c r="N162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O162" t="inlineStr">
-        <is>
-          <t>2264</t>
+      <c r="O162" t="n">
+        <v>2264</v>
+      </c>
+      <c r="P162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>2301</t>
         </is>
       </c>
     </row>
@@ -8385,9 +9217,15 @@
       <c r="N163" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="O163" t="inlineStr">
-        <is>
-          <t>2766</t>
+      <c r="O163" t="n">
+        <v>2766</v>
+      </c>
+      <c r="P163" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -8418,9 +9256,15 @@
       <c r="N164" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="O164" t="inlineStr">
-        <is>
-          <t>1638</t>
+      <c r="O164" t="n">
+        <v>1638</v>
+      </c>
+      <c r="P164" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q164" t="inlineStr">
+        <is>
+          <t>1737</t>
         </is>
       </c>
     </row>
@@ -8451,9 +9295,52 @@
       <c r="N165" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="O165" t="inlineStr">
-        <is>
-          <t>4922</t>
+      <c r="O165" t="n">
+        <v>4922</v>
+      </c>
+      <c r="P165" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>5173</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>59080634</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Chlove</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr"/>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F166" s="3" t="inlineStr"/>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" s="3" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" s="3" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" s="3" t="inlineStr"/>
+      <c r="M166" t="inlineStr"/>
+      <c r="N166" s="3" t="inlineStr"/>
+      <c r="O166" t="inlineStr"/>
+      <c r="P166" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q166" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-01 18:30:08
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -9308,10 +9308,8 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>59080634</t>
-        </is>
+      <c r="A166" t="n">
+        <v>59080634</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-04-03 16:48:02
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q166"/>
+  <dimension ref="A1:S166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>03-31_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>04-02_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>04-02_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,9 +542,15 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>2558</t>
+      <c r="Q2" t="n">
+        <v>2558</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -568,6 +584,8 @@
       <c r="O3" t="inlineStr"/>
       <c r="P3" s="3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
+      <c r="R3" s="3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -599,6 +617,8 @@
       <c r="O4" t="inlineStr"/>
       <c r="P4" s="3" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
+      <c r="R4" s="3" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -639,9 +659,15 @@
       <c r="P5" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>4901</t>
+      <c r="Q5" t="n">
+        <v>4901</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>5464</t>
         </is>
       </c>
     </row>
@@ -675,6 +701,8 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" s="3" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
+      <c r="R6" s="3" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -706,6 +734,8 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" s="3" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" s="3" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -750,9 +780,15 @@
       <c r="P8" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>5453</t>
+      <c r="Q8" t="n">
+        <v>5453</v>
+      </c>
+      <c r="R8" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>5923</t>
         </is>
       </c>
     </row>
@@ -786,6 +822,8 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" s="3" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" s="3" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -842,9 +880,15 @@
       <c r="P10" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>5050</t>
+      <c r="Q10" t="n">
+        <v>5050</v>
+      </c>
+      <c r="R10" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>5845</t>
         </is>
       </c>
     </row>
@@ -865,7 +909,11 @@
       <c r="D11" t="n">
         <v>7062</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
       <c r="F11" s="3" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr"/>
@@ -878,6 +926,14 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" s="3" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>5381</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -934,9 +990,15 @@
       <c r="P12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>4476</t>
+      <c r="Q12" t="n">
+        <v>4476</v>
+      </c>
+      <c r="R12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>4958</t>
         </is>
       </c>
     </row>
@@ -995,9 +1057,15 @@
       <c r="P13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>4479</t>
+      <c r="Q13" t="n">
+        <v>4479</v>
+      </c>
+      <c r="R13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>5018</t>
         </is>
       </c>
     </row>
@@ -1056,9 +1124,15 @@
       <c r="P14" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>4599</t>
+      <c r="Q14" t="n">
+        <v>4599</v>
+      </c>
+      <c r="R14" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>5109</t>
         </is>
       </c>
     </row>
@@ -1117,9 +1191,15 @@
       <c r="P15" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="Q15" t="n">
+        <v>4267</v>
+      </c>
+      <c r="R15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>4429</t>
         </is>
       </c>
     </row>
@@ -1165,6 +1245,8 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" s="3" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
+      <c r="R16" s="3" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1209,9 +1291,15 @@
       <c r="P17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>5213</t>
+      <c r="Q17" t="n">
+        <v>5213</v>
+      </c>
+      <c r="R17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>5854</t>
         </is>
       </c>
     </row>
@@ -1254,9 +1342,15 @@
       <c r="P18" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>5382</t>
+      <c r="Q18" t="n">
+        <v>5382</v>
+      </c>
+      <c r="R18" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>6069</t>
         </is>
       </c>
     </row>
@@ -1299,11 +1393,11 @@
       <c r="P19" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>4871</t>
-        </is>
-      </c>
+      <c r="Q19" t="n">
+        <v>4871</v>
+      </c>
+      <c r="R19" s="3" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1335,6 +1429,8 @@
       <c r="O20" t="inlineStr"/>
       <c r="P20" s="3" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
+      <c r="R20" s="3" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1383,9 +1479,15 @@
       <c r="P21" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>5041</t>
+      <c r="Q21" t="n">
+        <v>5041</v>
+      </c>
+      <c r="R21" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>5681</t>
         </is>
       </c>
     </row>
@@ -1419,6 +1521,8 @@
       <c r="O22" t="inlineStr"/>
       <c r="P22" s="3" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
+      <c r="R22" s="3" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1459,9 +1563,15 @@
       <c r="P23" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>5202</t>
+      <c r="Q23" t="n">
+        <v>5202</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>5753</t>
         </is>
       </c>
     </row>
@@ -1520,9 +1630,15 @@
       <c r="P24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>4693</t>
+      <c r="Q24" t="n">
+        <v>4693</v>
+      </c>
+      <c r="R24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>5164</t>
         </is>
       </c>
     </row>
@@ -1556,6 +1672,8 @@
       <c r="O25" t="inlineStr"/>
       <c r="P25" s="3" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
+      <c r="R25" s="3" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1587,6 +1705,8 @@
       <c r="O26" t="inlineStr"/>
       <c r="P26" s="3" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
+      <c r="R26" s="3" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1618,6 +1738,8 @@
       <c r="O27" t="inlineStr"/>
       <c r="P27" s="3" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
+      <c r="R27" s="3" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1649,6 +1771,8 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" s="3" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
+      <c r="R28" s="3" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1680,6 +1804,8 @@
       <c r="O29" t="inlineStr"/>
       <c r="P29" s="3" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
+      <c r="R29" s="3" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1711,6 +1837,8 @@
       <c r="O30" t="inlineStr"/>
       <c r="P30" s="3" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
+      <c r="R30" s="3" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1742,6 +1870,8 @@
       <c r="O31" t="inlineStr"/>
       <c r="P31" s="3" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
+      <c r="R31" s="3" t="inlineStr"/>
+      <c r="S31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1773,6 +1903,8 @@
       <c r="O32" t="inlineStr"/>
       <c r="P32" s="3" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
+      <c r="R32" s="3" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1804,6 +1936,8 @@
       <c r="O33" t="inlineStr"/>
       <c r="P33" s="3" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
+      <c r="R33" s="3" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1835,6 +1969,8 @@
       <c r="O34" t="inlineStr"/>
       <c r="P34" s="3" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
+      <c r="R34" s="3" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1891,9 +2027,15 @@
       <c r="P35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="Q35" t="n">
+        <v>2516</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -1943,6 +2085,8 @@
       <c r="O36" t="inlineStr"/>
       <c r="P36" s="3" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
+      <c r="R36" s="3" t="inlineStr"/>
+      <c r="S36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1974,6 +2118,8 @@
       <c r="O37" t="inlineStr"/>
       <c r="P37" s="3" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
+      <c r="R37" s="3" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2005,6 +2151,8 @@
       <c r="O38" t="inlineStr"/>
       <c r="P38" s="3" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
+      <c r="R38" s="3" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2061,9 +2209,15 @@
       <c r="P39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="Q39" t="n">
+        <v>3984</v>
+      </c>
+      <c r="R39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>4236</t>
         </is>
       </c>
     </row>
@@ -2122,9 +2276,15 @@
       <c r="P40" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>4096</t>
+      <c r="Q40" t="n">
+        <v>4096</v>
+      </c>
+      <c r="R40" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>4301</t>
         </is>
       </c>
     </row>
@@ -2158,6 +2318,8 @@
       <c r="O41" t="inlineStr"/>
       <c r="P41" s="3" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
+      <c r="R41" s="3" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2214,9 +2376,15 @@
       <c r="P42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>4258</t>
+      <c r="Q42" t="n">
+        <v>4258</v>
+      </c>
+      <c r="R42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>4616</t>
         </is>
       </c>
     </row>
@@ -2250,6 +2418,8 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" s="3" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
+      <c r="R43" s="3" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2306,9 +2476,15 @@
       <c r="P44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>4043</t>
+      <c r="Q44" t="n">
+        <v>4043</v>
+      </c>
+      <c r="R44" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>4372</t>
         </is>
       </c>
     </row>
@@ -2367,9 +2543,15 @@
       <c r="P45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>4171</t>
+      <c r="Q45" t="n">
+        <v>4171</v>
+      </c>
+      <c r="R45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4396</t>
         </is>
       </c>
     </row>
@@ -2428,9 +2610,15 @@
       <c r="P46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>2843</t>
+      <c r="Q46" t="n">
+        <v>2843</v>
+      </c>
+      <c r="R46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>3066</t>
         </is>
       </c>
     </row>
@@ -2489,9 +2677,15 @@
       <c r="P47" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="Q47" t="n">
+        <v>2998</v>
+      </c>
+      <c r="R47" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>3349</t>
         </is>
       </c>
     </row>
@@ -2550,7 +2744,13 @@
       <c r="P48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr">
+      <c r="Q48" t="n">
+        <v>0</v>
+      </c>
+      <c r="R48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2611,7 +2811,13 @@
       <c r="P49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q49" t="inlineStr">
+      <c r="Q49" t="n">
+        <v>0</v>
+      </c>
+      <c r="R49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2656,11 +2862,11 @@
       <c r="P50" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>4550</t>
-        </is>
-      </c>
+      <c r="Q50" t="n">
+        <v>4550</v>
+      </c>
+      <c r="R50" s="3" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2692,6 +2898,8 @@
       <c r="O51" t="inlineStr"/>
       <c r="P51" s="3" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
+      <c r="R51" s="3" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2748,9 +2956,15 @@
       <c r="P52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>4345</t>
+      <c r="Q52" t="n">
+        <v>4345</v>
+      </c>
+      <c r="R52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>4796</t>
         </is>
       </c>
     </row>
@@ -2809,9 +3023,15 @@
       <c r="P53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>4196</t>
+      <c r="Q53" t="n">
+        <v>4196</v>
+      </c>
+      <c r="R53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>4615</t>
         </is>
       </c>
     </row>
@@ -2845,6 +3065,8 @@
       <c r="O54" t="inlineStr"/>
       <c r="P54" s="3" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
+      <c r="R54" s="3" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -2901,9 +3123,15 @@
       <c r="P55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>4503</t>
+      <c r="Q55" t="n">
+        <v>4503</v>
+      </c>
+      <c r="R55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>4907</t>
         </is>
       </c>
     </row>
@@ -2962,9 +3190,15 @@
       <c r="P56" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>4600</t>
+      <c r="Q56" t="n">
+        <v>4600</v>
+      </c>
+      <c r="R56" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>4967</t>
         </is>
       </c>
     </row>
@@ -3023,9 +3257,15 @@
       <c r="P57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>4302</t>
+      <c r="Q57" t="n">
+        <v>4302</v>
+      </c>
+      <c r="R57" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4917</t>
         </is>
       </c>
     </row>
@@ -3084,9 +3324,15 @@
       <c r="P58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>4394</t>
+      <c r="Q58" t="n">
+        <v>4394</v>
+      </c>
+      <c r="R58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>4674</t>
         </is>
       </c>
     </row>
@@ -3145,9 +3391,15 @@
       <c r="P59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>4150</t>
+      <c r="Q59" t="n">
+        <v>4150</v>
+      </c>
+      <c r="R59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>4621</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3458,15 @@
       <c r="P60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>4324</t>
+      <c r="Q60" t="n">
+        <v>4324</v>
+      </c>
+      <c r="R60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>4617</t>
         </is>
       </c>
     </row>
@@ -3267,9 +3525,15 @@
       <c r="P61" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>3583</t>
+      <c r="Q61" t="n">
+        <v>3583</v>
+      </c>
+      <c r="R61" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>4129</t>
         </is>
       </c>
     </row>
@@ -3328,9 +3592,15 @@
       <c r="P62" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>4856</t>
+      <c r="Q62" t="n">
+        <v>4856</v>
+      </c>
+      <c r="R62" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>5357</t>
         </is>
       </c>
     </row>
@@ -3389,9 +3659,15 @@
       <c r="P63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>4593</t>
+      <c r="Q63" t="n">
+        <v>4593</v>
+      </c>
+      <c r="R63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>5127</t>
         </is>
       </c>
     </row>
@@ -3450,9 +3726,15 @@
       <c r="P64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>4728</t>
+      <c r="Q64" t="n">
+        <v>4728</v>
+      </c>
+      <c r="R64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>5196</t>
         </is>
       </c>
     </row>
@@ -3486,6 +3768,8 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" s="3" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
+      <c r="R65" s="3" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3542,9 +3826,15 @@
       <c r="P66" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>4429</t>
+      <c r="Q66" t="n">
+        <v>4429</v>
+      </c>
+      <c r="R66" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>4887</t>
         </is>
       </c>
     </row>
@@ -3603,9 +3893,15 @@
       <c r="P67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="Q67" t="n">
+        <v>4180</v>
+      </c>
+      <c r="R67" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>4553</t>
         </is>
       </c>
     </row>
@@ -3664,9 +3960,15 @@
       <c r="P68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>4286</t>
+      <c r="Q68" t="n">
+        <v>4286</v>
+      </c>
+      <c r="R68" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>4472</t>
         </is>
       </c>
     </row>
@@ -3725,9 +4027,15 @@
       <c r="P69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>4121</t>
+      <c r="Q69" t="n">
+        <v>4121</v>
+      </c>
+      <c r="R69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -3786,9 +4094,15 @@
       <c r="P70" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>4182</t>
+      <c r="Q70" t="n">
+        <v>4182</v>
+      </c>
+      <c r="R70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -3847,9 +4161,15 @@
       <c r="P71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="Q71" t="n">
+        <v>4548</v>
+      </c>
+      <c r="R71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>4877</t>
         </is>
       </c>
     </row>
@@ -3908,9 +4228,15 @@
       <c r="P72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>4224</t>
+      <c r="Q72" t="n">
+        <v>4224</v>
+      </c>
+      <c r="R72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>4479</t>
         </is>
       </c>
     </row>
@@ -3969,9 +4295,15 @@
       <c r="P73" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>3205</t>
+      <c r="Q73" t="n">
+        <v>3205</v>
+      </c>
+      <c r="R73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>3235</t>
         </is>
       </c>
     </row>
@@ -4030,9 +4362,15 @@
       <c r="P74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>3264</t>
+      <c r="Q74" t="n">
+        <v>3264</v>
+      </c>
+      <c r="R74" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>3870</t>
         </is>
       </c>
     </row>
@@ -4091,9 +4429,15 @@
       <c r="P75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>3089</t>
+      <c r="Q75" t="n">
+        <v>3089</v>
+      </c>
+      <c r="R75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>
@@ -4152,9 +4496,15 @@
       <c r="P76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>3399</t>
+      <c r="Q76" t="n">
+        <v>3399</v>
+      </c>
+      <c r="R76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>3444</t>
         </is>
       </c>
     </row>
@@ -4213,9 +4563,15 @@
       <c r="P77" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>4087</t>
+      <c r="Q77" t="n">
+        <v>4087</v>
+      </c>
+      <c r="R77" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>4195</t>
         </is>
       </c>
     </row>
@@ -4274,9 +4630,15 @@
       <c r="P78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>3692</t>
+      <c r="Q78" t="n">
+        <v>3692</v>
+      </c>
+      <c r="R78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>4033</t>
         </is>
       </c>
     </row>
@@ -4335,9 +4697,15 @@
       <c r="P79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>3571</t>
+      <c r="Q79" t="n">
+        <v>3571</v>
+      </c>
+      <c r="R79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -4396,9 +4764,15 @@
       <c r="P80" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>3710</t>
+      <c r="Q80" t="n">
+        <v>3710</v>
+      </c>
+      <c r="R80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>3979</t>
         </is>
       </c>
     </row>
@@ -4457,9 +4831,15 @@
       <c r="P81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>3482</t>
+      <c r="Q81" t="n">
+        <v>3482</v>
+      </c>
+      <c r="R81" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -4518,9 +4898,15 @@
       <c r="P82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>3566</t>
+      <c r="Q82" t="n">
+        <v>3566</v>
+      </c>
+      <c r="R82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>3972</t>
         </is>
       </c>
     </row>
@@ -4579,9 +4965,15 @@
       <c r="P83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="Q83" t="n">
+        <v>2529</v>
+      </c>
+      <c r="R83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -4631,6 +5023,8 @@
       <c r="O84" t="inlineStr"/>
       <c r="P84" s="3" t="inlineStr"/>
       <c r="Q84" t="inlineStr"/>
+      <c r="R84" s="3" t="inlineStr"/>
+      <c r="S84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -4670,6 +5064,8 @@
       <c r="O85" t="inlineStr"/>
       <c r="P85" s="3" t="inlineStr"/>
       <c r="Q85" t="inlineStr"/>
+      <c r="R85" s="3" t="inlineStr"/>
+      <c r="S85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -4717,6 +5113,8 @@
       <c r="O86" t="inlineStr"/>
       <c r="P86" s="3" t="inlineStr"/>
       <c r="Q86" t="inlineStr"/>
+      <c r="R86" s="3" t="inlineStr"/>
+      <c r="S86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -4773,9 +5171,15 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>4187</t>
+      <c r="Q87" t="n">
+        <v>4187</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>4189</t>
         </is>
       </c>
     </row>
@@ -4817,6 +5221,8 @@
       <c r="O88" t="inlineStr"/>
       <c r="P88" s="3" t="inlineStr"/>
       <c r="Q88" t="inlineStr"/>
+      <c r="R88" s="3" t="inlineStr"/>
+      <c r="S88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -4848,6 +5254,8 @@
       <c r="O89" t="inlineStr"/>
       <c r="P89" s="3" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
+      <c r="R89" s="3" t="inlineStr"/>
+      <c r="S89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -4904,9 +5312,15 @@
       <c r="P90" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>4491</t>
+      <c r="Q90" t="n">
+        <v>4491</v>
+      </c>
+      <c r="R90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>4793</t>
         </is>
       </c>
     </row>
@@ -4965,7 +5379,13 @@
       <c r="P91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q91" t="inlineStr">
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5026,9 +5446,15 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="Q92" t="n">
+        <v>2659</v>
+      </c>
+      <c r="R92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -5087,9 +5513,15 @@
       <c r="P93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="Q93" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -5148,9 +5580,15 @@
       <c r="P94" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>4079</t>
+      <c r="Q94" t="n">
+        <v>4079</v>
+      </c>
+      <c r="R94" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>4483</t>
         </is>
       </c>
     </row>
@@ -5209,9 +5647,15 @@
       <c r="P95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>4058</t>
+      <c r="Q95" t="n">
+        <v>4058</v>
+      </c>
+      <c r="R95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>4484</t>
         </is>
       </c>
     </row>
@@ -5270,9 +5714,15 @@
       <c r="P96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="Q96" t="n">
+        <v>2860</v>
+      </c>
+      <c r="R96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>2885</t>
         </is>
       </c>
     </row>
@@ -5331,9 +5781,15 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>3939</t>
+      <c r="Q97" t="n">
+        <v>3939</v>
+      </c>
+      <c r="R97" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>4226</t>
         </is>
       </c>
     </row>
@@ -5392,9 +5848,15 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
-        <is>
-          <t>2940</t>
+      <c r="Q98" t="n">
+        <v>2940</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>3111</t>
         </is>
       </c>
     </row>
@@ -5453,9 +5915,15 @@
       <c r="P99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>3207</t>
+      <c r="Q99" t="n">
+        <v>3207</v>
+      </c>
+      <c r="R99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -5514,9 +5982,15 @@
       <c r="P100" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q100" t="inlineStr">
-        <is>
-          <t>3655</t>
+      <c r="Q100" t="n">
+        <v>3655</v>
+      </c>
+      <c r="R100" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>4125</t>
         </is>
       </c>
     </row>
@@ -5575,9 +6049,15 @@
       <c r="P101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>4130</t>
+      <c r="Q101" t="n">
+        <v>4130</v>
+      </c>
+      <c r="R101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -5636,9 +6116,15 @@
       <c r="P102" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="Q102" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="Q102" t="n">
+        <v>3993</v>
+      </c>
+      <c r="R102" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -5697,9 +6183,15 @@
       <c r="P103" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>3980</t>
+      <c r="Q103" t="n">
+        <v>3980</v>
+      </c>
+      <c r="R103" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>4038</t>
         </is>
       </c>
     </row>
@@ -5758,9 +6250,15 @@
       <c r="P104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>3951</t>
+      <c r="Q104" t="n">
+        <v>3951</v>
+      </c>
+      <c r="R104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -5819,7 +6317,13 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
+      <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+      <c r="R105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5880,9 +6384,15 @@
       <c r="P106" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Q106" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="Q106" t="n">
+        <v>3989</v>
+      </c>
+      <c r="R106" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>4013</t>
         </is>
       </c>
     </row>
@@ -5941,9 +6451,15 @@
       <c r="P107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>3981</t>
+      <c r="Q107" t="n">
+        <v>3981</v>
+      </c>
+      <c r="R107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>4061</t>
         </is>
       </c>
     </row>
@@ -6002,9 +6518,15 @@
       <c r="P108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q108" t="inlineStr">
-        <is>
-          <t>3894</t>
+      <c r="Q108" t="n">
+        <v>3894</v>
+      </c>
+      <c r="R108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -6063,9 +6585,15 @@
       <c r="P109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>2540</t>
+      <c r="Q109" t="n">
+        <v>2540</v>
+      </c>
+      <c r="R109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>2972</t>
         </is>
       </c>
     </row>
@@ -6124,9 +6652,15 @@
       <c r="P110" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>3821</t>
+      <c r="Q110" t="n">
+        <v>3821</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -6160,6 +6694,8 @@
       <c r="O111" t="inlineStr"/>
       <c r="P111" s="3" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
+      <c r="R111" s="3" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6216,9 +6752,15 @@
       <c r="P112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q112" t="inlineStr">
-        <is>
-          <t>3696</t>
+      <c r="Q112" t="n">
+        <v>3696</v>
+      </c>
+      <c r="R112" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -6277,9 +6819,15 @@
       <c r="P113" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>3119</t>
+      <c r="Q113" t="n">
+        <v>3119</v>
+      </c>
+      <c r="R113" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>3327</t>
         </is>
       </c>
     </row>
@@ -6338,7 +6886,13 @@
       <c r="P114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr">
+      <c r="Q114" t="n">
+        <v>0</v>
+      </c>
+      <c r="R114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6399,9 +6953,15 @@
       <c r="P115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="Q115" t="n">
+        <v>3018</v>
+      </c>
+      <c r="R115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>3134</t>
         </is>
       </c>
     </row>
@@ -6460,9 +7020,15 @@
       <c r="P116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>2941</t>
+      <c r="Q116" t="n">
+        <v>2941</v>
+      </c>
+      <c r="R116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>3001</t>
         </is>
       </c>
     </row>
@@ -6504,6 +7070,8 @@
       <c r="O117" t="inlineStr"/>
       <c r="P117" s="3" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
+      <c r="R117" s="3" t="inlineStr"/>
+      <c r="S117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -6535,6 +7103,8 @@
       <c r="O118" t="inlineStr"/>
       <c r="P118" s="3" t="inlineStr"/>
       <c r="Q118" t="inlineStr"/>
+      <c r="R118" s="3" t="inlineStr"/>
+      <c r="S118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -6591,9 +7161,15 @@
       <c r="P119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q119" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="Q119" t="n">
+        <v>2773</v>
+      </c>
+      <c r="R119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>
@@ -6652,9 +7228,15 @@
       <c r="P120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>2824</t>
+      <c r="Q120" t="n">
+        <v>2824</v>
+      </c>
+      <c r="R120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -6713,9 +7295,15 @@
       <c r="P121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="Q121" t="n">
+        <v>2603</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>2697</t>
         </is>
       </c>
     </row>
@@ -6774,9 +7362,15 @@
       <c r="P122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>2617</t>
+      <c r="Q122" t="n">
+        <v>2617</v>
+      </c>
+      <c r="R122" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>2971</t>
         </is>
       </c>
     </row>
@@ -6830,6 +7424,8 @@
       <c r="O123" t="inlineStr"/>
       <c r="P123" s="3" t="inlineStr"/>
       <c r="Q123" t="inlineStr"/>
+      <c r="R123" s="3" t="inlineStr"/>
+      <c r="S123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -6886,9 +7482,15 @@
       <c r="P124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="Q124" t="n">
+        <v>2487</v>
+      </c>
+      <c r="R124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>2478</t>
         </is>
       </c>
     </row>
@@ -6947,7 +7549,13 @@
       <c r="P125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q125" t="inlineStr">
+      <c r="Q125" t="n">
+        <v>0</v>
+      </c>
+      <c r="R125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7008,9 +7616,15 @@
       <c r="P126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>1490</t>
+      <c r="Q126" t="n">
+        <v>1490</v>
+      </c>
+      <c r="R126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>1481</t>
         </is>
       </c>
     </row>
@@ -7069,9 +7683,15 @@
       <c r="P127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q127" t="inlineStr">
-        <is>
-          <t>1574</t>
+      <c r="Q127" t="n">
+        <v>1574</v>
+      </c>
+      <c r="R127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>1573</t>
         </is>
       </c>
     </row>
@@ -7130,9 +7750,15 @@
       <c r="P128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q128" t="inlineStr">
-        <is>
-          <t>1180</t>
+      <c r="Q128" t="n">
+        <v>1180</v>
+      </c>
+      <c r="R128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>1209</t>
         </is>
       </c>
     </row>
@@ -7191,7 +7817,13 @@
       <c r="P129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q129" t="inlineStr">
+      <c r="Q129" t="n">
+        <v>0</v>
+      </c>
+      <c r="R129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7252,7 +7884,13 @@
       <c r="P130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q130" t="inlineStr">
+      <c r="Q130" t="n">
+        <v>0</v>
+      </c>
+      <c r="R130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7313,7 +7951,13 @@
       <c r="P131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q131" t="inlineStr">
+      <c r="Q131" t="n">
+        <v>0</v>
+      </c>
+      <c r="R131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7374,7 +8018,13 @@
       <c r="P132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q132" t="inlineStr">
+      <c r="Q132" t="n">
+        <v>0</v>
+      </c>
+      <c r="R132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7435,7 +8085,13 @@
       <c r="P133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q133" t="inlineStr">
+      <c r="Q133" t="n">
+        <v>0</v>
+      </c>
+      <c r="R133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7496,7 +8152,13 @@
       <c r="P134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q134" t="inlineStr">
+      <c r="Q134" t="n">
+        <v>0</v>
+      </c>
+      <c r="R134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7557,9 +8219,15 @@
       <c r="P135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q135" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="Q135" t="n">
+        <v>2701</v>
+      </c>
+      <c r="R135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -7618,9 +8286,15 @@
       <c r="P136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="Q136" t="n">
+        <v>3236</v>
+      </c>
+      <c r="R136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>3209</t>
         </is>
       </c>
     </row>
@@ -7679,7 +8353,13 @@
       <c r="P137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q137" t="inlineStr">
+      <c r="Q137" t="n">
+        <v>0</v>
+      </c>
+      <c r="R137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7740,9 +8420,15 @@
       <c r="P138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q138" t="inlineStr">
-        <is>
-          <t>2706</t>
+      <c r="Q138" t="n">
+        <v>2706</v>
+      </c>
+      <c r="R138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>2742</t>
         </is>
       </c>
     </row>
@@ -7801,7 +8487,13 @@
       <c r="P139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q139" t="inlineStr">
+      <c r="Q139" t="n">
+        <v>0</v>
+      </c>
+      <c r="R139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7862,7 +8554,13 @@
       <c r="P140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" t="inlineStr">
+      <c r="Q140" t="n">
+        <v>0</v>
+      </c>
+      <c r="R140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7923,7 +8621,13 @@
       <c r="P141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q141" t="inlineStr">
+      <c r="Q141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="R141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S141" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -7984,9 +8688,15 @@
       <c r="P142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q142" t="inlineStr">
-        <is>
-          <t>1657</t>
+      <c r="Q142" t="n">
+        <v>1657</v>
+      </c>
+      <c r="R142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>1702</t>
         </is>
       </c>
     </row>
@@ -8045,7 +8755,13 @@
       <c r="P143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q143" t="inlineStr">
+      <c r="Q143" t="n">
+        <v>0</v>
+      </c>
+      <c r="R143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8106,7 +8822,13 @@
       <c r="P144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q144" t="inlineStr">
+      <c r="Q144" t="n">
+        <v>0</v>
+      </c>
+      <c r="R144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8167,7 +8889,13 @@
       <c r="P145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q145" t="inlineStr">
+      <c r="Q145" t="n">
+        <v>0</v>
+      </c>
+      <c r="R145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8228,7 +8956,13 @@
       <c r="P146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q146" t="inlineStr">
+      <c r="Q146" t="n">
+        <v>0</v>
+      </c>
+      <c r="R146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8289,7 +9023,13 @@
       <c r="P147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q147" t="inlineStr">
+      <c r="Q147" t="n">
+        <v>0</v>
+      </c>
+      <c r="R147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8350,7 +9090,13 @@
       <c r="P148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q148" t="inlineStr">
+      <c r="Q148" t="n">
+        <v>0</v>
+      </c>
+      <c r="R148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8411,7 +9157,13 @@
       <c r="P149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q149" t="inlineStr">
+      <c r="Q149" t="n">
+        <v>0</v>
+      </c>
+      <c r="R149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8472,7 +9224,13 @@
       <c r="P150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q150" t="inlineStr">
+      <c r="Q150" t="n">
+        <v>0</v>
+      </c>
+      <c r="R150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8533,9 +9291,15 @@
       <c r="P151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q151" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="Q151" t="n">
+        <v>2499</v>
+      </c>
+      <c r="R151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>2617</t>
         </is>
       </c>
     </row>
@@ -8594,7 +9358,13 @@
       <c r="P152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q152" t="inlineStr">
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8655,7 +9425,13 @@
       <c r="P153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q153" t="inlineStr">
+      <c r="Q153" t="n">
+        <v>0</v>
+      </c>
+      <c r="R153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8716,7 +9492,13 @@
       <c r="P154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q154" t="inlineStr">
+      <c r="Q154" t="n">
+        <v>0</v>
+      </c>
+      <c r="R154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8777,7 +9559,13 @@
       <c r="P155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q155" t="inlineStr">
+      <c r="Q155" t="n">
+        <v>0</v>
+      </c>
+      <c r="R155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8838,7 +9626,13 @@
       <c r="P156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q156" t="inlineStr">
+      <c r="Q156" t="n">
+        <v>0</v>
+      </c>
+      <c r="R156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8899,7 +9693,13 @@
       <c r="P157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q157" t="inlineStr">
+      <c r="Q157" t="n">
+        <v>0</v>
+      </c>
+      <c r="R157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8960,7 +9760,13 @@
       <c r="P158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q158" t="inlineStr">
+      <c r="Q158" t="n">
+        <v>0</v>
+      </c>
+      <c r="R158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9015,9 +9821,15 @@
       <c r="P159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q159" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="Q159" t="n">
+        <v>2587</v>
+      </c>
+      <c r="R159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -9070,9 +9882,15 @@
       <c r="P160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q160" t="inlineStr">
-        <is>
-          <t>1728</t>
+      <c r="Q160" t="n">
+        <v>1728</v>
+      </c>
+      <c r="R160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>1737</t>
         </is>
       </c>
     </row>
@@ -9125,9 +9943,15 @@
       <c r="P161" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Q161" t="inlineStr">
-        <is>
-          <t>1556</t>
+      <c r="Q161" t="n">
+        <v>1556</v>
+      </c>
+      <c r="R161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>1585</t>
         </is>
       </c>
     </row>
@@ -9176,9 +10000,15 @@
       <c r="P162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q162" t="inlineStr">
-        <is>
-          <t>2301</t>
+      <c r="Q162" t="n">
+        <v>2301</v>
+      </c>
+      <c r="R162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>2296</t>
         </is>
       </c>
     </row>
@@ -9223,9 +10053,15 @@
       <c r="P163" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="Q163" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="Q163" t="n">
+        <v>2875</v>
+      </c>
+      <c r="R163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -9262,11 +10098,11 @@
       <c r="P164" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="Q164" t="inlineStr">
-        <is>
-          <t>1737</t>
-        </is>
-      </c>
+      <c r="Q164" t="n">
+        <v>1737</v>
+      </c>
+      <c r="R164" s="3" t="inlineStr"/>
+      <c r="S164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -9281,7 +10117,7 @@
       <c r="D165" t="inlineStr"/>
       <c r="E165" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F165" s="3" t="inlineStr"/>
@@ -9301,9 +10137,15 @@
       <c r="P165" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="Q165" t="inlineStr">
-        <is>
-          <t>5173</t>
+      <c r="Q165" t="n">
+        <v>5173</v>
+      </c>
+      <c r="R165" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="S165" t="inlineStr">
+        <is>
+          <t>5777</t>
         </is>
       </c>
     </row>
@@ -9336,9 +10178,15 @@
       <c r="P166" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q166" t="inlineStr">
-        <is>
-          <t>2769</t>
+      <c r="Q166" t="n">
+        <v>2769</v>
+      </c>
+      <c r="R166" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>2999</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-04 06:33:08
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S166"/>
+  <dimension ref="A1:U166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>04-02_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>04-03_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>04-03_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,7 +558,13 @@
       <c r="R2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S2" t="n">
+        <v>2585</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="inlineStr">
         <is>
           <t>2585</t>
         </is>
@@ -586,6 +602,8 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" s="3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
+      <c r="T3" s="3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -619,6 +637,8 @@
       <c r="Q4" t="inlineStr"/>
       <c r="R4" s="3" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
+      <c r="T4" s="3" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -665,7 +685,13 @@
       <c r="R5" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S5" t="n">
+        <v>5464</v>
+      </c>
+      <c r="T5" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>5464</t>
         </is>
@@ -703,6 +729,8 @@
       <c r="Q6" t="inlineStr"/>
       <c r="R6" s="3" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
+      <c r="T6" s="3" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -736,6 +764,8 @@
       <c r="Q7" t="inlineStr"/>
       <c r="R7" s="3" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" s="3" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -786,7 +816,13 @@
       <c r="R8" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="S8" t="n">
+        <v>5923</v>
+      </c>
+      <c r="T8" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U8" t="inlineStr">
         <is>
           <t>5923</t>
         </is>
@@ -824,6 +860,8 @@
       <c r="Q9" t="inlineStr"/>
       <c r="R9" s="3" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" s="3" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -886,7 +924,13 @@
       <c r="R10" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="S10" t="n">
+        <v>5845</v>
+      </c>
+      <c r="T10" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U10" t="inlineStr">
         <is>
           <t>5845</t>
         </is>
@@ -929,7 +973,13 @@
       <c r="R11" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="S11" t="n">
+        <v>5381</v>
+      </c>
+      <c r="T11" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U11" t="inlineStr">
         <is>
           <t>5381</t>
         </is>
@@ -996,7 +1046,13 @@
       <c r="R12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="S12" t="n">
+        <v>4958</v>
+      </c>
+      <c r="T12" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>4958</t>
         </is>
@@ -1063,7 +1119,13 @@
       <c r="R13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="S13" t="n">
+        <v>5018</v>
+      </c>
+      <c r="T13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U13" t="inlineStr">
         <is>
           <t>5018</t>
         </is>
@@ -1130,7 +1192,13 @@
       <c r="R14" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="S14" t="n">
+        <v>5109</v>
+      </c>
+      <c r="T14" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="U14" t="inlineStr">
         <is>
           <t>5109</t>
         </is>
@@ -1197,7 +1265,13 @@
       <c r="R15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="S15" t="n">
+        <v>4429</v>
+      </c>
+      <c r="T15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>4429</t>
         </is>
@@ -1247,6 +1321,8 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" s="3" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
+      <c r="T16" s="3" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1297,7 +1373,13 @@
       <c r="R17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="S17" t="n">
+        <v>5854</v>
+      </c>
+      <c r="T17" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U17" t="inlineStr">
         <is>
           <t>5854</t>
         </is>
@@ -1348,7 +1430,13 @@
       <c r="R18" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="S18" t="n">
+        <v>6069</v>
+      </c>
+      <c r="T18" s="4" t="n">
+        <v>37</v>
+      </c>
+      <c r="U18" t="inlineStr">
         <is>
           <t>6069</t>
         </is>
@@ -1398,6 +1486,8 @@
       </c>
       <c r="R19" s="3" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
+      <c r="T19" s="3" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1431,6 +1521,8 @@
       <c r="Q20" t="inlineStr"/>
       <c r="R20" s="3" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
+      <c r="T20" s="3" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1485,7 +1577,13 @@
       <c r="R21" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S21" t="inlineStr">
+      <c r="S21" t="n">
+        <v>5681</v>
+      </c>
+      <c r="T21" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U21" t="inlineStr">
         <is>
           <t>5681</t>
         </is>
@@ -1523,6 +1621,8 @@
       <c r="Q22" t="inlineStr"/>
       <c r="R22" s="3" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
+      <c r="T22" s="3" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1569,7 +1669,13 @@
       <c r="R23" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="S23" t="n">
+        <v>5753</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U23" t="inlineStr">
         <is>
           <t>5753</t>
         </is>
@@ -1636,7 +1742,13 @@
       <c r="R24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="S24" t="n">
+        <v>5164</v>
+      </c>
+      <c r="T24" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="U24" t="inlineStr">
         <is>
           <t>5164</t>
         </is>
@@ -1674,6 +1786,8 @@
       <c r="Q25" t="inlineStr"/>
       <c r="R25" s="3" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
+      <c r="T25" s="3" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1707,6 +1821,8 @@
       <c r="Q26" t="inlineStr"/>
       <c r="R26" s="3" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
+      <c r="T26" s="3" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1740,6 +1856,8 @@
       <c r="Q27" t="inlineStr"/>
       <c r="R27" s="3" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
+      <c r="T27" s="3" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1773,6 +1891,8 @@
       <c r="Q28" t="inlineStr"/>
       <c r="R28" s="3" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
+      <c r="T28" s="3" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1806,6 +1926,8 @@
       <c r="Q29" t="inlineStr"/>
       <c r="R29" s="3" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
+      <c r="T29" s="3" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1839,6 +1961,8 @@
       <c r="Q30" t="inlineStr"/>
       <c r="R30" s="3" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
+      <c r="T30" s="3" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1872,6 +1996,8 @@
       <c r="Q31" t="inlineStr"/>
       <c r="R31" s="3" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
+      <c r="T31" s="3" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1905,6 +2031,8 @@
       <c r="Q32" t="inlineStr"/>
       <c r="R32" s="3" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
+      <c r="T32" s="3" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1938,6 +2066,8 @@
       <c r="Q33" t="inlineStr"/>
       <c r="R33" s="3" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
+      <c r="T33" s="3" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1971,6 +2101,8 @@
       <c r="Q34" t="inlineStr"/>
       <c r="R34" s="3" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
+      <c r="T34" s="3" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2033,7 +2165,13 @@
       <c r="R35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S35" t="inlineStr">
+      <c r="S35" t="n">
+        <v>2530</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="inlineStr">
         <is>
           <t>2530</t>
         </is>
@@ -2087,6 +2225,8 @@
       <c r="Q36" t="inlineStr"/>
       <c r="R36" s="3" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
+      <c r="T36" s="3" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2120,6 +2260,8 @@
       <c r="Q37" t="inlineStr"/>
       <c r="R37" s="3" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
+      <c r="T37" s="3" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2153,6 +2295,8 @@
       <c r="Q38" t="inlineStr"/>
       <c r="R38" s="3" t="inlineStr"/>
       <c r="S38" t="inlineStr"/>
+      <c r="T38" s="3" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2215,7 +2359,13 @@
       <c r="R39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S39" t="inlineStr">
+      <c r="S39" t="n">
+        <v>4236</v>
+      </c>
+      <c r="T39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U39" t="inlineStr">
         <is>
           <t>4236</t>
         </is>
@@ -2282,7 +2432,13 @@
       <c r="R40" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="S40" t="inlineStr">
+      <c r="S40" t="n">
+        <v>4301</v>
+      </c>
+      <c r="T40" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="U40" t="inlineStr">
         <is>
           <t>4301</t>
         </is>
@@ -2320,6 +2476,8 @@
       <c r="Q41" t="inlineStr"/>
       <c r="R41" s="3" t="inlineStr"/>
       <c r="S41" t="inlineStr"/>
+      <c r="T41" s="3" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2382,7 +2540,13 @@
       <c r="R42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S42" t="inlineStr">
+      <c r="S42" t="n">
+        <v>4616</v>
+      </c>
+      <c r="T42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U42" t="inlineStr">
         <is>
           <t>4616</t>
         </is>
@@ -2420,6 +2584,8 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" s="3" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
+      <c r="T43" s="3" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2482,7 +2648,13 @@
       <c r="R44" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S44" t="inlineStr">
+      <c r="S44" t="n">
+        <v>4372</v>
+      </c>
+      <c r="T44" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U44" t="inlineStr">
         <is>
           <t>4372</t>
         </is>
@@ -2549,7 +2721,13 @@
       <c r="R45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S45" t="inlineStr">
+      <c r="S45" t="n">
+        <v>4396</v>
+      </c>
+      <c r="T45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U45" t="inlineStr">
         <is>
           <t>4396</t>
         </is>
@@ -2616,7 +2794,13 @@
       <c r="R46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S46" t="inlineStr">
+      <c r="S46" t="n">
+        <v>3066</v>
+      </c>
+      <c r="T46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U46" t="inlineStr">
         <is>
           <t>3066</t>
         </is>
@@ -2683,7 +2867,13 @@
       <c r="R47" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S47" t="inlineStr">
+      <c r="S47" t="n">
+        <v>3349</v>
+      </c>
+      <c r="T47" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U47" t="inlineStr">
         <is>
           <t>3349</t>
         </is>
@@ -2750,7 +2940,13 @@
       <c r="R48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S48" t="inlineStr">
+      <c r="S48" t="n">
+        <v>0</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2817,7 +3013,13 @@
       <c r="R49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S49" t="inlineStr">
+      <c r="S49" t="n">
+        <v>0</v>
+      </c>
+      <c r="T49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2867,6 +3069,8 @@
       </c>
       <c r="R50" s="3" t="inlineStr"/>
       <c r="S50" t="inlineStr"/>
+      <c r="T50" s="3" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2900,6 +3104,8 @@
       <c r="Q51" t="inlineStr"/>
       <c r="R51" s="3" t="inlineStr"/>
       <c r="S51" t="inlineStr"/>
+      <c r="T51" s="3" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -2962,7 +3168,13 @@
       <c r="R52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S52" t="inlineStr">
+      <c r="S52" t="n">
+        <v>4796</v>
+      </c>
+      <c r="T52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U52" t="inlineStr">
         <is>
           <t>4796</t>
         </is>
@@ -3029,7 +3241,13 @@
       <c r="R53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S53" t="inlineStr">
+      <c r="S53" t="n">
+        <v>4615</v>
+      </c>
+      <c r="T53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U53" t="inlineStr">
         <is>
           <t>4615</t>
         </is>
@@ -3067,6 +3285,8 @@
       <c r="Q54" t="inlineStr"/>
       <c r="R54" s="3" t="inlineStr"/>
       <c r="S54" t="inlineStr"/>
+      <c r="T54" s="3" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3129,7 +3349,13 @@
       <c r="R55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="S55" t="inlineStr">
+      <c r="S55" t="n">
+        <v>4907</v>
+      </c>
+      <c r="T55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="U55" t="inlineStr">
         <is>
           <t>4907</t>
         </is>
@@ -3196,7 +3422,13 @@
       <c r="R56" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S56" t="inlineStr">
+      <c r="S56" t="n">
+        <v>4967</v>
+      </c>
+      <c r="T56" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U56" t="inlineStr">
         <is>
           <t>4967</t>
         </is>
@@ -3263,7 +3495,13 @@
       <c r="R57" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="S57" t="inlineStr">
+      <c r="S57" t="n">
+        <v>4917</v>
+      </c>
+      <c r="T57" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="U57" t="inlineStr">
         <is>
           <t>4917</t>
         </is>
@@ -3330,7 +3568,13 @@
       <c r="R58" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="S58" t="inlineStr">
+      <c r="S58" t="n">
+        <v>4674</v>
+      </c>
+      <c r="T58" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="U58" t="inlineStr">
         <is>
           <t>4674</t>
         </is>
@@ -3397,7 +3641,13 @@
       <c r="R59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S59" t="inlineStr">
+      <c r="S59" t="n">
+        <v>4621</v>
+      </c>
+      <c r="T59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U59" t="inlineStr">
         <is>
           <t>4621</t>
         </is>
@@ -3464,7 +3714,13 @@
       <c r="R60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S60" t="inlineStr">
+      <c r="S60" t="n">
+        <v>4617</v>
+      </c>
+      <c r="T60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U60" t="inlineStr">
         <is>
           <t>4617</t>
         </is>
@@ -3531,7 +3787,13 @@
       <c r="R61" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S61" t="inlineStr">
+      <c r="S61" t="n">
+        <v>4129</v>
+      </c>
+      <c r="T61" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U61" t="inlineStr">
         <is>
           <t>4129</t>
         </is>
@@ -3598,7 +3860,13 @@
       <c r="R62" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S62" t="inlineStr">
+      <c r="S62" t="n">
+        <v>5357</v>
+      </c>
+      <c r="T62" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U62" t="inlineStr">
         <is>
           <t>5357</t>
         </is>
@@ -3665,7 +3933,13 @@
       <c r="R63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S63" t="inlineStr">
+      <c r="S63" t="n">
+        <v>5127</v>
+      </c>
+      <c r="T63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U63" t="inlineStr">
         <is>
           <t>5127</t>
         </is>
@@ -3732,7 +4006,13 @@
       <c r="R64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S64" t="inlineStr">
+      <c r="S64" t="n">
+        <v>5196</v>
+      </c>
+      <c r="T64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U64" t="inlineStr">
         <is>
           <t>5196</t>
         </is>
@@ -3770,6 +4050,8 @@
       <c r="Q65" t="inlineStr"/>
       <c r="R65" s="3" t="inlineStr"/>
       <c r="S65" t="inlineStr"/>
+      <c r="T65" s="3" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3832,7 +4114,13 @@
       <c r="R66" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S66" t="inlineStr">
+      <c r="S66" t="n">
+        <v>4887</v>
+      </c>
+      <c r="T66" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U66" t="inlineStr">
         <is>
           <t>4887</t>
         </is>
@@ -3899,7 +4187,13 @@
       <c r="R67" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S67" t="inlineStr">
+      <c r="S67" t="n">
+        <v>4553</v>
+      </c>
+      <c r="T67" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U67" t="inlineStr">
         <is>
           <t>4553</t>
         </is>
@@ -3966,7 +4260,13 @@
       <c r="R68" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="S68" t="inlineStr">
+      <c r="S68" t="n">
+        <v>4472</v>
+      </c>
+      <c r="T68" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="U68" t="inlineStr">
         <is>
           <t>4472</t>
         </is>
@@ -4033,7 +4333,13 @@
       <c r="R69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S69" t="inlineStr">
+      <c r="S69" t="n">
+        <v>4397</v>
+      </c>
+      <c r="T69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U69" t="inlineStr">
         <is>
           <t>4397</t>
         </is>
@@ -4100,7 +4406,13 @@
       <c r="R70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S70" t="inlineStr">
+      <c r="S70" t="n">
+        <v>4506</v>
+      </c>
+      <c r="T70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U70" t="inlineStr">
         <is>
           <t>4506</t>
         </is>
@@ -4167,7 +4479,13 @@
       <c r="R71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S71" t="inlineStr">
+      <c r="S71" t="n">
+        <v>4877</v>
+      </c>
+      <c r="T71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U71" t="inlineStr">
         <is>
           <t>4877</t>
         </is>
@@ -4234,7 +4552,13 @@
       <c r="R72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S72" t="inlineStr">
+      <c r="S72" t="n">
+        <v>4479</v>
+      </c>
+      <c r="T72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U72" t="inlineStr">
         <is>
           <t>4479</t>
         </is>
@@ -4301,7 +4625,13 @@
       <c r="R73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S73" t="inlineStr">
+      <c r="S73" t="n">
+        <v>3235</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U73" t="inlineStr">
         <is>
           <t>3235</t>
         </is>
@@ -4368,7 +4698,13 @@
       <c r="R74" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="S74" t="inlineStr">
+      <c r="S74" t="n">
+        <v>3870</v>
+      </c>
+      <c r="T74" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="U74" t="inlineStr">
         <is>
           <t>3870</t>
         </is>
@@ -4435,7 +4771,13 @@
       <c r="R75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S75" t="inlineStr">
+      <c r="S75" t="n">
+        <v>3085</v>
+      </c>
+      <c r="T75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U75" t="inlineStr">
         <is>
           <t>3085</t>
         </is>
@@ -4502,7 +4844,13 @@
       <c r="R76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S76" t="inlineStr">
+      <c r="S76" t="n">
+        <v>3444</v>
+      </c>
+      <c r="T76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U76" t="inlineStr">
         <is>
           <t>3444</t>
         </is>
@@ -4569,7 +4917,13 @@
       <c r="R77" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="S77" t="inlineStr">
+      <c r="S77" t="n">
+        <v>4195</v>
+      </c>
+      <c r="T77" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="U77" t="inlineStr">
         <is>
           <t>4195</t>
         </is>
@@ -4636,7 +4990,13 @@
       <c r="R78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S78" t="inlineStr">
+      <c r="S78" t="n">
+        <v>4033</v>
+      </c>
+      <c r="T78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U78" t="inlineStr">
         <is>
           <t>4033</t>
         </is>
@@ -4703,7 +5063,13 @@
       <c r="R79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S79" t="inlineStr">
+      <c r="S79" t="n">
+        <v>3875</v>
+      </c>
+      <c r="T79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U79" t="inlineStr">
         <is>
           <t>3875</t>
         </is>
@@ -4770,7 +5136,13 @@
       <c r="R80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S80" t="inlineStr">
+      <c r="S80" t="n">
+        <v>3979</v>
+      </c>
+      <c r="T80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U80" t="inlineStr">
         <is>
           <t>3979</t>
         </is>
@@ -4837,7 +5209,13 @@
       <c r="R81" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S81" t="inlineStr">
+      <c r="S81" t="n">
+        <v>3771</v>
+      </c>
+      <c r="T81" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U81" t="inlineStr">
         <is>
           <t>3771</t>
         </is>
@@ -4904,7 +5282,13 @@
       <c r="R82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S82" t="inlineStr">
+      <c r="S82" t="n">
+        <v>3972</v>
+      </c>
+      <c r="T82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U82" t="inlineStr">
         <is>
           <t>3972</t>
         </is>
@@ -4971,7 +5355,13 @@
       <c r="R83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S83" t="inlineStr">
+      <c r="S83" t="n">
+        <v>2592</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U83" t="inlineStr">
         <is>
           <t>2592</t>
         </is>
@@ -5025,6 +5415,8 @@
       <c r="Q84" t="inlineStr"/>
       <c r="R84" s="3" t="inlineStr"/>
       <c r="S84" t="inlineStr"/>
+      <c r="T84" s="3" t="inlineStr"/>
+      <c r="U84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5066,6 +5458,8 @@
       <c r="Q85" t="inlineStr"/>
       <c r="R85" s="3" t="inlineStr"/>
       <c r="S85" t="inlineStr"/>
+      <c r="T85" s="3" t="inlineStr"/>
+      <c r="U85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5115,6 +5509,8 @@
       <c r="Q86" t="inlineStr"/>
       <c r="R86" s="3" t="inlineStr"/>
       <c r="S86" t="inlineStr"/>
+      <c r="T86" s="3" t="inlineStr"/>
+      <c r="U86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5177,7 +5573,13 @@
       <c r="R87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S87" t="inlineStr">
+      <c r="S87" t="n">
+        <v>4189</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="inlineStr">
         <is>
           <t>4189</t>
         </is>
@@ -5223,6 +5625,8 @@
       <c r="Q88" t="inlineStr"/>
       <c r="R88" s="3" t="inlineStr"/>
       <c r="S88" t="inlineStr"/>
+      <c r="T88" s="3" t="inlineStr"/>
+      <c r="U88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5256,6 +5660,8 @@
       <c r="Q89" t="inlineStr"/>
       <c r="R89" s="3" t="inlineStr"/>
       <c r="S89" t="inlineStr"/>
+      <c r="T89" s="3" t="inlineStr"/>
+      <c r="U89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5318,7 +5724,13 @@
       <c r="R90" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="S90" t="inlineStr">
+      <c r="S90" t="n">
+        <v>4793</v>
+      </c>
+      <c r="T90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="U90" t="inlineStr">
         <is>
           <t>4793</t>
         </is>
@@ -5385,7 +5797,13 @@
       <c r="R91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S91" t="inlineStr">
+      <c r="S91" t="n">
+        <v>0</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5452,7 +5870,13 @@
       <c r="R92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>2713</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>2713</t>
         </is>
@@ -5519,7 +5943,13 @@
       <c r="R93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="inlineStr">
+      <c r="S93" t="n">
+        <v>2516</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -5586,7 +6016,13 @@
       <c r="R94" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="S94" t="inlineStr">
+      <c r="S94" t="n">
+        <v>4483</v>
+      </c>
+      <c r="T94" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="U94" t="inlineStr">
         <is>
           <t>4483</t>
         </is>
@@ -5653,7 +6089,13 @@
       <c r="R95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S95" t="inlineStr">
+      <c r="S95" t="n">
+        <v>4484</v>
+      </c>
+      <c r="T95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U95" t="inlineStr">
         <is>
           <t>4484</t>
         </is>
@@ -5720,7 +6162,13 @@
       <c r="R96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="inlineStr">
+      <c r="S96" t="n">
+        <v>2885</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
         <is>
           <t>2885</t>
         </is>
@@ -5787,7 +6235,13 @@
       <c r="R97" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="S97" t="inlineStr">
+      <c r="S97" t="n">
+        <v>4226</v>
+      </c>
+      <c r="T97" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U97" t="inlineStr">
         <is>
           <t>4226</t>
         </is>
@@ -5854,7 +6308,13 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>3111</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>3111</t>
         </is>
@@ -5921,7 +6381,13 @@
       <c r="R99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S99" t="inlineStr">
+      <c r="S99" t="n">
+        <v>3693</v>
+      </c>
+      <c r="T99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U99" t="inlineStr">
         <is>
           <t>3693</t>
         </is>
@@ -5988,7 +6454,13 @@
       <c r="R100" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S100" t="inlineStr">
+      <c r="S100" t="n">
+        <v>4125</v>
+      </c>
+      <c r="T100" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U100" t="inlineStr">
         <is>
           <t>4125</t>
         </is>
@@ -6055,7 +6527,13 @@
       <c r="R101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S101" t="inlineStr">
+      <c r="S101" t="n">
+        <v>4465</v>
+      </c>
+      <c r="T101" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U101" t="inlineStr">
         <is>
           <t>4465</t>
         </is>
@@ -6122,7 +6600,13 @@
       <c r="R102" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="S102" t="inlineStr">
+      <c r="S102" t="n">
+        <v>4186</v>
+      </c>
+      <c r="T102" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="U102" t="inlineStr">
         <is>
           <t>4186</t>
         </is>
@@ -6189,7 +6673,13 @@
       <c r="R103" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="S103" t="inlineStr">
+      <c r="S103" t="n">
+        <v>4038</v>
+      </c>
+      <c r="T103" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="U103" t="inlineStr">
         <is>
           <t>4038</t>
         </is>
@@ -6256,7 +6746,13 @@
       <c r="R104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S104" t="inlineStr">
+      <c r="S104" t="n">
+        <v>3993</v>
+      </c>
+      <c r="T104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U104" t="inlineStr">
         <is>
           <t>3993</t>
         </is>
@@ -6323,7 +6819,13 @@
       <c r="R105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S105" t="inlineStr">
+      <c r="S105" t="n">
+        <v>0</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6390,7 +6892,13 @@
       <c r="R106" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S106" t="inlineStr">
+      <c r="S106" t="n">
+        <v>4013</v>
+      </c>
+      <c r="T106" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U106" t="inlineStr">
         <is>
           <t>4013</t>
         </is>
@@ -6457,7 +6965,13 @@
       <c r="R107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S107" t="inlineStr">
+      <c r="S107" t="n">
+        <v>4061</v>
+      </c>
+      <c r="T107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U107" t="inlineStr">
         <is>
           <t>4061</t>
         </is>
@@ -6524,7 +7038,13 @@
       <c r="R108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S108" t="inlineStr">
+      <c r="S108" t="n">
+        <v>4114</v>
+      </c>
+      <c r="T108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U108" t="inlineStr">
         <is>
           <t>4114</t>
         </is>
@@ -6591,7 +7111,13 @@
       <c r="R109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S109" t="inlineStr">
+      <c r="S109" t="n">
+        <v>2972</v>
+      </c>
+      <c r="T109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U109" t="inlineStr">
         <is>
           <t>2972</t>
         </is>
@@ -6658,7 +7184,13 @@
       <c r="R110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S110" t="inlineStr">
+      <c r="S110" t="n">
+        <v>3992</v>
+      </c>
+      <c r="T110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U110" t="inlineStr">
         <is>
           <t>3992</t>
         </is>
@@ -6696,6 +7228,8 @@
       <c r="Q111" t="inlineStr"/>
       <c r="R111" s="3" t="inlineStr"/>
       <c r="S111" t="inlineStr"/>
+      <c r="T111" s="3" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6758,7 +7292,13 @@
       <c r="R112" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="S112" t="inlineStr">
+      <c r="S112" t="n">
+        <v>3995</v>
+      </c>
+      <c r="T112" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="U112" t="inlineStr">
         <is>
           <t>3995</t>
         </is>
@@ -6825,7 +7365,13 @@
       <c r="R113" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="S113" t="inlineStr">
+      <c r="S113" t="n">
+        <v>3327</v>
+      </c>
+      <c r="T113" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="U113" t="inlineStr">
         <is>
           <t>3327</t>
         </is>
@@ -6892,7 +7438,13 @@
       <c r="R114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S114" t="inlineStr">
+      <c r="S114" t="n">
+        <v>0</v>
+      </c>
+      <c r="T114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6959,7 +7511,13 @@
       <c r="R115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S115" t="inlineStr">
+      <c r="S115" t="n">
+        <v>3134</v>
+      </c>
+      <c r="T115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U115" t="inlineStr">
         <is>
           <t>3134</t>
         </is>
@@ -7026,7 +7584,13 @@
       <c r="R116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S116" t="inlineStr">
+      <c r="S116" t="n">
+        <v>3001</v>
+      </c>
+      <c r="T116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U116" t="inlineStr">
         <is>
           <t>3001</t>
         </is>
@@ -7072,6 +7636,8 @@
       <c r="Q117" t="inlineStr"/>
       <c r="R117" s="3" t="inlineStr"/>
       <c r="S117" t="inlineStr"/>
+      <c r="T117" s="3" t="inlineStr"/>
+      <c r="U117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7105,6 +7671,8 @@
       <c r="Q118" t="inlineStr"/>
       <c r="R118" s="3" t="inlineStr"/>
       <c r="S118" t="inlineStr"/>
+      <c r="T118" s="3" t="inlineStr"/>
+      <c r="U118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -7167,7 +7735,13 @@
       <c r="R119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S119" t="inlineStr">
+      <c r="S119" t="n">
+        <v>2769</v>
+      </c>
+      <c r="T119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U119" t="inlineStr">
         <is>
           <t>2769</t>
         </is>
@@ -7234,7 +7808,13 @@
       <c r="R120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S120" t="inlineStr">
+      <c r="S120" t="n">
+        <v>2807</v>
+      </c>
+      <c r="T120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U120" t="inlineStr">
         <is>
           <t>2807</t>
         </is>
@@ -7301,7 +7881,13 @@
       <c r="R121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S121" t="inlineStr">
+      <c r="S121" t="n">
+        <v>2697</v>
+      </c>
+      <c r="T121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U121" t="inlineStr">
         <is>
           <t>2697</t>
         </is>
@@ -7368,7 +7954,13 @@
       <c r="R122" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S122" t="inlineStr">
+      <c r="S122" t="n">
+        <v>2971</v>
+      </c>
+      <c r="T122" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U122" t="inlineStr">
         <is>
           <t>2971</t>
         </is>
@@ -7426,6 +8018,8 @@
       <c r="Q123" t="inlineStr"/>
       <c r="R123" s="3" t="inlineStr"/>
       <c r="S123" t="inlineStr"/>
+      <c r="T123" s="3" t="inlineStr"/>
+      <c r="U123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -7488,7 +8082,13 @@
       <c r="R124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S124" t="inlineStr">
+      <c r="S124" t="n">
+        <v>2478</v>
+      </c>
+      <c r="T124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U124" t="inlineStr">
         <is>
           <t>2478</t>
         </is>
@@ -7555,7 +8155,13 @@
       <c r="R125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S125" t="inlineStr">
+      <c r="S125" t="n">
+        <v>0</v>
+      </c>
+      <c r="T125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7622,7 +8228,13 @@
       <c r="R126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S126" t="inlineStr">
+      <c r="S126" t="n">
+        <v>1481</v>
+      </c>
+      <c r="T126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U126" t="inlineStr">
         <is>
           <t>1481</t>
         </is>
@@ -7689,7 +8301,13 @@
       <c r="R127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S127" t="inlineStr">
+      <c r="S127" t="n">
+        <v>1573</v>
+      </c>
+      <c r="T127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U127" t="inlineStr">
         <is>
           <t>1573</t>
         </is>
@@ -7756,7 +8374,13 @@
       <c r="R128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S128" t="inlineStr">
+      <c r="S128" t="n">
+        <v>1209</v>
+      </c>
+      <c r="T128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U128" t="inlineStr">
         <is>
           <t>1209</t>
         </is>
@@ -7823,7 +8447,13 @@
       <c r="R129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S129" t="inlineStr">
+      <c r="S129" t="n">
+        <v>0</v>
+      </c>
+      <c r="T129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7890,7 +8520,13 @@
       <c r="R130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S130" t="inlineStr">
+      <c r="S130" t="n">
+        <v>0</v>
+      </c>
+      <c r="T130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7957,7 +8593,13 @@
       <c r="R131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S131" t="inlineStr">
+      <c r="S131" t="n">
+        <v>0</v>
+      </c>
+      <c r="T131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8024,7 +8666,13 @@
       <c r="R132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S132" t="inlineStr">
+      <c r="S132" t="n">
+        <v>0</v>
+      </c>
+      <c r="T132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8091,7 +8739,13 @@
       <c r="R133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S133" t="inlineStr">
+      <c r="S133" t="n">
+        <v>0</v>
+      </c>
+      <c r="T133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8158,7 +8812,13 @@
       <c r="R134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S134" t="inlineStr">
+      <c r="S134" t="n">
+        <v>0</v>
+      </c>
+      <c r="T134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8225,7 +8885,13 @@
       <c r="R135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S135" t="inlineStr">
+      <c r="S135" t="n">
+        <v>2808</v>
+      </c>
+      <c r="T135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U135" t="inlineStr">
         <is>
           <t>2808</t>
         </is>
@@ -8292,7 +8958,13 @@
       <c r="R136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S136" t="inlineStr">
+      <c r="S136" t="n">
+        <v>3209</v>
+      </c>
+      <c r="T136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U136" t="inlineStr">
         <is>
           <t>3209</t>
         </is>
@@ -8359,7 +9031,13 @@
       <c r="R137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S137" t="inlineStr">
+      <c r="S137" t="n">
+        <v>0</v>
+      </c>
+      <c r="T137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8426,7 +9104,13 @@
       <c r="R138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S138" t="inlineStr">
+      <c r="S138" t="n">
+        <v>2742</v>
+      </c>
+      <c r="T138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U138" t="inlineStr">
         <is>
           <t>2742</t>
         </is>
@@ -8493,7 +9177,13 @@
       <c r="R139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S139" t="inlineStr">
+      <c r="S139" t="n">
+        <v>0</v>
+      </c>
+      <c r="T139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8560,7 +9250,13 @@
       <c r="R140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S140" t="inlineStr">
+      <c r="S140" t="n">
+        <v>0</v>
+      </c>
+      <c r="T140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8627,7 +9323,13 @@
       <c r="R141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S141" t="inlineStr">
+      <c r="S141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="T141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U141" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -8694,7 +9396,13 @@
       <c r="R142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S142" t="inlineStr">
+      <c r="S142" t="n">
+        <v>1702</v>
+      </c>
+      <c r="T142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U142" t="inlineStr">
         <is>
           <t>1702</t>
         </is>
@@ -8761,7 +9469,13 @@
       <c r="R143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S143" t="inlineStr">
+      <c r="S143" t="n">
+        <v>0</v>
+      </c>
+      <c r="T143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8828,7 +9542,13 @@
       <c r="R144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S144" t="inlineStr">
+      <c r="S144" t="n">
+        <v>0</v>
+      </c>
+      <c r="T144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8895,7 +9615,13 @@
       <c r="R145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S145" t="inlineStr">
+      <c r="S145" t="n">
+        <v>0</v>
+      </c>
+      <c r="T145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8962,7 +9688,13 @@
       <c r="R146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S146" t="inlineStr">
+      <c r="S146" t="n">
+        <v>0</v>
+      </c>
+      <c r="T146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9029,7 +9761,13 @@
       <c r="R147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S147" t="inlineStr">
+      <c r="S147" t="n">
+        <v>0</v>
+      </c>
+      <c r="T147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9096,7 +9834,13 @@
       <c r="R148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S148" t="inlineStr">
+      <c r="S148" t="n">
+        <v>0</v>
+      </c>
+      <c r="T148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9163,7 +9907,13 @@
       <c r="R149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S149" t="inlineStr">
+      <c r="S149" t="n">
+        <v>0</v>
+      </c>
+      <c r="T149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9230,7 +9980,13 @@
       <c r="R150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S150" t="inlineStr">
+      <c r="S150" t="n">
+        <v>0</v>
+      </c>
+      <c r="T150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9297,7 +10053,13 @@
       <c r="R151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S151" t="inlineStr">
+      <c r="S151" t="n">
+        <v>2617</v>
+      </c>
+      <c r="T151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U151" t="inlineStr">
         <is>
           <t>2617</t>
         </is>
@@ -9364,7 +10126,13 @@
       <c r="R152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S152" t="inlineStr">
+      <c r="S152" t="n">
+        <v>0</v>
+      </c>
+      <c r="T152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9431,7 +10199,13 @@
       <c r="R153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S153" t="inlineStr">
+      <c r="S153" t="n">
+        <v>0</v>
+      </c>
+      <c r="T153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9498,7 +10272,13 @@
       <c r="R154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S154" t="inlineStr">
+      <c r="S154" t="n">
+        <v>0</v>
+      </c>
+      <c r="T154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9565,7 +10345,13 @@
       <c r="R155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S155" t="inlineStr">
+      <c r="S155" t="n">
+        <v>0</v>
+      </c>
+      <c r="T155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9632,7 +10418,13 @@
       <c r="R156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S156" t="inlineStr">
+      <c r="S156" t="n">
+        <v>0</v>
+      </c>
+      <c r="T156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9699,7 +10491,13 @@
       <c r="R157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S157" t="inlineStr">
+      <c r="S157" t="n">
+        <v>0</v>
+      </c>
+      <c r="T157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9766,7 +10564,13 @@
       <c r="R158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S158" t="inlineStr">
+      <c r="S158" t="n">
+        <v>0</v>
+      </c>
+      <c r="T158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9827,7 +10631,13 @@
       <c r="R159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S159" t="inlineStr">
+      <c r="S159" t="n">
+        <v>2664</v>
+      </c>
+      <c r="T159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U159" t="inlineStr">
         <is>
           <t>2664</t>
         </is>
@@ -9888,7 +10698,13 @@
       <c r="R160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S160" t="inlineStr">
+      <c r="S160" t="n">
+        <v>1737</v>
+      </c>
+      <c r="T160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U160" t="inlineStr">
         <is>
           <t>1737</t>
         </is>
@@ -9949,7 +10765,13 @@
       <c r="R161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S161" t="inlineStr">
+      <c r="S161" t="n">
+        <v>1585</v>
+      </c>
+      <c r="T161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U161" t="inlineStr">
         <is>
           <t>1585</t>
         </is>
@@ -10006,7 +10828,13 @@
       <c r="R162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S162" t="inlineStr">
+      <c r="S162" t="n">
+        <v>2296</v>
+      </c>
+      <c r="T162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U162" t="inlineStr">
         <is>
           <t>2296</t>
         </is>
@@ -10059,7 +10887,13 @@
       <c r="R163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S163" t="inlineStr">
+      <c r="S163" t="n">
+        <v>2830</v>
+      </c>
+      <c r="T163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U163" t="inlineStr">
         <is>
           <t>2830</t>
         </is>
@@ -10103,6 +10937,8 @@
       </c>
       <c r="R164" s="3" t="inlineStr"/>
       <c r="S164" t="inlineStr"/>
+      <c r="T164" s="3" t="inlineStr"/>
+      <c r="U164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -10143,7 +10979,13 @@
       <c r="R165" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="S165" t="inlineStr">
+      <c r="S165" t="n">
+        <v>5777</v>
+      </c>
+      <c r="T165" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="U165" t="inlineStr">
         <is>
           <t>5777</t>
         </is>
@@ -10184,7 +11026,13 @@
       <c r="R166" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S166" t="inlineStr">
+      <c r="S166" t="n">
+        <v>2999</v>
+      </c>
+      <c r="T166" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U166" t="inlineStr">
         <is>
           <t>2999</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-04 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U166"/>
+  <dimension ref="A1:U167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,10 +564,8 @@
       <c r="T2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>2585</t>
-        </is>
+      <c r="U2" t="n">
+        <v>2585</v>
       </c>
     </row>
     <row r="3">
@@ -691,10 +689,8 @@
       <c r="T5" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>5464</t>
-        </is>
+      <c r="U5" t="n">
+        <v>5464</v>
       </c>
     </row>
     <row r="6">
@@ -822,10 +818,8 @@
       <c r="T8" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>5923</t>
-        </is>
+      <c r="U8" t="n">
+        <v>5923</v>
       </c>
     </row>
     <row r="9">
@@ -930,10 +924,8 @@
       <c r="T10" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>5845</t>
-        </is>
+      <c r="U10" t="n">
+        <v>5845</v>
       </c>
     </row>
     <row r="11">
@@ -981,7 +973,7 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>5381</t>
+          <t>5695</t>
         </is>
       </c>
     </row>
@@ -1052,10 +1044,8 @@
       <c r="T12" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>4958</t>
-        </is>
+      <c r="U12" t="n">
+        <v>4958</v>
       </c>
     </row>
     <row r="13">
@@ -1127,7 +1117,7 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>5018</t>
+          <t>5317</t>
         </is>
       </c>
     </row>
@@ -1198,10 +1188,8 @@
       <c r="T14" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>5109</t>
-        </is>
+      <c r="U14" t="n">
+        <v>5109</v>
       </c>
     </row>
     <row r="15">
@@ -1271,10 +1259,8 @@
       <c r="T15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>4429</t>
-        </is>
+      <c r="U15" t="n">
+        <v>4429</v>
       </c>
     </row>
     <row r="16">
@@ -1379,10 +1365,8 @@
       <c r="T17" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>5854</t>
-        </is>
+      <c r="U17" t="n">
+        <v>5854</v>
       </c>
     </row>
     <row r="18">
@@ -1436,10 +1420,8 @@
       <c r="T18" s="4" t="n">
         <v>37</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>6069</t>
-        </is>
+      <c r="U18" t="n">
+        <v>6069</v>
       </c>
     </row>
     <row r="19">
@@ -1583,10 +1565,8 @@
       <c r="T21" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>5681</t>
-        </is>
+      <c r="U21" t="n">
+        <v>5681</v>
       </c>
     </row>
     <row r="22">
@@ -1675,10 +1655,8 @@
       <c r="T23" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>5753</t>
-        </is>
+      <c r="U23" t="n">
+        <v>5753</v>
       </c>
     </row>
     <row r="24">
@@ -1748,10 +1726,8 @@
       <c r="T24" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>5164</t>
-        </is>
+      <c r="U24" t="n">
+        <v>5164</v>
       </c>
     </row>
     <row r="25">
@@ -2173,7 +2149,7 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>2530</t>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -2363,11 +2339,11 @@
         <v>4236</v>
       </c>
       <c r="T39" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>4236</t>
+          <t>4543</t>
         </is>
       </c>
     </row>
@@ -2436,11 +2412,11 @@
         <v>4301</v>
       </c>
       <c r="T40" s="5" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="U40" t="inlineStr">
         <is>
-          <t>4301</t>
+          <t>4607</t>
         </is>
       </c>
     </row>
@@ -2548,7 +2524,7 @@
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>4616</t>
+          <t>4673</t>
         </is>
       </c>
     </row>
@@ -2651,8 +2627,8 @@
       <c r="S44" t="n">
         <v>4372</v>
       </c>
-      <c r="T44" s="3" t="n">
-        <v>21</v>
+      <c r="T44" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
@@ -2729,7 +2705,7 @@
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>4396</t>
+          <t>4502</t>
         </is>
       </c>
     </row>
@@ -2797,12 +2773,12 @@
       <c r="S46" t="n">
         <v>3066</v>
       </c>
-      <c r="T46" s="2" t="n">
-        <v>0</v>
+      <c r="T46" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>3066</t>
+          <t>3402</t>
         </is>
       </c>
     </row>
@@ -2870,8 +2846,8 @@
       <c r="S47" t="n">
         <v>3349</v>
       </c>
-      <c r="T47" s="5" t="n">
-        <v>11</v>
+      <c r="T47" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
@@ -2948,7 +2924,7 @@
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3176,7 +3152,7 @@
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>4796</t>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3225,7 @@
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>4615</t>
+          <t>4732</t>
         </is>
       </c>
     </row>
@@ -3357,7 +3333,7 @@
       </c>
       <c r="U55" t="inlineStr">
         <is>
-          <t>4907</t>
+          <t>4986</t>
         </is>
       </c>
     </row>
@@ -3430,7 +3406,7 @@
       </c>
       <c r="U56" t="inlineStr">
         <is>
-          <t>4967</t>
+          <t>5235</t>
         </is>
       </c>
     </row>
@@ -3499,11 +3475,11 @@
         <v>4917</v>
       </c>
       <c r="T57" s="3" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>4917</t>
+          <t>4953</t>
         </is>
       </c>
     </row>
@@ -3572,11 +3548,11 @@
         <v>4674</v>
       </c>
       <c r="T58" s="4" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>4674</t>
+          <t>4817</t>
         </is>
       </c>
     </row>
@@ -3649,7 +3625,7 @@
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>4621</t>
+          <t>4783</t>
         </is>
       </c>
     </row>
@@ -3722,7 +3698,7 @@
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>4617</t>
+          <t>4830</t>
         </is>
       </c>
     </row>
@@ -3790,12 +3766,12 @@
       <c r="S61" t="n">
         <v>4129</v>
       </c>
-      <c r="T61" s="5" t="n">
-        <v>11</v>
+      <c r="T61" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>4129</t>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -3864,11 +3840,11 @@
         <v>5357</v>
       </c>
       <c r="T62" s="4" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>5357</t>
+          <t>5615</t>
         </is>
       </c>
     </row>
@@ -3937,11 +3913,11 @@
         <v>5127</v>
       </c>
       <c r="T63" s="3" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>5127</t>
+          <t>5334</t>
         </is>
       </c>
     </row>
@@ -4014,7 +3990,7 @@
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>5196</t>
+          <t>5285</t>
         </is>
       </c>
     </row>
@@ -4117,12 +4093,12 @@
       <c r="S66" t="n">
         <v>4887</v>
       </c>
-      <c r="T66" s="3" t="n">
-        <v>23</v>
+      <c r="T66" s="4" t="n">
+        <v>33</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>4887</t>
+          <t>5018</t>
         </is>
       </c>
     </row>
@@ -4191,11 +4167,11 @@
         <v>4553</v>
       </c>
       <c r="T67" s="3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U67" t="inlineStr">
         <is>
-          <t>4553</t>
+          <t>4739</t>
         </is>
       </c>
     </row>
@@ -4264,11 +4240,11 @@
         <v>4472</v>
       </c>
       <c r="T68" s="4" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>4472</t>
+          <t>4798</t>
         </is>
       </c>
     </row>
@@ -4341,7 +4317,7 @@
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>4397</t>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -4414,7 +4390,7 @@
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>4506</t>
+          <t>4612</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4463,7 @@
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>4877</t>
+          <t>5150</t>
         </is>
       </c>
     </row>
@@ -4560,7 +4536,7 @@
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>4479</t>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -4633,7 +4609,7 @@
       </c>
       <c r="U73" t="inlineStr">
         <is>
-          <t>3235</t>
+          <t>3231</t>
         </is>
       </c>
     </row>
@@ -4701,12 +4677,12 @@
       <c r="S74" t="n">
         <v>3870</v>
       </c>
-      <c r="T74" s="5" t="n">
-        <v>11</v>
+      <c r="T74" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>3870</t>
+          <t>4225</t>
         </is>
       </c>
     </row>
@@ -4779,7 +4755,7 @@
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>3085</t>
+          <t>3129</t>
         </is>
       </c>
     </row>
@@ -4852,7 +4828,7 @@
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>3444</t>
+          <t>3454</t>
         </is>
       </c>
     </row>
@@ -4920,12 +4896,12 @@
       <c r="S77" t="n">
         <v>4195</v>
       </c>
-      <c r="T77" s="5" t="n">
-        <v>12</v>
+      <c r="T77" s="3" t="n">
+        <v>28</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>4195</t>
+          <t>4420</t>
         </is>
       </c>
     </row>
@@ -4998,7 +4974,7 @@
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>4033</t>
+          <t>4237</t>
         </is>
       </c>
     </row>
@@ -5071,7 +5047,7 @@
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>3875</t>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -5144,7 +5120,7 @@
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>3979</t>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -5213,11 +5189,11 @@
         <v>3771</v>
       </c>
       <c r="T81" s="3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>3771</t>
+          <t>3914</t>
         </is>
       </c>
     </row>
@@ -5290,7 +5266,7 @@
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>3972</t>
+          <t>4056</t>
         </is>
       </c>
     </row>
@@ -5358,12 +5334,12 @@
       <c r="S83" t="n">
         <v>2592</v>
       </c>
-      <c r="T83" s="2" t="n">
-        <v>0</v>
+      <c r="T83" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>2592</t>
+          <t>2627</t>
         </is>
       </c>
     </row>
@@ -5727,12 +5703,12 @@
       <c r="S90" t="n">
         <v>4793</v>
       </c>
-      <c r="T90" s="4" t="n">
-        <v>32</v>
+      <c r="T90" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="U90" t="inlineStr">
         <is>
-          <t>4793</t>
+          <t>4976</t>
         </is>
       </c>
     </row>
@@ -5878,7 +5854,7 @@
       </c>
       <c r="U92" t="inlineStr">
         <is>
-          <t>2713</t>
+          <t>2708</t>
         </is>
       </c>
     </row>
@@ -6020,11 +5996,11 @@
         <v>4483</v>
       </c>
       <c r="T94" s="3" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>4483</t>
+          <t>4681</t>
         </is>
       </c>
     </row>
@@ -6092,12 +6068,12 @@
       <c r="S95" t="n">
         <v>4484</v>
       </c>
-      <c r="T95" s="3" t="n">
-        <v>20</v>
+      <c r="T95" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>4484</t>
+          <t>4477</t>
         </is>
       </c>
     </row>
@@ -6170,7 +6146,7 @@
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>2885</t>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -6238,12 +6214,12 @@
       <c r="S97" t="n">
         <v>4226</v>
       </c>
-      <c r="T97" s="5" t="n">
-        <v>3</v>
+      <c r="T97" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>4226</t>
+          <t>4295</t>
         </is>
       </c>
     </row>
@@ -6316,7 +6292,7 @@
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>3111</t>
+          <t>3204</t>
         </is>
       </c>
     </row>
@@ -6385,11 +6361,11 @@
         <v>3693</v>
       </c>
       <c r="T99" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>3693</t>
+          <t>3846</t>
         </is>
       </c>
     </row>
@@ -6458,11 +6434,11 @@
         <v>4125</v>
       </c>
       <c r="T100" s="3" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="U100" t="inlineStr">
         <is>
-          <t>4125</t>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -6535,7 +6511,7 @@
       </c>
       <c r="U101" t="inlineStr">
         <is>
-          <t>4465</t>
+          <t>4545</t>
         </is>
       </c>
     </row>
@@ -6603,12 +6579,12 @@
       <c r="S102" t="n">
         <v>4186</v>
       </c>
-      <c r="T102" s="5" t="n">
-        <v>13</v>
+      <c r="T102" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>4186</t>
+          <t>4350</t>
         </is>
       </c>
     </row>
@@ -6676,12 +6652,12 @@
       <c r="S103" t="n">
         <v>4038</v>
       </c>
-      <c r="T103" s="5" t="n">
-        <v>18</v>
+      <c r="T103" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>4038</t>
+          <t>4123</t>
         </is>
       </c>
     </row>
@@ -6754,7 +6730,7 @@
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>3993</t>
+          <t>4017</t>
         </is>
       </c>
     </row>
@@ -6896,11 +6872,11 @@
         <v>4013</v>
       </c>
       <c r="T106" s="3" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>4013</t>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -6973,7 +6949,7 @@
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>4061</t>
+          <t>4077</t>
         </is>
       </c>
     </row>
@@ -7046,7 +7022,7 @@
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>4114</t>
+          <t>4132</t>
         </is>
       </c>
     </row>
@@ -7114,12 +7090,12 @@
       <c r="S109" t="n">
         <v>2972</v>
       </c>
-      <c r="T109" s="2" t="n">
-        <v>0</v>
+      <c r="T109" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>2972</t>
+          <t>3032</t>
         </is>
       </c>
     </row>
@@ -7192,7 +7168,7 @@
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>3992</t>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -7295,12 +7271,12 @@
       <c r="S112" t="n">
         <v>3995</v>
       </c>
-      <c r="T112" s="5" t="n">
-        <v>5</v>
+      <c r="T112" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>3995</t>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -7369,11 +7345,11 @@
         <v>3327</v>
       </c>
       <c r="T113" s="5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>3327</t>
+          <t>3379</t>
         </is>
       </c>
     </row>
@@ -7519,7 +7495,7 @@
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>3134</t>
+          <t>3217</t>
         </is>
       </c>
     </row>
@@ -7592,7 +7568,7 @@
       </c>
       <c r="U116" t="inlineStr">
         <is>
-          <t>3001</t>
+          <t>3043</t>
         </is>
       </c>
     </row>
@@ -7743,7 +7719,7 @@
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>2769</t>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -7814,10 +7790,8 @@
       <c r="T120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>2807</t>
-        </is>
+      <c r="U120" t="n">
+        <v>2807</v>
       </c>
     </row>
     <row r="121">
@@ -7889,7 +7863,7 @@
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>2697</t>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -7957,12 +7931,12 @@
       <c r="S122" t="n">
         <v>2971</v>
       </c>
-      <c r="T122" s="3" t="n">
-        <v>20</v>
+      <c r="T122" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>2971</t>
+          <t>2992</t>
         </is>
       </c>
     </row>
@@ -8090,7 +8064,7 @@
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>2478</t>
+          <t>2466</t>
         </is>
       </c>
     </row>
@@ -8236,7 +8210,7 @@
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>1481</t>
+          <t>1474</t>
         </is>
       </c>
     </row>
@@ -8382,7 +8356,7 @@
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>1209</t>
+          <t>1208</t>
         </is>
       </c>
     </row>
@@ -8893,7 +8867,7 @@
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>2808</t>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -8903,7 +8877,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Jialong</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -8961,12 +8935,12 @@
       <c r="S136" t="n">
         <v>3209</v>
       </c>
-      <c r="T136" s="2" t="n">
-        <v>0</v>
+      <c r="T136" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>3209</t>
+          <t>3476</t>
         </is>
       </c>
     </row>
@@ -9112,7 +9086,7 @@
       </c>
       <c r="U138" t="inlineStr">
         <is>
-          <t>2742</t>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -9404,7 +9378,7 @@
       </c>
       <c r="U142" t="inlineStr">
         <is>
-          <t>1702</t>
+          <t>1735</t>
         </is>
       </c>
     </row>
@@ -10061,7 +10035,7 @@
       </c>
       <c r="U151" t="inlineStr">
         <is>
-          <t>2617</t>
+          <t>2789</t>
         </is>
       </c>
     </row>
@@ -10639,7 +10613,7 @@
       </c>
       <c r="U159" t="inlineStr">
         <is>
-          <t>2664</t>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -10706,7 +10680,7 @@
       </c>
       <c r="U160" t="inlineStr">
         <is>
-          <t>1737</t>
+          <t>1760</t>
         </is>
       </c>
     </row>
@@ -10773,7 +10747,7 @@
       </c>
       <c r="U161" t="inlineStr">
         <is>
-          <t>1585</t>
+          <t>1600</t>
         </is>
       </c>
     </row>
@@ -10836,7 +10810,7 @@
       </c>
       <c r="U162" t="inlineStr">
         <is>
-          <t>2296</t>
+          <t>2306</t>
         </is>
       </c>
     </row>
@@ -10895,7 +10869,7 @@
       </c>
       <c r="U163" t="inlineStr">
         <is>
-          <t>2830</t>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -10985,10 +10959,8 @@
       <c r="T165" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U165" t="inlineStr">
-        <is>
-          <t>5777</t>
-        </is>
+      <c r="U165" t="n">
+        <v>5777</v>
       </c>
     </row>
     <row r="166">
@@ -11034,7 +11006,48 @@
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>2999</t>
+          <t>3122</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>58379115</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Player-58379115</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr"/>
+      <c r="D167" t="inlineStr"/>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F167" s="3" t="inlineStr"/>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" s="3" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" s="3" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
+      <c r="L167" s="3" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" s="3" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" s="3" t="inlineStr"/>
+      <c r="Q167" t="inlineStr"/>
+      <c r="R167" s="3" t="inlineStr"/>
+      <c r="S167" t="inlineStr"/>
+      <c r="T167" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>2059</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-05 11:31:00
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U167"/>
+  <dimension ref="A1:W168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>04-03_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>04-04_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>04-04_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -567,6 +577,8 @@
       <c r="U2" t="n">
         <v>2585</v>
       </c>
+      <c r="V2" s="3" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -602,6 +614,8 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" s="3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
+      <c r="V3" s="3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -637,6 +651,8 @@
       <c r="S4" t="inlineStr"/>
       <c r="T4" s="3" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
+      <c r="V4" s="3" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -692,6 +708,8 @@
       <c r="U5" t="n">
         <v>5464</v>
       </c>
+      <c r="V5" s="3" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -727,6 +745,8 @@
       <c r="S6" t="inlineStr"/>
       <c r="T6" s="3" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
+      <c r="V6" s="3" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -762,6 +782,8 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" s="3" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" s="3" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -821,6 +843,8 @@
       <c r="U8" t="n">
         <v>5923</v>
       </c>
+      <c r="V8" s="3" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -856,6 +880,8 @@
       <c r="S9" t="inlineStr"/>
       <c r="T9" s="3" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
+      <c r="V9" s="3" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -927,6 +953,8 @@
       <c r="U10" t="n">
         <v>5845</v>
       </c>
+      <c r="V10" s="3" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -971,11 +999,11 @@
       <c r="T11" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>5695</t>
-        </is>
-      </c>
+      <c r="U11" t="n">
+        <v>5695</v>
+      </c>
+      <c r="V11" s="3" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1047,6 +1075,8 @@
       <c r="U12" t="n">
         <v>4958</v>
       </c>
+      <c r="V12" s="3" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1115,9 +1145,15 @@
       <c r="T13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>5317</t>
+      <c r="U13" t="n">
+        <v>5317</v>
+      </c>
+      <c r="V13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>5544</t>
         </is>
       </c>
     </row>
@@ -1191,6 +1227,8 @@
       <c r="U14" t="n">
         <v>5109</v>
       </c>
+      <c r="V14" s="3" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1262,6 +1300,8 @@
       <c r="U15" t="n">
         <v>4429</v>
       </c>
+      <c r="V15" s="3" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1309,6 +1349,8 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" s="3" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
+      <c r="V16" s="3" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1368,6 +1410,8 @@
       <c r="U17" t="n">
         <v>5854</v>
       </c>
+      <c r="V17" s="3" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1423,6 +1467,8 @@
       <c r="U18" t="n">
         <v>6069</v>
       </c>
+      <c r="V18" s="3" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1470,6 +1516,8 @@
       <c r="S19" t="inlineStr"/>
       <c r="T19" s="3" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
+      <c r="V19" s="3" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1505,6 +1553,8 @@
       <c r="S20" t="inlineStr"/>
       <c r="T20" s="3" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
+      <c r="V20" s="3" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1568,6 +1618,8 @@
       <c r="U21" t="n">
         <v>5681</v>
       </c>
+      <c r="V21" s="3" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1603,6 +1655,8 @@
       <c r="S22" t="inlineStr"/>
       <c r="T22" s="3" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
+      <c r="V22" s="3" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1658,6 +1712,8 @@
       <c r="U23" t="n">
         <v>5753</v>
       </c>
+      <c r="V23" s="3" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1729,6 +1785,8 @@
       <c r="U24" t="n">
         <v>5164</v>
       </c>
+      <c r="V24" s="3" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1764,6 +1822,8 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" s="3" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
+      <c r="V25" s="3" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1799,6 +1859,8 @@
       <c r="S26" t="inlineStr"/>
       <c r="T26" s="3" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
+      <c r="V26" s="3" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1834,6 +1896,8 @@
       <c r="S27" t="inlineStr"/>
       <c r="T27" s="3" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
+      <c r="V27" s="3" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1869,6 +1933,8 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" s="3" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
+      <c r="V28" s="3" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1904,6 +1970,8 @@
       <c r="S29" t="inlineStr"/>
       <c r="T29" s="3" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
+      <c r="V29" s="3" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1939,6 +2007,8 @@
       <c r="S30" t="inlineStr"/>
       <c r="T30" s="3" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
+      <c r="V30" s="3" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1974,6 +2044,8 @@
       <c r="S31" t="inlineStr"/>
       <c r="T31" s="3" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
+      <c r="V31" s="3" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2009,6 +2081,8 @@
       <c r="S32" t="inlineStr"/>
       <c r="T32" s="3" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
+      <c r="V32" s="3" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2044,6 +2118,8 @@
       <c r="S33" t="inlineStr"/>
       <c r="T33" s="3" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
+      <c r="V33" s="3" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2079,6 +2155,8 @@
       <c r="S34" t="inlineStr"/>
       <c r="T34" s="3" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
+      <c r="V34" s="3" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2147,7 +2225,13 @@
       <c r="T35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="U35" t="n">
+        <v>2529</v>
+      </c>
+      <c r="V35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="inlineStr">
         <is>
           <t>2529</t>
         </is>
@@ -2203,6 +2287,8 @@
       <c r="S36" t="inlineStr"/>
       <c r="T36" s="3" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
+      <c r="V36" s="3" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2238,6 +2324,8 @@
       <c r="S37" t="inlineStr"/>
       <c r="T37" s="3" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
+      <c r="V37" s="3" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2273,6 +2361,8 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" s="3" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
+      <c r="V38" s="3" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2341,9 +2431,15 @@
       <c r="T39" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>4543</t>
+      <c r="U39" t="n">
+        <v>4543</v>
+      </c>
+      <c r="V39" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>4922</t>
         </is>
       </c>
     </row>
@@ -2366,7 +2462,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F40" s="3" t="n">
@@ -2414,9 +2510,15 @@
       <c r="T40" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>4607</t>
+      <c r="U40" t="n">
+        <v>4607</v>
+      </c>
+      <c r="V40" s="5" t="n">
+        <v>19</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>4897</t>
         </is>
       </c>
     </row>
@@ -2454,6 +2556,8 @@
       <c r="S41" t="inlineStr"/>
       <c r="T41" s="3" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
+      <c r="V41" s="3" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2522,9 +2626,15 @@
       <c r="T42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>4673</t>
+      <c r="U42" t="n">
+        <v>4673</v>
+      </c>
+      <c r="V42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>4867</t>
         </is>
       </c>
     </row>
@@ -2562,6 +2672,8 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" s="3" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" s="3" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2630,7 +2742,13 @@
       <c r="T44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U44" t="inlineStr">
+      <c r="U44" t="n">
+        <v>4372</v>
+      </c>
+      <c r="V44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W44" t="inlineStr">
         <is>
           <t>4372</t>
         </is>
@@ -2703,9 +2821,15 @@
       <c r="T45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>4502</t>
+      <c r="U45" t="n">
+        <v>4502</v>
+      </c>
+      <c r="V45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>4677</t>
         </is>
       </c>
     </row>
@@ -2776,7 +2900,13 @@
       <c r="T46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U46" t="inlineStr">
+      <c r="U46" t="n">
+        <v>3402</v>
+      </c>
+      <c r="V46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W46" t="inlineStr">
         <is>
           <t>3402</t>
         </is>
@@ -2849,7 +2979,13 @@
       <c r="T47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="U47" t="n">
+        <v>3349</v>
+      </c>
+      <c r="V47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W47" t="inlineStr">
         <is>
           <t>3349</t>
         </is>
@@ -2922,9 +3058,15 @@
       <c r="T48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="U48" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>2531</t>
         </is>
       </c>
     </row>
@@ -2995,7 +3137,13 @@
       <c r="T49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U49" t="inlineStr">
+      <c r="U49" t="n">
+        <v>0</v>
+      </c>
+      <c r="V49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3047,6 +3195,8 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" s="3" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
+      <c r="V50" s="3" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3082,6 +3232,8 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" s="3" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
+      <c r="V51" s="3" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3150,9 +3302,15 @@
       <c r="T52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="U52" t="n">
+        <v>5004</v>
+      </c>
+      <c r="V52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>5179</t>
         </is>
       </c>
     </row>
@@ -3223,9 +3381,15 @@
       <c r="T53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>4732</t>
+      <c r="U53" t="n">
+        <v>4732</v>
+      </c>
+      <c r="V53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>4825</t>
         </is>
       </c>
     </row>
@@ -3263,6 +3427,8 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" s="3" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
+      <c r="V54" s="3" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3331,9 +3497,15 @@
       <c r="T55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>4986</t>
+      <c r="U55" t="n">
+        <v>4986</v>
+      </c>
+      <c r="V55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>5301</t>
         </is>
       </c>
     </row>
@@ -3404,9 +3576,15 @@
       <c r="T56" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>5235</t>
+      <c r="U56" t="n">
+        <v>5235</v>
+      </c>
+      <c r="V56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>5382</t>
         </is>
       </c>
     </row>
@@ -3477,9 +3655,15 @@
       <c r="T57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>4953</t>
+      <c r="U57" t="n">
+        <v>4953</v>
+      </c>
+      <c r="V57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>5194</t>
         </is>
       </c>
     </row>
@@ -3550,9 +3734,15 @@
       <c r="T58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>4817</t>
+      <c r="U58" t="n">
+        <v>4817</v>
+      </c>
+      <c r="V58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -3623,9 +3813,15 @@
       <c r="T59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>4783</t>
+      <c r="U59" t="n">
+        <v>4783</v>
+      </c>
+      <c r="V59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>4917</t>
         </is>
       </c>
     </row>
@@ -3696,9 +3892,15 @@
       <c r="T60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>4830</t>
+      <c r="U60" t="n">
+        <v>4830</v>
+      </c>
+      <c r="V60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>4930</t>
         </is>
       </c>
     </row>
@@ -3769,9 +3971,15 @@
       <c r="T61" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="U61" t="n">
+        <v>4383</v>
+      </c>
+      <c r="V61" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>4574</t>
         </is>
       </c>
     </row>
@@ -3842,9 +4050,15 @@
       <c r="T62" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>5615</t>
+      <c r="U62" t="n">
+        <v>5615</v>
+      </c>
+      <c r="V62" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>5810</t>
         </is>
       </c>
     </row>
@@ -3915,9 +4129,15 @@
       <c r="T63" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>5334</t>
+      <c r="U63" t="n">
+        <v>5334</v>
+      </c>
+      <c r="V63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>5566</t>
         </is>
       </c>
     </row>
@@ -3988,9 +4208,15 @@
       <c r="T64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>5285</t>
+      <c r="U64" t="n">
+        <v>5285</v>
+      </c>
+      <c r="V64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>5505</t>
         </is>
       </c>
     </row>
@@ -4028,6 +4254,8 @@
       <c r="S65" t="inlineStr"/>
       <c r="T65" s="3" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
+      <c r="V65" s="3" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4096,9 +4324,15 @@
       <c r="T66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>5018</t>
+      <c r="U66" t="n">
+        <v>5018</v>
+      </c>
+      <c r="V66" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>5076</t>
         </is>
       </c>
     </row>
@@ -4169,9 +4403,15 @@
       <c r="T67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>4739</t>
+      <c r="U67" t="n">
+        <v>4739</v>
+      </c>
+      <c r="V67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>4901</t>
         </is>
       </c>
     </row>
@@ -4242,9 +4482,15 @@
       <c r="T68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="U68" t="inlineStr">
-        <is>
-          <t>4798</t>
+      <c r="U68" t="n">
+        <v>4798</v>
+      </c>
+      <c r="V68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>5000</t>
         </is>
       </c>
     </row>
@@ -4315,9 +4561,15 @@
       <c r="T69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="U69" t="n">
+        <v>4525</v>
+      </c>
+      <c r="V69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -4388,9 +4640,15 @@
       <c r="T70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U70" t="inlineStr">
-        <is>
-          <t>4612</t>
+      <c r="U70" t="n">
+        <v>4612</v>
+      </c>
+      <c r="V70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -4461,9 +4719,15 @@
       <c r="T71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>5150</t>
+      <c r="U71" t="n">
+        <v>5150</v>
+      </c>
+      <c r="V71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>5355</t>
         </is>
       </c>
     </row>
@@ -4534,9 +4798,15 @@
       <c r="T72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="U72" t="n">
+        <v>4601</v>
+      </c>
+      <c r="V72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>4749</t>
         </is>
       </c>
     </row>
@@ -4607,9 +4877,15 @@
       <c r="T73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>3231</t>
+      <c r="U73" t="n">
+        <v>3231</v>
+      </c>
+      <c r="V73" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>3291</t>
         </is>
       </c>
     </row>
@@ -4680,9 +4956,15 @@
       <c r="T74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>4225</t>
+      <c r="U74" t="n">
+        <v>4225</v>
+      </c>
+      <c r="V74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>4478</t>
         </is>
       </c>
     </row>
@@ -4753,9 +5035,15 @@
       <c r="T75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U75" t="inlineStr">
-        <is>
-          <t>3129</t>
+      <c r="U75" t="n">
+        <v>3129</v>
+      </c>
+      <c r="V75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>3232</t>
         </is>
       </c>
     </row>
@@ -4826,9 +5114,15 @@
       <c r="T76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>3454</t>
+      <c r="U76" t="n">
+        <v>3454</v>
+      </c>
+      <c r="V76" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>3554</t>
         </is>
       </c>
     </row>
@@ -4899,9 +5193,15 @@
       <c r="T77" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>4420</t>
+      <c r="U77" t="n">
+        <v>4420</v>
+      </c>
+      <c r="V77" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>4550</t>
         </is>
       </c>
     </row>
@@ -4972,9 +5272,15 @@
       <c r="T78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U78" t="inlineStr">
-        <is>
-          <t>4237</t>
+      <c r="U78" t="n">
+        <v>4237</v>
+      </c>
+      <c r="V78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>4264</t>
         </is>
       </c>
     </row>
@@ -5045,9 +5351,15 @@
       <c r="T79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U79" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="U79" t="n">
+        <v>3991</v>
+      </c>
+      <c r="V79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -5118,9 +5430,15 @@
       <c r="T80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U80" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="U80" t="n">
+        <v>4076</v>
+      </c>
+      <c r="V80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>4045</t>
         </is>
       </c>
     </row>
@@ -5191,9 +5509,15 @@
       <c r="T81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U81" t="inlineStr">
-        <is>
-          <t>3914</t>
+      <c r="U81" t="n">
+        <v>3914</v>
+      </c>
+      <c r="V81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W81" t="inlineStr">
+        <is>
+          <t>4019</t>
         </is>
       </c>
     </row>
@@ -5264,9 +5588,15 @@
       <c r="T82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U82" t="inlineStr">
-        <is>
-          <t>4056</t>
+      <c r="U82" t="n">
+        <v>4056</v>
+      </c>
+      <c r="V82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>4059</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5667,13 @@
       <c r="T83" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U83" t="inlineStr">
+      <c r="U83" t="n">
+        <v>2627</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W83" t="inlineStr">
         <is>
           <t>2627</t>
         </is>
@@ -5393,6 +5729,8 @@
       <c r="S84" t="inlineStr"/>
       <c r="T84" s="3" t="inlineStr"/>
       <c r="U84" t="inlineStr"/>
+      <c r="V84" s="3" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5436,6 +5774,8 @@
       <c r="S85" t="inlineStr"/>
       <c r="T85" s="3" t="inlineStr"/>
       <c r="U85" t="inlineStr"/>
+      <c r="V85" s="3" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5487,6 +5827,8 @@
       <c r="S86" t="inlineStr"/>
       <c r="T86" s="3" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
+      <c r="V86" s="3" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5555,7 +5897,13 @@
       <c r="T87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U87" t="inlineStr">
+      <c r="U87" t="n">
+        <v>4189</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="inlineStr">
         <is>
           <t>4189</t>
         </is>
@@ -5603,6 +5951,8 @@
       <c r="S88" t="inlineStr"/>
       <c r="T88" s="3" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
+      <c r="V88" s="3" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5638,6 +5988,8 @@
       <c r="S89" t="inlineStr"/>
       <c r="T89" s="3" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
+      <c r="V89" s="3" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -5706,9 +6058,15 @@
       <c r="T90" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U90" t="inlineStr">
-        <is>
-          <t>4976</t>
+      <c r="U90" t="n">
+        <v>4976</v>
+      </c>
+      <c r="V90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="W90" t="inlineStr">
+        <is>
+          <t>5103</t>
         </is>
       </c>
     </row>
@@ -5779,7 +6137,13 @@
       <c r="T91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U91" t="inlineStr">
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+      <c r="V91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5852,9 +6216,15 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
-        <is>
-          <t>2708</t>
+      <c r="U92" t="n">
+        <v>2708</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -5925,7 +6295,13 @@
       <c r="T93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U93" t="inlineStr">
+      <c r="U93" t="n">
+        <v>2516</v>
+      </c>
+      <c r="V93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W93" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -5998,9 +6374,15 @@
       <c r="T94" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="U94" t="inlineStr">
-        <is>
-          <t>4681</t>
+      <c r="U94" t="n">
+        <v>4681</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
+        <is>
+          <t>4687</t>
         </is>
       </c>
     </row>
@@ -6071,9 +6453,15 @@
       <c r="T95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="U95" t="n">
+        <v>4477</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="inlineStr">
+        <is>
+          <t>4523</t>
         </is>
       </c>
     </row>
@@ -6144,9 +6532,15 @@
       <c r="T96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="U96" t="n">
+        <v>2910</v>
+      </c>
+      <c r="V96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>2922</t>
         </is>
       </c>
     </row>
@@ -6217,9 +6611,15 @@
       <c r="T97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
-        <is>
-          <t>4295</t>
+      <c r="U97" t="n">
+        <v>4295</v>
+      </c>
+      <c r="V97" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W97" t="inlineStr">
+        <is>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -6290,9 +6690,15 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
-        <is>
-          <t>3204</t>
+      <c r="U98" t="n">
+        <v>3204</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
+        <is>
+          <t>3198</t>
         </is>
       </c>
     </row>
@@ -6363,9 +6769,15 @@
       <c r="T99" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="U99" t="inlineStr">
-        <is>
-          <t>3846</t>
+      <c r="U99" t="n">
+        <v>3846</v>
+      </c>
+      <c r="V99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -6436,9 +6848,15 @@
       <c r="T100" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="U100" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="U100" t="n">
+        <v>4281</v>
+      </c>
+      <c r="V100" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>4321</t>
         </is>
       </c>
     </row>
@@ -6509,9 +6927,15 @@
       <c r="T101" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U101" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="U101" t="n">
+        <v>4545</v>
+      </c>
+      <c r="V101" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W101" t="inlineStr">
+        <is>
+          <t>4618</t>
         </is>
       </c>
     </row>
@@ -6582,9 +7006,15 @@
       <c r="T102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>4350</t>
+      <c r="U102" t="n">
+        <v>4350</v>
+      </c>
+      <c r="V102" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>4353</t>
         </is>
       </c>
     </row>
@@ -6655,9 +7085,15 @@
       <c r="T103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U103" t="inlineStr">
-        <is>
-          <t>4123</t>
+      <c r="U103" t="n">
+        <v>4123</v>
+      </c>
+      <c r="V103" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W103" t="inlineStr">
+        <is>
+          <t>4253</t>
         </is>
       </c>
     </row>
@@ -6728,9 +7164,15 @@
       <c r="T104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U104" t="inlineStr">
-        <is>
-          <t>4017</t>
+      <c r="U104" t="n">
+        <v>4017</v>
+      </c>
+      <c r="V104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W104" t="inlineStr">
+        <is>
+          <t>4174</t>
         </is>
       </c>
     </row>
@@ -6801,7 +7243,13 @@
       <c r="T105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U105" t="inlineStr">
+      <c r="U105" t="n">
+        <v>0</v>
+      </c>
+      <c r="V105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6874,9 +7322,15 @@
       <c r="T106" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U106" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="U106" t="n">
+        <v>4167</v>
+      </c>
+      <c r="V106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W106" t="inlineStr">
+        <is>
+          <t>4251</t>
         </is>
       </c>
     </row>
@@ -6947,9 +7401,15 @@
       <c r="T107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U107" t="inlineStr">
-        <is>
-          <t>4077</t>
+      <c r="U107" t="n">
+        <v>4077</v>
+      </c>
+      <c r="V107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W107" t="inlineStr">
+        <is>
+          <t>4252</t>
         </is>
       </c>
     </row>
@@ -7020,9 +7480,15 @@
       <c r="T108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U108" t="inlineStr">
-        <is>
-          <t>4132</t>
+      <c r="U108" t="n">
+        <v>4132</v>
+      </c>
+      <c r="V108" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="W108" t="inlineStr">
+        <is>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -7093,7 +7559,13 @@
       <c r="T109" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="U109" t="inlineStr">
+      <c r="U109" t="n">
+        <v>3032</v>
+      </c>
+      <c r="V109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W109" t="inlineStr">
         <is>
           <t>3032</t>
         </is>
@@ -7166,9 +7638,15 @@
       <c r="T110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U110" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="U110" t="n">
+        <v>3996</v>
+      </c>
+      <c r="V110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W110" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -7206,6 +7684,8 @@
       <c r="S111" t="inlineStr"/>
       <c r="T111" s="3" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
+      <c r="V111" s="3" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7274,9 +7754,15 @@
       <c r="T112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="U112" t="n">
+        <v>3991</v>
+      </c>
+      <c r="V112" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -7347,9 +7833,15 @@
       <c r="T113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>3379</t>
+      <c r="U113" t="n">
+        <v>3379</v>
+      </c>
+      <c r="V113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>3423</t>
         </is>
       </c>
     </row>
@@ -7420,7 +7912,13 @@
       <c r="T114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U114" t="inlineStr">
+      <c r="U114" t="n">
+        <v>0</v>
+      </c>
+      <c r="V114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7493,9 +7991,15 @@
       <c r="T115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>3217</t>
+      <c r="U115" t="n">
+        <v>3217</v>
+      </c>
+      <c r="V115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>3287</t>
         </is>
       </c>
     </row>
@@ -7566,9 +8070,15 @@
       <c r="T116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>3043</t>
+      <c r="U116" t="n">
+        <v>3043</v>
+      </c>
+      <c r="V116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>3149</t>
         </is>
       </c>
     </row>
@@ -7614,6 +8124,8 @@
       <c r="S117" t="inlineStr"/>
       <c r="T117" s="3" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
+      <c r="V117" s="3" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7649,6 +8161,8 @@
       <c r="S118" t="inlineStr"/>
       <c r="T118" s="3" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
+      <c r="V118" s="3" t="inlineStr"/>
+      <c r="W118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -7717,9 +8231,15 @@
       <c r="T119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U119" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="U119" t="n">
+        <v>2765</v>
+      </c>
+      <c r="V119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W119" t="inlineStr">
+        <is>
+          <t>2757</t>
         </is>
       </c>
     </row>
@@ -7793,6 +8313,8 @@
       <c r="U120" t="n">
         <v>2807</v>
       </c>
+      <c r="V120" s="3" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -7861,9 +8383,15 @@
       <c r="T121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="U121" t="n">
+        <v>2750</v>
+      </c>
+      <c r="V121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>2808</t>
         </is>
       </c>
     </row>
@@ -7934,9 +8462,15 @@
       <c r="T122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>2992</t>
+      <c r="U122" t="n">
+        <v>2992</v>
+      </c>
+      <c r="V122" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>3017</t>
         </is>
       </c>
     </row>
@@ -7994,6 +8528,8 @@
       <c r="S123" t="inlineStr"/>
       <c r="T123" s="3" t="inlineStr"/>
       <c r="U123" t="inlineStr"/>
+      <c r="V123" s="3" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -8062,9 +8598,15 @@
       <c r="T124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>2466</t>
+      <c r="U124" t="n">
+        <v>2466</v>
+      </c>
+      <c r="V124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>2454</t>
         </is>
       </c>
     </row>
@@ -8135,7 +8677,13 @@
       <c r="T125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U125" t="inlineStr">
+      <c r="U125" t="n">
+        <v>0</v>
+      </c>
+      <c r="V125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8208,9 +8756,15 @@
       <c r="T126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>1474</t>
+      <c r="U126" t="n">
+        <v>1474</v>
+      </c>
+      <c r="V126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>1470</t>
         </is>
       </c>
     </row>
@@ -8281,9 +8835,15 @@
       <c r="T127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>1573</t>
+      <c r="U127" t="n">
+        <v>1573</v>
+      </c>
+      <c r="V127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>1601</t>
         </is>
       </c>
     </row>
@@ -8354,9 +8914,15 @@
       <c r="T128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>1208</t>
+      <c r="U128" t="n">
+        <v>1208</v>
+      </c>
+      <c r="V128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>1205</t>
         </is>
       </c>
     </row>
@@ -8427,7 +8993,13 @@
       <c r="T129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U129" t="inlineStr">
+      <c r="U129" t="n">
+        <v>0</v>
+      </c>
+      <c r="V129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8500,7 +9072,13 @@
       <c r="T130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U130" t="inlineStr">
+      <c r="U130" t="n">
+        <v>0</v>
+      </c>
+      <c r="V130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8573,7 +9151,13 @@
       <c r="T131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U131" t="inlineStr">
+      <c r="U131" t="n">
+        <v>0</v>
+      </c>
+      <c r="V131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8646,7 +9230,13 @@
       <c r="T132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U132" t="inlineStr">
+      <c r="U132" t="n">
+        <v>0</v>
+      </c>
+      <c r="V132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8719,7 +9309,13 @@
       <c r="T133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U133" t="inlineStr">
+      <c r="U133" t="n">
+        <v>0</v>
+      </c>
+      <c r="V133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8792,7 +9388,13 @@
       <c r="T134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U134" t="inlineStr">
+      <c r="U134" t="n">
+        <v>0</v>
+      </c>
+      <c r="V134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8865,9 +9467,15 @@
       <c r="T135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U135" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="U135" t="n">
+        <v>2893</v>
+      </c>
+      <c r="V135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W135" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -8877,7 +9485,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Jialong</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -8938,9 +9546,15 @@
       <c r="T136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U136" t="inlineStr">
-        <is>
-          <t>3476</t>
+      <c r="U136" t="n">
+        <v>3476</v>
+      </c>
+      <c r="V136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>3778</t>
         </is>
       </c>
     </row>
@@ -9011,7 +9625,13 @@
       <c r="T137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U137" t="inlineStr">
+      <c r="U137" t="n">
+        <v>0</v>
+      </c>
+      <c r="V137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9084,9 +9704,15 @@
       <c r="T138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U138" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="U138" t="n">
+        <v>2762</v>
+      </c>
+      <c r="V138" s="5" t="n">
+        <v>11</v>
+      </c>
+      <c r="W138" t="inlineStr">
+        <is>
+          <t>2909</t>
         </is>
       </c>
     </row>
@@ -9157,7 +9783,13 @@
       <c r="T139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U139" t="inlineStr">
+      <c r="U139" t="n">
+        <v>0</v>
+      </c>
+      <c r="V139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9230,7 +9862,13 @@
       <c r="T140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U140" t="inlineStr">
+      <c r="U140" t="n">
+        <v>0</v>
+      </c>
+      <c r="V140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9303,7 +9941,13 @@
       <c r="T141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U141" t="inlineStr">
+      <c r="U141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="V141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W141" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -9376,9 +10020,15 @@
       <c r="T142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U142" t="inlineStr">
-        <is>
-          <t>1735</t>
+      <c r="U142" t="n">
+        <v>1735</v>
+      </c>
+      <c r="V142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W142" t="inlineStr">
+        <is>
+          <t>1751</t>
         </is>
       </c>
     </row>
@@ -9449,7 +10099,13 @@
       <c r="T143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U143" t="inlineStr">
+      <c r="U143" t="n">
+        <v>0</v>
+      </c>
+      <c r="V143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9522,7 +10178,13 @@
       <c r="T144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U144" t="inlineStr">
+      <c r="U144" t="n">
+        <v>0</v>
+      </c>
+      <c r="V144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9595,7 +10257,13 @@
       <c r="T145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U145" t="inlineStr">
+      <c r="U145" t="n">
+        <v>0</v>
+      </c>
+      <c r="V145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9668,7 +10336,13 @@
       <c r="T146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U146" t="inlineStr">
+      <c r="U146" t="n">
+        <v>0</v>
+      </c>
+      <c r="V146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9741,7 +10415,13 @@
       <c r="T147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U147" t="inlineStr">
+      <c r="U147" t="n">
+        <v>0</v>
+      </c>
+      <c r="V147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9814,7 +10494,13 @@
       <c r="T148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U148" t="inlineStr">
+      <c r="U148" t="n">
+        <v>0</v>
+      </c>
+      <c r="V148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9887,7 +10573,13 @@
       <c r="T149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U149" t="inlineStr">
+      <c r="U149" t="n">
+        <v>0</v>
+      </c>
+      <c r="V149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9960,7 +10652,13 @@
       <c r="T150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U150" t="inlineStr">
+      <c r="U150" t="n">
+        <v>0</v>
+      </c>
+      <c r="V150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10033,9 +10731,15 @@
       <c r="T151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U151" t="inlineStr">
-        <is>
-          <t>2789</t>
+      <c r="U151" t="n">
+        <v>2789</v>
+      </c>
+      <c r="V151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W151" t="inlineStr">
+        <is>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -10106,7 +10810,13 @@
       <c r="T152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U152" t="inlineStr">
+      <c r="U152" t="n">
+        <v>0</v>
+      </c>
+      <c r="V152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10179,7 +10889,13 @@
       <c r="T153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U153" t="inlineStr">
+      <c r="U153" t="n">
+        <v>0</v>
+      </c>
+      <c r="V153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10252,7 +10968,13 @@
       <c r="T154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U154" t="inlineStr">
+      <c r="U154" t="n">
+        <v>0</v>
+      </c>
+      <c r="V154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10325,7 +11047,13 @@
       <c r="T155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U155" t="inlineStr">
+      <c r="U155" t="n">
+        <v>0</v>
+      </c>
+      <c r="V155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10398,7 +11126,13 @@
       <c r="T156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U156" t="inlineStr">
+      <c r="U156" t="n">
+        <v>0</v>
+      </c>
+      <c r="V156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10471,7 +11205,13 @@
       <c r="T157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U157" t="inlineStr">
+      <c r="U157" t="n">
+        <v>0</v>
+      </c>
+      <c r="V157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10544,7 +11284,13 @@
       <c r="T158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U158" t="inlineStr">
+      <c r="U158" t="n">
+        <v>0</v>
+      </c>
+      <c r="V158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10611,9 +11357,15 @@
       <c r="T159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U159" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="U159" t="n">
+        <v>2692</v>
+      </c>
+      <c r="V159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W159" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -10678,9 +11430,15 @@
       <c r="T160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U160" t="inlineStr">
-        <is>
-          <t>1760</t>
+      <c r="U160" t="n">
+        <v>1760</v>
+      </c>
+      <c r="V160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W160" t="inlineStr">
+        <is>
+          <t>1759</t>
         </is>
       </c>
     </row>
@@ -10745,9 +11503,15 @@
       <c r="T161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U161" t="inlineStr">
-        <is>
-          <t>1600</t>
+      <c r="U161" t="n">
+        <v>1600</v>
+      </c>
+      <c r="V161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W161" t="inlineStr">
+        <is>
+          <t>1599</t>
         </is>
       </c>
     </row>
@@ -10808,7 +11572,13 @@
       <c r="T162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U162" t="inlineStr">
+      <c r="U162" t="n">
+        <v>2306</v>
+      </c>
+      <c r="V162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W162" t="inlineStr">
         <is>
           <t>2306</t>
         </is>
@@ -10867,9 +11637,15 @@
       <c r="T163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U163" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="U163" t="n">
+        <v>2819</v>
+      </c>
+      <c r="V163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W163" t="inlineStr">
+        <is>
+          <t>2826</t>
         </is>
       </c>
     </row>
@@ -10913,6 +11689,8 @@
       <c r="S164" t="inlineStr"/>
       <c r="T164" s="3" t="inlineStr"/>
       <c r="U164" t="inlineStr"/>
+      <c r="V164" s="3" t="inlineStr"/>
+      <c r="W164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -10962,6 +11740,8 @@
       <c r="U165" t="n">
         <v>5777</v>
       </c>
+      <c r="V165" s="3" t="inlineStr"/>
+      <c r="W165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -11004,17 +11784,21 @@
       <c r="T166" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U166" t="inlineStr">
-        <is>
-          <t>3122</t>
+      <c r="U166" t="n">
+        <v>3122</v>
+      </c>
+      <c r="V166" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W166" t="inlineStr">
+        <is>
+          <t>3231</t>
         </is>
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>58379115</t>
-        </is>
+      <c r="A167" t="n">
+        <v>58379115</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -11045,9 +11829,52 @@
       <c r="T167" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="U167" t="inlineStr">
-        <is>
-          <t>2059</t>
+      <c r="U167" t="n">
+        <v>2059</v>
+      </c>
+      <c r="V167" s="3" t="inlineStr"/>
+      <c r="W167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>59112086</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>sigma</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr"/>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F168" s="3" t="inlineStr"/>
+      <c r="G168" t="inlineStr"/>
+      <c r="H168" s="3" t="inlineStr"/>
+      <c r="I168" t="inlineStr"/>
+      <c r="J168" s="3" t="inlineStr"/>
+      <c r="K168" t="inlineStr"/>
+      <c r="L168" s="3" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" s="3" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" s="3" t="inlineStr"/>
+      <c r="Q168" t="inlineStr"/>
+      <c r="R168" s="3" t="inlineStr"/>
+      <c r="S168" t="inlineStr"/>
+      <c r="T168" s="3" t="inlineStr"/>
+      <c r="U168" t="inlineStr"/>
+      <c r="V168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W168" t="inlineStr">
+        <is>
+          <t>1213</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-06 11:30:59
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W168"/>
+  <dimension ref="A1:Y169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
           <t>04-04_0</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>04-05_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>04-05_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -579,6 +589,8 @@
       </c>
       <c r="V2" s="3" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
+      <c r="X2" s="3" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -616,6 +628,8 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" s="3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
+      <c r="X3" s="3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -653,6 +667,8 @@
       <c r="U4" t="inlineStr"/>
       <c r="V4" s="3" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
+      <c r="X4" s="3" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -710,6 +726,8 @@
       </c>
       <c r="V5" s="3" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
+      <c r="X5" s="3" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -747,6 +765,8 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" s="3" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
+      <c r="X6" s="3" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -784,6 +804,8 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" s="3" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
+      <c r="X7" s="3" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -845,6 +867,8 @@
       </c>
       <c r="V8" s="3" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
+      <c r="X8" s="3" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -882,6 +906,8 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" s="3" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
+      <c r="X9" s="3" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -955,6 +981,8 @@
       </c>
       <c r="V10" s="3" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
+      <c r="X10" s="3" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1004,6 +1032,8 @@
       </c>
       <c r="V11" s="3" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
+      <c r="X11" s="3" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1077,6 +1107,8 @@
       </c>
       <c r="V12" s="3" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
+      <c r="X12" s="3" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1151,9 +1183,15 @@
       <c r="V13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>5544</t>
+      <c r="W13" t="n">
+        <v>5544</v>
+      </c>
+      <c r="X13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>5663</t>
         </is>
       </c>
     </row>
@@ -1229,6 +1267,8 @@
       </c>
       <c r="V14" s="3" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
+      <c r="X14" s="3" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1302,6 +1342,8 @@
       </c>
       <c r="V15" s="3" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
+      <c r="X15" s="3" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1351,6 +1393,8 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" s="3" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
+      <c r="X16" s="3" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1412,6 +1456,8 @@
       </c>
       <c r="V17" s="3" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
+      <c r="X17" s="3" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1469,6 +1515,8 @@
       </c>
       <c r="V18" s="3" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
+      <c r="X18" s="3" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1518,6 +1566,8 @@
       <c r="U19" t="inlineStr"/>
       <c r="V19" s="3" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
+      <c r="X19" s="3" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1555,6 +1605,8 @@
       <c r="U20" t="inlineStr"/>
       <c r="V20" s="3" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
+      <c r="X20" s="3" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1620,6 +1672,8 @@
       </c>
       <c r="V21" s="3" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
+      <c r="X21" s="3" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1657,6 +1711,8 @@
       <c r="U22" t="inlineStr"/>
       <c r="V22" s="3" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
+      <c r="X22" s="3" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1714,6 +1770,8 @@
       </c>
       <c r="V23" s="3" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
+      <c r="X23" s="3" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1787,6 +1845,8 @@
       </c>
       <c r="V24" s="3" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
+      <c r="X24" s="3" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1824,6 +1884,8 @@
       <c r="U25" t="inlineStr"/>
       <c r="V25" s="3" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
+      <c r="X25" s="3" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1861,6 +1923,8 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" s="3" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
+      <c r="X26" s="3" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1898,6 +1962,8 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" s="3" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
+      <c r="X27" s="3" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1935,6 +2001,8 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" s="3" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
+      <c r="X28" s="3" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1972,6 +2040,8 @@
       <c r="U29" t="inlineStr"/>
       <c r="V29" s="3" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
+      <c r="X29" s="3" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2009,6 +2079,8 @@
       <c r="U30" t="inlineStr"/>
       <c r="V30" s="3" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
+      <c r="X30" s="3" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2046,6 +2118,8 @@
       <c r="U31" t="inlineStr"/>
       <c r="V31" s="3" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
+      <c r="X31" s="3" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2083,6 +2157,8 @@
       <c r="U32" t="inlineStr"/>
       <c r="V32" s="3" t="inlineStr"/>
       <c r="W32" t="inlineStr"/>
+      <c r="X32" s="3" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2120,6 +2196,8 @@
       <c r="U33" t="inlineStr"/>
       <c r="V33" s="3" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
+      <c r="X33" s="3" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2157,6 +2235,8 @@
       <c r="U34" t="inlineStr"/>
       <c r="V34" s="3" t="inlineStr"/>
       <c r="W34" t="inlineStr"/>
+      <c r="X34" s="3" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2231,9 +2311,15 @@
       <c r="V35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="W35" t="n">
+        <v>2529</v>
+      </c>
+      <c r="X35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>2559</t>
         </is>
       </c>
     </row>
@@ -2289,6 +2375,8 @@
       <c r="U36" t="inlineStr"/>
       <c r="V36" s="3" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
+      <c r="X36" s="3" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2326,6 +2414,8 @@
       <c r="U37" t="inlineStr"/>
       <c r="V37" s="3" t="inlineStr"/>
       <c r="W37" t="inlineStr"/>
+      <c r="X37" s="3" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2363,6 +2453,8 @@
       <c r="U38" t="inlineStr"/>
       <c r="V38" s="3" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
+      <c r="X38" s="3" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2437,9 +2529,15 @@
       <c r="V39" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>4922</t>
+      <c r="W39" t="n">
+        <v>4922</v>
+      </c>
+      <c r="X39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>5303</t>
         </is>
       </c>
     </row>
@@ -2516,9 +2614,15 @@
       <c r="V40" s="5" t="n">
         <v>19</v>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>4897</t>
+      <c r="W40" t="n">
+        <v>4897</v>
+      </c>
+      <c r="X40" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>5101</t>
         </is>
       </c>
     </row>
@@ -2558,6 +2662,8 @@
       <c r="U41" t="inlineStr"/>
       <c r="V41" s="3" t="inlineStr"/>
       <c r="W41" t="inlineStr"/>
+      <c r="X41" s="3" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2632,9 +2738,15 @@
       <c r="V42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>4867</t>
+      <c r="W42" t="n">
+        <v>4867</v>
+      </c>
+      <c r="X42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>5059</t>
         </is>
       </c>
     </row>
@@ -2674,6 +2786,8 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" s="3" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
+      <c r="X43" s="3" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2748,9 +2862,15 @@
       <c r="V44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>4372</t>
+      <c r="W44" t="n">
+        <v>4372</v>
+      </c>
+      <c r="X44" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>4577</t>
         </is>
       </c>
     </row>
@@ -2827,9 +2947,15 @@
       <c r="V45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>4677</t>
+      <c r="W45" t="n">
+        <v>4677</v>
+      </c>
+      <c r="X45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>4686</t>
         </is>
       </c>
     </row>
@@ -2906,9 +3032,15 @@
       <c r="V46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>3402</t>
+      <c r="W46" t="n">
+        <v>3402</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>3736</t>
         </is>
       </c>
     </row>
@@ -2985,7 +3117,13 @@
       <c r="V47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W47" t="inlineStr">
+      <c r="W47" t="n">
+        <v>3349</v>
+      </c>
+      <c r="X47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="inlineStr">
         <is>
           <t>3349</t>
         </is>
@@ -3064,9 +3202,15 @@
       <c r="V48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>2531</t>
+      <c r="W48" t="n">
+        <v>2531</v>
+      </c>
+      <c r="X48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -3143,7 +3287,13 @@
       <c r="V49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W49" t="inlineStr">
+      <c r="W49" t="n">
+        <v>0</v>
+      </c>
+      <c r="X49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3197,6 +3347,8 @@
       <c r="U50" t="inlineStr"/>
       <c r="V50" s="3" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
+      <c r="X50" s="3" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3234,6 +3386,8 @@
       <c r="U51" t="inlineStr"/>
       <c r="V51" s="3" t="inlineStr"/>
       <c r="W51" t="inlineStr"/>
+      <c r="X51" s="3" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3308,9 +3462,15 @@
       <c r="V52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>5179</t>
+      <c r="W52" t="n">
+        <v>5179</v>
+      </c>
+      <c r="X52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>5373</t>
         </is>
       </c>
     </row>
@@ -3387,9 +3547,15 @@
       <c r="V53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>4825</t>
+      <c r="W53" t="n">
+        <v>4825</v>
+      </c>
+      <c r="X53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -3429,6 +3595,8 @@
       <c r="U54" t="inlineStr"/>
       <c r="V54" s="3" t="inlineStr"/>
       <c r="W54" t="inlineStr"/>
+      <c r="X54" s="3" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3503,9 +3671,15 @@
       <c r="V55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>5301</t>
+      <c r="W55" t="n">
+        <v>5301</v>
+      </c>
+      <c r="X55" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>5391</t>
         </is>
       </c>
     </row>
@@ -3582,9 +3756,15 @@
       <c r="V56" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>5382</t>
+      <c r="W56" t="n">
+        <v>5382</v>
+      </c>
+      <c r="X56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>5642</t>
         </is>
       </c>
     </row>
@@ -3661,9 +3841,15 @@
       <c r="V57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>5194</t>
+      <c r="W57" t="n">
+        <v>5194</v>
+      </c>
+      <c r="X57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>5414</t>
         </is>
       </c>
     </row>
@@ -3740,9 +3926,15 @@
       <c r="V58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="W58" t="n">
+        <v>5004</v>
+      </c>
+      <c r="X58" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>5202</t>
         </is>
       </c>
     </row>
@@ -3819,9 +4011,15 @@
       <c r="V59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>4917</t>
+      <c r="W59" t="n">
+        <v>4917</v>
+      </c>
+      <c r="X59" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>5059</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4096,15 @@
       <c r="V60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>4930</t>
+      <c r="W60" t="n">
+        <v>4930</v>
+      </c>
+      <c r="X60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>5052</t>
         </is>
       </c>
     </row>
@@ -3977,9 +4181,15 @@
       <c r="V61" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>4574</t>
+      <c r="W61" t="n">
+        <v>4574</v>
+      </c>
+      <c r="X61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>4818</t>
         </is>
       </c>
     </row>
@@ -4056,9 +4266,15 @@
       <c r="V62" s="4" t="n">
         <v>35</v>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>5810</t>
+      <c r="W62" t="n">
+        <v>5810</v>
+      </c>
+      <c r="X62" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>5851</t>
         </is>
       </c>
     </row>
@@ -4135,9 +4351,15 @@
       <c r="V63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>5566</t>
+      <c r="W63" t="n">
+        <v>5566</v>
+      </c>
+      <c r="X63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>5743</t>
         </is>
       </c>
     </row>
@@ -4214,9 +4436,15 @@
       <c r="V64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>5505</t>
+      <c r="W64" t="n">
+        <v>5505</v>
+      </c>
+      <c r="X64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>5728</t>
         </is>
       </c>
     </row>
@@ -4256,6 +4484,8 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" s="3" t="inlineStr"/>
       <c r="W65" t="inlineStr"/>
+      <c r="X65" s="3" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4330,9 +4560,15 @@
       <c r="V66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>5076</t>
+      <c r="W66" t="n">
+        <v>5076</v>
+      </c>
+      <c r="X66" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>5242</t>
         </is>
       </c>
     </row>
@@ -4409,9 +4645,15 @@
       <c r="V67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>4901</t>
+      <c r="W67" t="n">
+        <v>4901</v>
+      </c>
+      <c r="X67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>5034</t>
         </is>
       </c>
     </row>
@@ -4488,9 +4730,15 @@
       <c r="V68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>5000</t>
+      <c r="W68" t="n">
+        <v>5000</v>
+      </c>
+      <c r="X68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>5130</t>
         </is>
       </c>
     </row>
@@ -4567,9 +4815,15 @@
       <c r="V69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="W69" t="n">
+        <v>4731</v>
+      </c>
+      <c r="X69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>4820</t>
         </is>
       </c>
     </row>
@@ -4646,9 +4900,15 @@
       <c r="V70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>4765</t>
+      <c r="W70" t="n">
+        <v>4765</v>
+      </c>
+      <c r="X70" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>4926</t>
         </is>
       </c>
     </row>
@@ -4725,9 +4985,15 @@
       <c r="V71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>5355</t>
+      <c r="W71" t="n">
+        <v>5355</v>
+      </c>
+      <c r="X71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>5484</t>
         </is>
       </c>
     </row>
@@ -4804,9 +5070,15 @@
       <c r="V72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W72" t="inlineStr">
-        <is>
-          <t>4749</t>
+      <c r="W72" t="n">
+        <v>4749</v>
+      </c>
+      <c r="X72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y72" t="inlineStr">
+        <is>
+          <t>4854</t>
         </is>
       </c>
     </row>
@@ -4883,9 +5155,15 @@
       <c r="V73" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>3291</t>
+      <c r="W73" t="n">
+        <v>3291</v>
+      </c>
+      <c r="X73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>3322</t>
         </is>
       </c>
     </row>
@@ -4962,9 +5240,15 @@
       <c r="V74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W74" t="inlineStr">
-        <is>
-          <t>4478</t>
+      <c r="W74" t="n">
+        <v>4478</v>
+      </c>
+      <c r="X74" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>4644</t>
         </is>
       </c>
     </row>
@@ -5041,9 +5325,15 @@
       <c r="V75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W75" t="inlineStr">
-        <is>
-          <t>3232</t>
+      <c r="W75" t="n">
+        <v>3232</v>
+      </c>
+      <c r="X75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>3228</t>
         </is>
       </c>
     </row>
@@ -5120,11 +5410,11 @@
       <c r="V76" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>3554</t>
-        </is>
-      </c>
+      <c r="W76" t="n">
+        <v>3554</v>
+      </c>
+      <c r="X76" s="3" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5199,9 +5489,15 @@
       <c r="V77" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>4550</t>
+      <c r="W77" t="n">
+        <v>4550</v>
+      </c>
+      <c r="X77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>4651</t>
         </is>
       </c>
     </row>
@@ -5278,9 +5574,15 @@
       <c r="V78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>4264</t>
+      <c r="W78" t="n">
+        <v>4264</v>
+      </c>
+      <c r="X78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>4380</t>
         </is>
       </c>
     </row>
@@ -5357,9 +5659,15 @@
       <c r="V79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W79" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="W79" t="n">
+        <v>3996</v>
+      </c>
+      <c r="X79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y79" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -5436,9 +5744,15 @@
       <c r="V80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>4045</t>
+      <c r="W80" t="n">
+        <v>4045</v>
+      </c>
+      <c r="X80" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y80" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -5515,9 +5829,15 @@
       <c r="V81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>4019</t>
+      <c r="W81" t="n">
+        <v>4019</v>
+      </c>
+      <c r="X81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y81" t="inlineStr">
+        <is>
+          <t>4062</t>
         </is>
       </c>
     </row>
@@ -5594,9 +5914,15 @@
       <c r="V82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W82" t="inlineStr">
-        <is>
-          <t>4059</t>
+      <c r="W82" t="n">
+        <v>4059</v>
+      </c>
+      <c r="X82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y82" t="inlineStr">
+        <is>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -5673,9 +5999,15 @@
       <c r="V83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W83" t="inlineStr">
-        <is>
-          <t>2627</t>
+      <c r="W83" t="n">
+        <v>2627</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -5731,6 +6063,8 @@
       <c r="U84" t="inlineStr"/>
       <c r="V84" s="3" t="inlineStr"/>
       <c r="W84" t="inlineStr"/>
+      <c r="X84" s="3" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5776,6 +6110,8 @@
       <c r="U85" t="inlineStr"/>
       <c r="V85" s="3" t="inlineStr"/>
       <c r="W85" t="inlineStr"/>
+      <c r="X85" s="3" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5829,6 +6165,8 @@
       <c r="U86" t="inlineStr"/>
       <c r="V86" s="3" t="inlineStr"/>
       <c r="W86" t="inlineStr"/>
+      <c r="X86" s="3" t="inlineStr"/>
+      <c r="Y86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5903,7 +6241,13 @@
       <c r="V87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W87" t="inlineStr">
+      <c r="W87" t="n">
+        <v>4189</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="inlineStr">
         <is>
           <t>4189</t>
         </is>
@@ -5953,6 +6297,8 @@
       <c r="U88" t="inlineStr"/>
       <c r="V88" s="3" t="inlineStr"/>
       <c r="W88" t="inlineStr"/>
+      <c r="X88" s="3" t="inlineStr"/>
+      <c r="Y88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -5990,6 +6336,8 @@
       <c r="U89" t="inlineStr"/>
       <c r="V89" s="3" t="inlineStr"/>
       <c r="W89" t="inlineStr"/>
+      <c r="X89" s="3" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6064,9 +6412,15 @@
       <c r="V90" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="W90" t="inlineStr">
-        <is>
-          <t>5103</t>
+      <c r="W90" t="n">
+        <v>5103</v>
+      </c>
+      <c r="X90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y90" t="inlineStr">
+        <is>
+          <t>5244</t>
         </is>
       </c>
     </row>
@@ -6143,7 +6497,13 @@
       <c r="V91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W91" t="inlineStr">
+      <c r="W91" t="n">
+        <v>0</v>
+      </c>
+      <c r="X91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6222,9 +6582,15 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="W92" t="n">
+        <v>2720</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -6301,7 +6667,13 @@
       <c r="V93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W93" t="inlineStr">
+      <c r="W93" t="n">
+        <v>2516</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -6380,9 +6752,15 @@
       <c r="V94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W94" t="inlineStr">
-        <is>
-          <t>4687</t>
+      <c r="W94" t="n">
+        <v>4687</v>
+      </c>
+      <c r="X94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y94" t="inlineStr">
+        <is>
+          <t>4762</t>
         </is>
       </c>
     </row>
@@ -6459,9 +6837,15 @@
       <c r="V95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W95" t="inlineStr">
-        <is>
-          <t>4523</t>
+      <c r="W95" t="n">
+        <v>4523</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="inlineStr">
+        <is>
+          <t>4521</t>
         </is>
       </c>
     </row>
@@ -6538,9 +6922,15 @@
       <c r="V96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>2922</t>
+      <c r="W96" t="n">
+        <v>2922</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="inlineStr">
+        <is>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -6617,9 +7007,15 @@
       <c r="V97" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W97" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="W97" t="n">
+        <v>4383</v>
+      </c>
+      <c r="X97" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y97" t="inlineStr">
+        <is>
+          <t>4696</t>
         </is>
       </c>
     </row>
@@ -6696,9 +7092,15 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
-        <is>
-          <t>3198</t>
+      <c r="W98" t="n">
+        <v>3198</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>
@@ -6775,9 +7177,15 @@
       <c r="V99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W99" t="inlineStr">
-        <is>
-          <t>3976</t>
+      <c r="W99" t="n">
+        <v>3976</v>
+      </c>
+      <c r="X99" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y99" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -6854,9 +7262,15 @@
       <c r="V100" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W100" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="W100" t="n">
+        <v>4321</v>
+      </c>
+      <c r="X100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="inlineStr">
+        <is>
+          <t>4291</t>
         </is>
       </c>
     </row>
@@ -6933,9 +7347,15 @@
       <c r="V101" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W101" t="inlineStr">
-        <is>
-          <t>4618</t>
+      <c r="W101" t="n">
+        <v>4618</v>
+      </c>
+      <c r="X101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y101" t="inlineStr">
+        <is>
+          <t>4786</t>
         </is>
       </c>
     </row>
@@ -7012,9 +7432,15 @@
       <c r="V102" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="W102" t="inlineStr">
-        <is>
-          <t>4353</t>
+      <c r="W102" t="n">
+        <v>4353</v>
+      </c>
+      <c r="X102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y102" t="inlineStr">
+        <is>
+          <t>4471</t>
         </is>
       </c>
     </row>
@@ -7091,9 +7517,15 @@
       <c r="V103" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W103" t="inlineStr">
-        <is>
-          <t>4253</t>
+      <c r="W103" t="n">
+        <v>4253</v>
+      </c>
+      <c r="X103" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y103" t="inlineStr">
+        <is>
+          <t>4311</t>
         </is>
       </c>
     </row>
@@ -7170,9 +7602,15 @@
       <c r="V104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W104" t="inlineStr">
-        <is>
-          <t>4174</t>
+      <c r="W104" t="n">
+        <v>4174</v>
+      </c>
+      <c r="X104" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y104" t="inlineStr">
+        <is>
+          <t>4306</t>
         </is>
       </c>
     </row>
@@ -7249,7 +7687,13 @@
       <c r="V105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W105" t="inlineStr">
+      <c r="W105" t="n">
+        <v>0</v>
+      </c>
+      <c r="X105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7328,9 +7772,15 @@
       <c r="V106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W106" t="inlineStr">
-        <is>
-          <t>4251</t>
+      <c r="W106" t="n">
+        <v>4251</v>
+      </c>
+      <c r="X106" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y106" t="inlineStr">
+        <is>
+          <t>4359</t>
         </is>
       </c>
     </row>
@@ -7407,9 +7857,15 @@
       <c r="V107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W107" t="inlineStr">
-        <is>
-          <t>4252</t>
+      <c r="W107" t="n">
+        <v>4252</v>
+      </c>
+      <c r="X107" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y107" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -7486,9 +7942,15 @@
       <c r="V108" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="W108" t="inlineStr">
-        <is>
-          <t>4183</t>
+      <c r="W108" t="n">
+        <v>4183</v>
+      </c>
+      <c r="X108" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y108" t="inlineStr">
+        <is>
+          <t>4369</t>
         </is>
       </c>
     </row>
@@ -7565,7 +8027,13 @@
       <c r="V109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W109" t="inlineStr">
+      <c r="W109" t="n">
+        <v>3032</v>
+      </c>
+      <c r="X109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y109" t="inlineStr">
         <is>
           <t>3032</t>
         </is>
@@ -7644,9 +8112,15 @@
       <c r="V110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W110" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="W110" t="n">
+        <v>4135</v>
+      </c>
+      <c r="X110" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y110" t="inlineStr">
+        <is>
+          <t>4179</t>
         </is>
       </c>
     </row>
@@ -7686,6 +8160,8 @@
       <c r="U111" t="inlineStr"/>
       <c r="V111" s="3" t="inlineStr"/>
       <c r="W111" t="inlineStr"/>
+      <c r="X111" s="3" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7760,9 +8236,15 @@
       <c r="V112" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W112" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="W112" t="n">
+        <v>4106</v>
+      </c>
+      <c r="X112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y112" t="inlineStr">
+        <is>
+          <t>4025</t>
         </is>
       </c>
     </row>
@@ -7839,9 +8321,15 @@
       <c r="V113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>3423</t>
+      <c r="W113" t="n">
+        <v>3423</v>
+      </c>
+      <c r="X113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -7918,7 +8406,13 @@
       <c r="V114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W114" t="inlineStr">
+      <c r="W114" t="n">
+        <v>0</v>
+      </c>
+      <c r="X114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7997,11 +8491,11 @@
       <c r="V115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>3287</t>
-        </is>
-      </c>
+      <c r="W115" t="n">
+        <v>3287</v>
+      </c>
+      <c r="X115" s="3" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -8076,9 +8570,15 @@
       <c r="V116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>3149</t>
+      <c r="W116" t="n">
+        <v>3149</v>
+      </c>
+      <c r="X116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y116" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -8126,6 +8626,8 @@
       <c r="U117" t="inlineStr"/>
       <c r="V117" s="3" t="inlineStr"/>
       <c r="W117" t="inlineStr"/>
+      <c r="X117" s="3" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8163,6 +8665,8 @@
       <c r="U118" t="inlineStr"/>
       <c r="V118" s="3" t="inlineStr"/>
       <c r="W118" t="inlineStr"/>
+      <c r="X118" s="3" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -8237,9 +8741,15 @@
       <c r="V119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>2757</t>
+      <c r="W119" t="n">
+        <v>2757</v>
+      </c>
+      <c r="X119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y119" t="inlineStr">
+        <is>
+          <t>2750</t>
         </is>
       </c>
     </row>
@@ -8315,6 +8825,8 @@
       </c>
       <c r="V120" s="3" t="inlineStr"/>
       <c r="W120" t="inlineStr"/>
+      <c r="X120" s="3" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -8389,9 +8901,15 @@
       <c r="V121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W121" t="inlineStr">
-        <is>
-          <t>2808</t>
+      <c r="W121" t="n">
+        <v>2808</v>
+      </c>
+      <c r="X121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y121" t="inlineStr">
+        <is>
+          <t>2861</t>
         </is>
       </c>
     </row>
@@ -8468,9 +8986,15 @@
       <c r="V122" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="W122" t="inlineStr">
-        <is>
-          <t>3017</t>
+      <c r="W122" t="n">
+        <v>3017</v>
+      </c>
+      <c r="X122" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y122" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -8530,6 +9054,8 @@
       <c r="U123" t="inlineStr"/>
       <c r="V123" s="3" t="inlineStr"/>
       <c r="W123" t="inlineStr"/>
+      <c r="X123" s="3" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -8604,9 +9130,15 @@
       <c r="V124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>2454</t>
+      <c r="W124" t="n">
+        <v>2454</v>
+      </c>
+      <c r="X124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y124" t="inlineStr">
+        <is>
+          <t>2451</t>
         </is>
       </c>
     </row>
@@ -8683,7 +9215,13 @@
       <c r="V125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W125" t="inlineStr">
+      <c r="W125" t="n">
+        <v>0</v>
+      </c>
+      <c r="X125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8762,9 +9300,15 @@
       <c r="V126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>1470</t>
+      <c r="W126" t="n">
+        <v>1470</v>
+      </c>
+      <c r="X126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y126" t="inlineStr">
+        <is>
+          <t>1469</t>
         </is>
       </c>
     </row>
@@ -8841,9 +9385,15 @@
       <c r="V127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>1601</t>
+      <c r="W127" t="n">
+        <v>1601</v>
+      </c>
+      <c r="X127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y127" t="inlineStr">
+        <is>
+          <t>1600</t>
         </is>
       </c>
     </row>
@@ -8920,9 +9470,15 @@
       <c r="V128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W128" t="inlineStr">
-        <is>
-          <t>1205</t>
+      <c r="W128" t="n">
+        <v>1205</v>
+      </c>
+      <c r="X128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y128" t="inlineStr">
+        <is>
+          <t>1202</t>
         </is>
       </c>
     </row>
@@ -8999,7 +9555,13 @@
       <c r="V129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W129" t="inlineStr">
+      <c r="W129" t="n">
+        <v>0</v>
+      </c>
+      <c r="X129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9078,7 +9640,13 @@
       <c r="V130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W130" t="inlineStr">
+      <c r="W130" t="n">
+        <v>0</v>
+      </c>
+      <c r="X130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9157,7 +9725,13 @@
       <c r="V131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W131" t="inlineStr">
+      <c r="W131" t="n">
+        <v>0</v>
+      </c>
+      <c r="X131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9236,7 +9810,13 @@
       <c r="V132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W132" t="inlineStr">
+      <c r="W132" t="n">
+        <v>0</v>
+      </c>
+      <c r="X132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9315,7 +9895,13 @@
       <c r="V133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W133" t="inlineStr">
+      <c r="W133" t="n">
+        <v>0</v>
+      </c>
+      <c r="X133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9394,7 +9980,13 @@
       <c r="V134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W134" t="inlineStr">
+      <c r="W134" t="n">
+        <v>0</v>
+      </c>
+      <c r="X134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9473,9 +10065,15 @@
       <c r="V135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W135" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="W135" t="n">
+        <v>2952</v>
+      </c>
+      <c r="X135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y135" t="inlineStr">
+        <is>
+          <t>3010</t>
         </is>
       </c>
     </row>
@@ -9552,9 +10150,15 @@
       <c r="V136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W136" t="inlineStr">
-        <is>
-          <t>3778</t>
+      <c r="W136" t="n">
+        <v>3778</v>
+      </c>
+      <c r="X136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y136" t="inlineStr">
+        <is>
+          <t>3772</t>
         </is>
       </c>
     </row>
@@ -9631,7 +10235,13 @@
       <c r="V137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W137" t="inlineStr">
+      <c r="W137" t="n">
+        <v>0</v>
+      </c>
+      <c r="X137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9710,9 +10320,15 @@
       <c r="V138" s="5" t="n">
         <v>11</v>
       </c>
-      <c r="W138" t="inlineStr">
-        <is>
-          <t>2909</t>
+      <c r="W138" t="n">
+        <v>2909</v>
+      </c>
+      <c r="X138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y138" t="inlineStr">
+        <is>
+          <t>2903</t>
         </is>
       </c>
     </row>
@@ -9789,7 +10405,13 @@
       <c r="V139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W139" t="inlineStr">
+      <c r="W139" t="n">
+        <v>0</v>
+      </c>
+      <c r="X139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9868,7 +10490,13 @@
       <c r="V140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W140" t="inlineStr">
+      <c r="W140" t="n">
+        <v>0</v>
+      </c>
+      <c r="X140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9947,7 +10575,13 @@
       <c r="V141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W141" t="inlineStr">
+      <c r="W141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y141" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -10026,9 +10660,15 @@
       <c r="V142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W142" t="inlineStr">
-        <is>
-          <t>1751</t>
+      <c r="W142" t="n">
+        <v>1751</v>
+      </c>
+      <c r="X142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y142" t="inlineStr">
+        <is>
+          <t>1750</t>
         </is>
       </c>
     </row>
@@ -10105,9 +10745,15 @@
       <c r="V143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W143" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="W143" t="n">
+        <v>0</v>
+      </c>
+      <c r="X143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y143" t="inlineStr">
+        <is>
+          <t>1398</t>
         </is>
       </c>
     </row>
@@ -10184,7 +10830,13 @@
       <c r="V144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W144" t="inlineStr">
+      <c r="W144" t="n">
+        <v>0</v>
+      </c>
+      <c r="X144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10263,7 +10915,13 @@
       <c r="V145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W145" t="inlineStr">
+      <c r="W145" t="n">
+        <v>0</v>
+      </c>
+      <c r="X145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10342,7 +11000,13 @@
       <c r="V146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W146" t="inlineStr">
+      <c r="W146" t="n">
+        <v>0</v>
+      </c>
+      <c r="X146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10421,7 +11085,13 @@
       <c r="V147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W147" t="inlineStr">
+      <c r="W147" t="n">
+        <v>0</v>
+      </c>
+      <c r="X147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10500,7 +11170,13 @@
       <c r="V148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W148" t="inlineStr">
+      <c r="W148" t="n">
+        <v>0</v>
+      </c>
+      <c r="X148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10579,7 +11255,13 @@
       <c r="V149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W149" t="inlineStr">
+      <c r="W149" t="n">
+        <v>0</v>
+      </c>
+      <c r="X149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10658,7 +11340,13 @@
       <c r="V150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W150" t="inlineStr">
+      <c r="W150" t="n">
+        <v>0</v>
+      </c>
+      <c r="X150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10737,9 +11425,15 @@
       <c r="V151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W151" t="inlineStr">
-        <is>
-          <t>2925</t>
+      <c r="W151" t="n">
+        <v>2925</v>
+      </c>
+      <c r="X151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y151" t="inlineStr">
+        <is>
+          <t>3105</t>
         </is>
       </c>
     </row>
@@ -10816,7 +11510,13 @@
       <c r="V152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W152" t="inlineStr">
+      <c r="W152" t="n">
+        <v>0</v>
+      </c>
+      <c r="X152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10895,7 +11595,13 @@
       <c r="V153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W153" t="inlineStr">
+      <c r="W153" t="n">
+        <v>0</v>
+      </c>
+      <c r="X153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10974,7 +11680,13 @@
       <c r="V154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W154" t="inlineStr">
+      <c r="W154" t="n">
+        <v>0</v>
+      </c>
+      <c r="X154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11053,7 +11765,13 @@
       <c r="V155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W155" t="inlineStr">
+      <c r="W155" t="n">
+        <v>0</v>
+      </c>
+      <c r="X155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11132,7 +11850,13 @@
       <c r="V156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W156" t="inlineStr">
+      <c r="W156" t="n">
+        <v>0</v>
+      </c>
+      <c r="X156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11211,7 +11935,13 @@
       <c r="V157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W157" t="inlineStr">
+      <c r="W157" t="n">
+        <v>0</v>
+      </c>
+      <c r="X157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11290,7 +12020,13 @@
       <c r="V158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W158" t="inlineStr">
+      <c r="W158" t="n">
+        <v>0</v>
+      </c>
+      <c r="X158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11363,9 +12099,15 @@
       <c r="V159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W159" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="W159" t="n">
+        <v>2717</v>
+      </c>
+      <c r="X159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y159" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -11436,9 +12178,15 @@
       <c r="V160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W160" t="inlineStr">
-        <is>
-          <t>1759</t>
+      <c r="W160" t="n">
+        <v>1759</v>
+      </c>
+      <c r="X160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y160" t="inlineStr">
+        <is>
+          <t>1758</t>
         </is>
       </c>
     </row>
@@ -11509,9 +12257,15 @@
       <c r="V161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W161" t="inlineStr">
-        <is>
-          <t>1599</t>
+      <c r="W161" t="n">
+        <v>1599</v>
+      </c>
+      <c r="X161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y161" t="inlineStr">
+        <is>
+          <t>1598</t>
         </is>
       </c>
     </row>
@@ -11578,9 +12332,15 @@
       <c r="V162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W162" t="inlineStr">
-        <is>
-          <t>2306</t>
+      <c r="W162" t="n">
+        <v>2306</v>
+      </c>
+      <c r="X162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y162" t="inlineStr">
+        <is>
+          <t>2305</t>
         </is>
       </c>
     </row>
@@ -11643,9 +12403,15 @@
       <c r="V163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W163" t="inlineStr">
-        <is>
-          <t>2826</t>
+      <c r="W163" t="n">
+        <v>2826</v>
+      </c>
+      <c r="X163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y163" t="inlineStr">
+        <is>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -11691,6 +12457,8 @@
       <c r="U164" t="inlineStr"/>
       <c r="V164" s="3" t="inlineStr"/>
       <c r="W164" t="inlineStr"/>
+      <c r="X164" s="3" t="inlineStr"/>
+      <c r="Y164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -11742,6 +12510,8 @@
       </c>
       <c r="V165" s="3" t="inlineStr"/>
       <c r="W165" t="inlineStr"/>
+      <c r="X165" s="3" t="inlineStr"/>
+      <c r="Y165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -11790,11 +12560,11 @@
       <c r="V166" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W166" t="inlineStr">
-        <is>
-          <t>3231</t>
-        </is>
-      </c>
+      <c r="W166" t="n">
+        <v>3231</v>
+      </c>
+      <c r="X166" s="3" t="inlineStr"/>
+      <c r="Y166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -11834,12 +12604,12 @@
       </c>
       <c r="V167" s="3" t="inlineStr"/>
       <c r="W167" t="inlineStr"/>
+      <c r="X167" s="3" t="inlineStr"/>
+      <c r="Y167" t="inlineStr"/>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>59112086</t>
-        </is>
+      <c r="A168" t="n">
+        <v>59112086</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -11872,9 +12642,60 @@
       <c r="V168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W168" t="inlineStr">
-        <is>
-          <t>1213</t>
+      <c r="W168" t="n">
+        <v>1213</v>
+      </c>
+      <c r="X168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y168" t="inlineStr">
+        <is>
+          <t>1229</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>24787683</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>陳畯泓</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr"/>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="F169" s="3" t="inlineStr"/>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" s="3" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" s="3" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
+      <c r="L169" s="3" t="inlineStr"/>
+      <c r="M169" t="inlineStr"/>
+      <c r="N169" s="3" t="inlineStr"/>
+      <c r="O169" t="inlineStr"/>
+      <c r="P169" s="3" t="inlineStr"/>
+      <c r="Q169" t="inlineStr"/>
+      <c r="R169" s="3" t="inlineStr"/>
+      <c r="S169" t="inlineStr"/>
+      <c r="T169" s="3" t="inlineStr"/>
+      <c r="U169" t="inlineStr"/>
+      <c r="V169" s="3" t="inlineStr"/>
+      <c r="W169" t="inlineStr"/>
+      <c r="X169" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y169" t="inlineStr">
+        <is>
+          <t>4096</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-07 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y169"/>
+  <dimension ref="A1:AA170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,16 @@
           <t>04-05_0</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>04-06_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>04-06_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -591,6 +601,8 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" s="3" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
+      <c r="Z2" s="3" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -630,6 +642,8 @@
       <c r="W3" t="inlineStr"/>
       <c r="X3" s="3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
+      <c r="Z3" s="3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -669,6 +683,8 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" s="3" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
+      <c r="Z4" s="3" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -728,6 +744,8 @@
       <c r="W5" t="inlineStr"/>
       <c r="X5" s="3" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
+      <c r="Z5" s="3" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -767,6 +785,8 @@
       <c r="W6" t="inlineStr"/>
       <c r="X6" s="3" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
+      <c r="Z6" s="3" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -806,6 +826,8 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" s="3" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
+      <c r="Z7" s="3" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -869,6 +891,8 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" s="3" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
+      <c r="Z8" s="3" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -908,6 +932,8 @@
       <c r="W9" t="inlineStr"/>
       <c r="X9" s="3" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
+      <c r="Z9" s="3" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -983,6 +1009,8 @@
       <c r="W10" t="inlineStr"/>
       <c r="X10" s="3" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
+      <c r="Z10" s="3" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1034,6 +1062,8 @@
       <c r="W11" t="inlineStr"/>
       <c r="X11" s="3" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
+      <c r="Z11" s="3" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1109,6 +1139,8 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" s="3" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
+      <c r="Z12" s="3" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1129,7 +1161,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F13" s="3" t="n">
@@ -1189,9 +1221,15 @@
       <c r="X13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>5663</t>
+      <c r="Y13" t="n">
+        <v>5663</v>
+      </c>
+      <c r="Z13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>5808</t>
         </is>
       </c>
     </row>
@@ -1269,6 +1307,8 @@
       <c r="W14" t="inlineStr"/>
       <c r="X14" s="3" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
+      <c r="Z14" s="3" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1344,6 +1384,8 @@
       <c r="W15" t="inlineStr"/>
       <c r="X15" s="3" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
+      <c r="Z15" s="3" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1395,6 +1437,8 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" s="3" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
+      <c r="Z16" s="3" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1458,6 +1502,8 @@
       <c r="W17" t="inlineStr"/>
       <c r="X17" s="3" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
+      <c r="Z17" s="3" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1517,6 +1563,8 @@
       <c r="W18" t="inlineStr"/>
       <c r="X18" s="3" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
+      <c r="Z18" s="3" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1568,6 +1616,8 @@
       <c r="W19" t="inlineStr"/>
       <c r="X19" s="3" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
+      <c r="Z19" s="3" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1607,6 +1657,8 @@
       <c r="W20" t="inlineStr"/>
       <c r="X20" s="3" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
+      <c r="Z20" s="3" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1674,6 +1726,8 @@
       <c r="W21" t="inlineStr"/>
       <c r="X21" s="3" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
+      <c r="Z21" s="3" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1713,6 +1767,8 @@
       <c r="W22" t="inlineStr"/>
       <c r="X22" s="3" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
+      <c r="Z22" s="3" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1772,6 +1828,8 @@
       <c r="W23" t="inlineStr"/>
       <c r="X23" s="3" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
+      <c r="Z23" s="3" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1847,6 +1905,8 @@
       <c r="W24" t="inlineStr"/>
       <c r="X24" s="3" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
+      <c r="Z24" s="3" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1886,6 +1946,8 @@
       <c r="W25" t="inlineStr"/>
       <c r="X25" s="3" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
+      <c r="Z25" s="3" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1925,6 +1987,8 @@
       <c r="W26" t="inlineStr"/>
       <c r="X26" s="3" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
+      <c r="Z26" s="3" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1964,6 +2028,8 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" s="3" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
+      <c r="Z27" s="3" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2003,6 +2069,8 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" s="3" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
+      <c r="Z28" s="3" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2042,6 +2110,8 @@
       <c r="W29" t="inlineStr"/>
       <c r="X29" s="3" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
+      <c r="Z29" s="3" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2081,6 +2151,8 @@
       <c r="W30" t="inlineStr"/>
       <c r="X30" s="3" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
+      <c r="Z30" s="3" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2120,6 +2192,8 @@
       <c r="W31" t="inlineStr"/>
       <c r="X31" s="3" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
+      <c r="Z31" s="3" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2159,6 +2233,8 @@
       <c r="W32" t="inlineStr"/>
       <c r="X32" s="3" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
+      <c r="Z32" s="3" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2198,6 +2274,8 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" s="3" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
+      <c r="Z33" s="3" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2237,6 +2315,8 @@
       <c r="W34" t="inlineStr"/>
       <c r="X34" s="3" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
+      <c r="Z34" s="3" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2317,7 +2397,13 @@
       <c r="X35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y35" t="inlineStr">
+      <c r="Y35" t="n">
+        <v>2559</v>
+      </c>
+      <c r="Z35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="inlineStr">
         <is>
           <t>2559</t>
         </is>
@@ -2377,6 +2463,8 @@
       <c r="W36" t="inlineStr"/>
       <c r="X36" s="3" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
+      <c r="Z36" s="3" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2416,6 +2504,8 @@
       <c r="W37" t="inlineStr"/>
       <c r="X37" s="3" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
+      <c r="Z37" s="3" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2455,6 +2545,8 @@
       <c r="W38" t="inlineStr"/>
       <c r="X38" s="3" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
+      <c r="Z38" s="3" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2535,9 +2627,15 @@
       <c r="X39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>5303</t>
+      <c r="Y39" t="n">
+        <v>5303</v>
+      </c>
+      <c r="Z39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>5598</t>
         </is>
       </c>
     </row>
@@ -2620,9 +2718,15 @@
       <c r="X40" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>5101</t>
+      <c r="Y40" t="n">
+        <v>5101</v>
+      </c>
+      <c r="Z40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>5189</t>
         </is>
       </c>
     </row>
@@ -2664,6 +2768,8 @@
       <c r="W41" t="inlineStr"/>
       <c r="X41" s="3" t="inlineStr"/>
       <c r="Y41" t="inlineStr"/>
+      <c r="Z41" s="3" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2744,9 +2850,15 @@
       <c r="X42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>5059</t>
+      <c r="Y42" t="n">
+        <v>5059</v>
+      </c>
+      <c r="Z42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>5192</t>
         </is>
       </c>
     </row>
@@ -2788,6 +2900,8 @@
       <c r="W43" t="inlineStr"/>
       <c r="X43" s="3" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
+      <c r="Z43" s="3" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2868,7 +2982,13 @@
       <c r="X44" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="Y44" t="inlineStr">
+      <c r="Y44" t="n">
+        <v>4577</v>
+      </c>
+      <c r="Z44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA44" t="inlineStr">
         <is>
           <t>4577</t>
         </is>
@@ -2953,9 +3073,15 @@
       <c r="X45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>4686</t>
+      <c r="Y45" t="n">
+        <v>4686</v>
+      </c>
+      <c r="Z45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>4729</t>
         </is>
       </c>
     </row>
@@ -3038,7 +3164,13 @@
       <c r="X46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y46" t="inlineStr">
+      <c r="Y46" t="n">
+        <v>3736</v>
+      </c>
+      <c r="Z46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA46" t="inlineStr">
         <is>
           <t>3736</t>
         </is>
@@ -3123,7 +3255,13 @@
       <c r="X47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y47" t="inlineStr">
+      <c r="Y47" t="n">
+        <v>3349</v>
+      </c>
+      <c r="Z47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="inlineStr">
         <is>
           <t>3349</t>
         </is>
@@ -3208,7 +3346,13 @@
       <c r="X48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y48" t="inlineStr">
+      <c r="Y48" t="n">
+        <v>2563</v>
+      </c>
+      <c r="Z48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="inlineStr">
         <is>
           <t>2563</t>
         </is>
@@ -3293,7 +3437,13 @@
       <c r="X49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y49" t="inlineStr">
+      <c r="Y49" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3349,6 +3499,8 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" s="3" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
+      <c r="Z50" s="3" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3388,6 +3540,8 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" s="3" t="inlineStr"/>
       <c r="Y51" t="inlineStr"/>
+      <c r="Z51" s="3" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3468,9 +3622,15 @@
       <c r="X52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>5373</t>
+      <c r="Y52" t="n">
+        <v>5373</v>
+      </c>
+      <c r="Z52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>5513</t>
         </is>
       </c>
     </row>
@@ -3553,9 +3713,15 @@
       <c r="X53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="Y53" t="n">
+        <v>4994</v>
+      </c>
+      <c r="Z53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>5154</t>
         </is>
       </c>
     </row>
@@ -3597,6 +3763,8 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" s="3" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
+      <c r="Z54" s="3" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3677,9 +3845,15 @@
       <c r="X55" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>5391</t>
+      <c r="Y55" t="n">
+        <v>5391</v>
+      </c>
+      <c r="Z55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>5539</t>
         </is>
       </c>
     </row>
@@ -3762,9 +3936,15 @@
       <c r="X56" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>5642</t>
+      <c r="Y56" t="n">
+        <v>5642</v>
+      </c>
+      <c r="Z56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>5754</t>
         </is>
       </c>
     </row>
@@ -3847,9 +4027,15 @@
       <c r="X57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>5414</t>
+      <c r="Y57" t="n">
+        <v>5414</v>
+      </c>
+      <c r="Z57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>5472</t>
         </is>
       </c>
     </row>
@@ -3932,9 +4118,15 @@
       <c r="X58" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>5202</t>
+      <c r="Y58" t="n">
+        <v>5202</v>
+      </c>
+      <c r="Z58" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>5291</t>
         </is>
       </c>
     </row>
@@ -4017,9 +4209,15 @@
       <c r="X59" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>5059</t>
+      <c r="Y59" t="n">
+        <v>5059</v>
+      </c>
+      <c r="Z59" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>5054</t>
         </is>
       </c>
     </row>
@@ -4102,9 +4300,15 @@
       <c r="X60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>5052</t>
+      <c r="Y60" t="n">
+        <v>5052</v>
+      </c>
+      <c r="Z60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>5212</t>
         </is>
       </c>
     </row>
@@ -4187,9 +4391,15 @@
       <c r="X61" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>4818</t>
+      <c r="Y61" t="n">
+        <v>4818</v>
+      </c>
+      <c r="Z61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>4964</t>
         </is>
       </c>
     </row>
@@ -4272,9 +4482,15 @@
       <c r="X62" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>5851</t>
+      <c r="Y62" t="n">
+        <v>5851</v>
+      </c>
+      <c r="Z62" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>6131</t>
         </is>
       </c>
     </row>
@@ -4357,9 +4573,15 @@
       <c r="X63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>5743</t>
+      <c r="Y63" t="n">
+        <v>5743</v>
+      </c>
+      <c r="Z63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>5918</t>
         </is>
       </c>
     </row>
@@ -4442,9 +4664,15 @@
       <c r="X64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>5728</t>
+      <c r="Y64" t="n">
+        <v>5728</v>
+      </c>
+      <c r="Z64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>5941</t>
         </is>
       </c>
     </row>
@@ -4486,6 +4714,8 @@
       <c r="W65" t="inlineStr"/>
       <c r="X65" s="3" t="inlineStr"/>
       <c r="Y65" t="inlineStr"/>
+      <c r="Z65" s="3" t="inlineStr"/>
+      <c r="AA65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4566,9 +4796,15 @@
       <c r="X66" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y66" t="inlineStr">
-        <is>
-          <t>5242</t>
+      <c r="Y66" t="n">
+        <v>5242</v>
+      </c>
+      <c r="Z66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA66" t="inlineStr">
+        <is>
+          <t>5609</t>
         </is>
       </c>
     </row>
@@ -4651,9 +4887,15 @@
       <c r="X67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y67" t="inlineStr">
-        <is>
-          <t>5034</t>
+      <c r="Y67" t="n">
+        <v>5034</v>
+      </c>
+      <c r="Z67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>5279</t>
         </is>
       </c>
     </row>
@@ -4736,9 +4978,15 @@
       <c r="X68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="Y68" t="inlineStr">
-        <is>
-          <t>5130</t>
+      <c r="Y68" t="n">
+        <v>5130</v>
+      </c>
+      <c r="Z68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>5282</t>
         </is>
       </c>
     </row>
@@ -4821,9 +5069,15 @@
       <c r="X69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>4820</t>
+      <c r="Y69" t="n">
+        <v>4820</v>
+      </c>
+      <c r="Z69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -4906,9 +5160,15 @@
       <c r="X70" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y70" t="inlineStr">
-        <is>
-          <t>4926</t>
+      <c r="Y70" t="n">
+        <v>4926</v>
+      </c>
+      <c r="Z70" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>4953</t>
         </is>
       </c>
     </row>
@@ -4991,9 +5251,15 @@
       <c r="X71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y71" t="inlineStr">
-        <is>
-          <t>5484</t>
+      <c r="Y71" t="n">
+        <v>5484</v>
+      </c>
+      <c r="Z71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>5728</t>
         </is>
       </c>
     </row>
@@ -5076,9 +5342,15 @@
       <c r="X72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y72" t="inlineStr">
-        <is>
-          <t>4854</t>
+      <c r="Y72" t="n">
+        <v>4854</v>
+      </c>
+      <c r="Z72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>5075</t>
         </is>
       </c>
     </row>
@@ -5161,9 +5433,15 @@
       <c r="X73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y73" t="inlineStr">
-        <is>
-          <t>3322</t>
+      <c r="Y73" t="n">
+        <v>3322</v>
+      </c>
+      <c r="Z73" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>3958</t>
         </is>
       </c>
     </row>
@@ -5246,9 +5524,15 @@
       <c r="X74" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y74" t="inlineStr">
-        <is>
-          <t>4644</t>
+      <c r="Y74" t="n">
+        <v>4644</v>
+      </c>
+      <c r="Z74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>4584</t>
         </is>
       </c>
     </row>
@@ -5331,9 +5615,15 @@
       <c r="X75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y75" t="inlineStr">
-        <is>
-          <t>3228</t>
+      <c r="Y75" t="n">
+        <v>3228</v>
+      </c>
+      <c r="Z75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>3809</t>
         </is>
       </c>
     </row>
@@ -5415,6 +5705,8 @@
       </c>
       <c r="X76" s="3" t="inlineStr"/>
       <c r="Y76" t="inlineStr"/>
+      <c r="Z76" s="3" t="inlineStr"/>
+      <c r="AA76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5495,9 +5787,15 @@
       <c r="X77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>4651</t>
+      <c r="Y77" t="n">
+        <v>4651</v>
+      </c>
+      <c r="Z77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>4804</t>
         </is>
       </c>
     </row>
@@ -5580,9 +5878,15 @@
       <c r="X78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y78" t="inlineStr">
-        <is>
-          <t>4380</t>
+      <c r="Y78" t="n">
+        <v>4380</v>
+      </c>
+      <c r="Z78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>4405</t>
         </is>
       </c>
     </row>
@@ -5665,9 +5969,15 @@
       <c r="X79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y79" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="Y79" t="n">
+        <v>4106</v>
+      </c>
+      <c r="Z79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA79" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -5750,9 +6060,15 @@
       <c r="X80" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y80" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="Y80" t="n">
+        <v>4098</v>
+      </c>
+      <c r="Z80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -5835,9 +6151,15 @@
       <c r="X81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y81" t="inlineStr">
-        <is>
-          <t>4062</t>
+      <c r="Y81" t="n">
+        <v>4062</v>
+      </c>
+      <c r="Z81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA81" t="inlineStr">
+        <is>
+          <t>4173</t>
         </is>
       </c>
     </row>
@@ -5920,9 +6242,15 @@
       <c r="X82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y82" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="Y82" t="n">
+        <v>4106</v>
+      </c>
+      <c r="Z82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA82" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -6005,7 +6333,13 @@
       <c r="X83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y83" t="inlineStr">
+      <c r="Y83" t="n">
+        <v>2659</v>
+      </c>
+      <c r="Z83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="inlineStr">
         <is>
           <t>2659</t>
         </is>
@@ -6065,6 +6399,8 @@
       <c r="W84" t="inlineStr"/>
       <c r="X84" s="3" t="inlineStr"/>
       <c r="Y84" t="inlineStr"/>
+      <c r="Z84" s="3" t="inlineStr"/>
+      <c r="AA84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -6112,6 +6448,8 @@
       <c r="W85" t="inlineStr"/>
       <c r="X85" s="3" t="inlineStr"/>
       <c r="Y85" t="inlineStr"/>
+      <c r="Z85" s="3" t="inlineStr"/>
+      <c r="AA85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -6167,6 +6505,8 @@
       <c r="W86" t="inlineStr"/>
       <c r="X86" s="3" t="inlineStr"/>
       <c r="Y86" t="inlineStr"/>
+      <c r="Z86" s="3" t="inlineStr"/>
+      <c r="AA86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -6247,7 +6587,13 @@
       <c r="X87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y87" t="inlineStr">
+      <c r="Y87" t="n">
+        <v>4189</v>
+      </c>
+      <c r="Z87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="inlineStr">
         <is>
           <t>4189</t>
         </is>
@@ -6299,6 +6645,8 @@
       <c r="W88" t="inlineStr"/>
       <c r="X88" s="3" t="inlineStr"/>
       <c r="Y88" t="inlineStr"/>
+      <c r="Z88" s="3" t="inlineStr"/>
+      <c r="AA88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6338,6 +6686,8 @@
       <c r="W89" t="inlineStr"/>
       <c r="X89" s="3" t="inlineStr"/>
       <c r="Y89" t="inlineStr"/>
+      <c r="Z89" s="3" t="inlineStr"/>
+      <c r="AA89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6418,9 +6768,15 @@
       <c r="X90" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="Y90" t="inlineStr">
-        <is>
-          <t>5244</t>
+      <c r="Y90" t="n">
+        <v>5244</v>
+      </c>
+      <c r="Z90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA90" t="inlineStr">
+        <is>
+          <t>5399</t>
         </is>
       </c>
     </row>
@@ -6503,7 +6859,13 @@
       <c r="X91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y91" t="inlineStr">
+      <c r="Y91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6588,9 +6950,15 @@
       <c r="X92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y92" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="Y92" t="n">
+        <v>2717</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -6673,9 +7041,15 @@
       <c r="X93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y93" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="Y93" t="n">
+        <v>2516</v>
+      </c>
+      <c r="Z93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA93" t="inlineStr">
+        <is>
+          <t>2540</t>
         </is>
       </c>
     </row>
@@ -6758,9 +7132,15 @@
       <c r="X94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y94" t="inlineStr">
-        <is>
-          <t>4762</t>
+      <c r="Y94" t="n">
+        <v>4762</v>
+      </c>
+      <c r="Z94" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA94" t="inlineStr">
+        <is>
+          <t>4819</t>
         </is>
       </c>
     </row>
@@ -6843,9 +7223,15 @@
       <c r="X95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y95" t="inlineStr">
-        <is>
-          <t>4521</t>
+      <c r="Y95" t="n">
+        <v>4521</v>
+      </c>
+      <c r="Z95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA95" t="inlineStr">
+        <is>
+          <t>4773</t>
         </is>
       </c>
     </row>
@@ -6928,9 +7314,15 @@
       <c r="X96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y96" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="Y96" t="n">
+        <v>2916</v>
+      </c>
+      <c r="Z96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA96" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -7013,9 +7405,15 @@
       <c r="X97" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y97" t="inlineStr">
-        <is>
-          <t>4696</t>
+      <c r="Y97" t="n">
+        <v>4696</v>
+      </c>
+      <c r="Z97" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA97" t="inlineStr">
+        <is>
+          <t>4743</t>
         </is>
       </c>
     </row>
@@ -7098,9 +7496,15 @@
       <c r="X98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y98" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="Y98" t="n">
+        <v>3334</v>
+      </c>
+      <c r="Z98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA98" t="inlineStr">
+        <is>
+          <t>3361</t>
         </is>
       </c>
     </row>
@@ -7183,9 +7587,15 @@
       <c r="X99" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="Y99" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="Y99" t="n">
+        <v>4172</v>
+      </c>
+      <c r="Z99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA99" t="inlineStr">
+        <is>
+          <t>4376</t>
         </is>
       </c>
     </row>
@@ -7268,9 +7678,15 @@
       <c r="X100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y100" t="inlineStr">
-        <is>
-          <t>4291</t>
+      <c r="Y100" t="n">
+        <v>4291</v>
+      </c>
+      <c r="Z100" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA100" t="inlineStr">
+        <is>
+          <t>4497</t>
         </is>
       </c>
     </row>
@@ -7353,9 +7769,15 @@
       <c r="X101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y101" t="inlineStr">
-        <is>
-          <t>4786</t>
+      <c r="Y101" t="n">
+        <v>4786</v>
+      </c>
+      <c r="Z101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA101" t="inlineStr">
+        <is>
+          <t>4957</t>
         </is>
       </c>
     </row>
@@ -7438,9 +7860,15 @@
       <c r="X102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y102" t="inlineStr">
-        <is>
-          <t>4471</t>
+      <c r="Y102" t="n">
+        <v>4471</v>
+      </c>
+      <c r="Z102" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA102" t="inlineStr">
+        <is>
+          <t>4499</t>
         </is>
       </c>
     </row>
@@ -7523,9 +7951,15 @@
       <c r="X103" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="Y103" t="inlineStr">
-        <is>
-          <t>4311</t>
+      <c r="Y103" t="n">
+        <v>4311</v>
+      </c>
+      <c r="Z103" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA103" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -7608,9 +8042,15 @@
       <c r="X104" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Y104" t="inlineStr">
-        <is>
-          <t>4306</t>
+      <c r="Y104" t="n">
+        <v>4306</v>
+      </c>
+      <c r="Z104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA104" t="inlineStr">
+        <is>
+          <t>4332</t>
         </is>
       </c>
     </row>
@@ -7693,7 +8133,13 @@
       <c r="X105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y105" t="inlineStr">
+      <c r="Y105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7778,9 +8224,15 @@
       <c r="X106" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y106" t="inlineStr">
-        <is>
-          <t>4359</t>
+      <c r="Y106" t="n">
+        <v>4359</v>
+      </c>
+      <c r="Z106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA106" t="inlineStr">
+        <is>
+          <t>4410</t>
         </is>
       </c>
     </row>
@@ -7863,9 +8315,15 @@
       <c r="X107" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="Y107" t="inlineStr">
-        <is>
-          <t>4258</t>
+      <c r="Y107" t="n">
+        <v>4258</v>
+      </c>
+      <c r="Z107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA107" t="inlineStr">
+        <is>
+          <t>4316</t>
         </is>
       </c>
     </row>
@@ -7948,9 +8406,15 @@
       <c r="X108" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y108" t="inlineStr">
-        <is>
-          <t>4369</t>
+      <c r="Y108" t="n">
+        <v>4369</v>
+      </c>
+      <c r="Z108" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA108" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -8033,9 +8497,15 @@
       <c r="X109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y109" t="inlineStr">
-        <is>
-          <t>3032</t>
+      <c r="Y109" t="n">
+        <v>3032</v>
+      </c>
+      <c r="Z109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA109" t="inlineStr">
+        <is>
+          <t>3169</t>
         </is>
       </c>
     </row>
@@ -8118,9 +8588,15 @@
       <c r="X110" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y110" t="inlineStr">
-        <is>
-          <t>4179</t>
+      <c r="Y110" t="n">
+        <v>4179</v>
+      </c>
+      <c r="Z110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA110" t="inlineStr">
+        <is>
+          <t>4217</t>
         </is>
       </c>
     </row>
@@ -8162,6 +8638,8 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" s="3" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
+      <c r="Z111" s="3" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8242,9 +8720,15 @@
       <c r="X112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y112" t="inlineStr">
-        <is>
-          <t>4025</t>
+      <c r="Y112" t="n">
+        <v>4025</v>
+      </c>
+      <c r="Z112" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA112" t="inlineStr">
+        <is>
+          <t>4123</t>
         </is>
       </c>
     </row>
@@ -8327,9 +8811,15 @@
       <c r="X113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="Y113" t="n">
+        <v>3496</v>
+      </c>
+      <c r="Z113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA113" t="inlineStr">
+        <is>
+          <t>3590</t>
         </is>
       </c>
     </row>
@@ -8412,7 +8902,13 @@
       <c r="X114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y114" t="inlineStr">
+      <c r="Y114" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8496,6 +8992,14 @@
       </c>
       <c r="X115" s="3" t="inlineStr"/>
       <c r="Y115" t="inlineStr"/>
+      <c r="Z115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>3445</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -8576,9 +9080,15 @@
       <c r="X116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y116" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="Y116" t="n">
+        <v>3147</v>
+      </c>
+      <c r="Z116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA116" t="inlineStr">
+        <is>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -8628,6 +9138,8 @@
       <c r="W117" t="inlineStr"/>
       <c r="X117" s="3" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
+      <c r="Z117" s="3" t="inlineStr"/>
+      <c r="AA117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8667,6 +9179,8 @@
       <c r="W118" t="inlineStr"/>
       <c r="X118" s="3" t="inlineStr"/>
       <c r="Y118" t="inlineStr"/>
+      <c r="Z118" s="3" t="inlineStr"/>
+      <c r="AA118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -8747,9 +9261,15 @@
       <c r="X119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y119" t="inlineStr">
-        <is>
-          <t>2750</t>
+      <c r="Y119" t="n">
+        <v>2750</v>
+      </c>
+      <c r="Z119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA119" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -8827,6 +9347,8 @@
       <c r="W120" t="inlineStr"/>
       <c r="X120" s="3" t="inlineStr"/>
       <c r="Y120" t="inlineStr"/>
+      <c r="Z120" s="3" t="inlineStr"/>
+      <c r="AA120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -8907,9 +9429,15 @@
       <c r="X121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y121" t="inlineStr">
-        <is>
-          <t>2861</t>
+      <c r="Y121" t="n">
+        <v>2861</v>
+      </c>
+      <c r="Z121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA121" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -8992,9 +9520,15 @@
       <c r="X122" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y122" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="Y122" t="n">
+        <v>3241</v>
+      </c>
+      <c r="Z122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA122" t="inlineStr">
+        <is>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -9056,6 +9590,8 @@
       <c r="W123" t="inlineStr"/>
       <c r="X123" s="3" t="inlineStr"/>
       <c r="Y123" t="inlineStr"/>
+      <c r="Z123" s="3" t="inlineStr"/>
+      <c r="AA123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -9136,9 +9672,15 @@
       <c r="X124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y124" t="inlineStr">
-        <is>
-          <t>2451</t>
+      <c r="Y124" t="n">
+        <v>2451</v>
+      </c>
+      <c r="Z124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA124" t="inlineStr">
+        <is>
+          <t>2444</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9763,13 @@
       <c r="X125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y125" t="inlineStr">
+      <c r="Y125" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9306,9 +9854,15 @@
       <c r="X126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y126" t="inlineStr">
-        <is>
-          <t>1469</t>
+      <c r="Y126" t="n">
+        <v>1469</v>
+      </c>
+      <c r="Z126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA126" t="inlineStr">
+        <is>
+          <t>1464</t>
         </is>
       </c>
     </row>
@@ -9391,9 +9945,15 @@
       <c r="X127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y127" t="inlineStr">
-        <is>
-          <t>1600</t>
+      <c r="Y127" t="n">
+        <v>1600</v>
+      </c>
+      <c r="Z127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA127" t="inlineStr">
+        <is>
+          <t>1613</t>
         </is>
       </c>
     </row>
@@ -9476,9 +10036,15 @@
       <c r="X128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y128" t="inlineStr">
-        <is>
-          <t>1202</t>
+      <c r="Y128" t="n">
+        <v>1202</v>
+      </c>
+      <c r="Z128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA128" t="inlineStr">
+        <is>
+          <t>1230</t>
         </is>
       </c>
     </row>
@@ -9561,7 +10127,13 @@
       <c r="X129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y129" t="inlineStr">
+      <c r="Y129" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9646,7 +10218,13 @@
       <c r="X130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y130" t="inlineStr">
+      <c r="Y130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9731,7 +10309,13 @@
       <c r="X131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y131" t="inlineStr">
+      <c r="Y131" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9816,7 +10400,13 @@
       <c r="X132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y132" t="inlineStr">
+      <c r="Y132" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9901,7 +10491,13 @@
       <c r="X133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y133" t="inlineStr">
+      <c r="Y133" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9986,7 +10582,13 @@
       <c r="X134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y134" t="inlineStr">
+      <c r="Y134" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10071,9 +10673,15 @@
       <c r="X135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y135" t="inlineStr">
-        <is>
-          <t>3010</t>
+      <c r="Y135" t="n">
+        <v>3010</v>
+      </c>
+      <c r="Z135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA135" t="inlineStr">
+        <is>
+          <t>3034</t>
         </is>
       </c>
     </row>
@@ -10156,9 +10764,15 @@
       <c r="X136" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y136" t="inlineStr">
-        <is>
-          <t>3772</t>
+      <c r="Y136" t="n">
+        <v>3772</v>
+      </c>
+      <c r="Z136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA136" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -10241,7 +10855,13 @@
       <c r="X137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y137" t="inlineStr">
+      <c r="Y137" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10326,9 +10946,15 @@
       <c r="X138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y138" t="inlineStr">
-        <is>
-          <t>2903</t>
+      <c r="Y138" t="n">
+        <v>2903</v>
+      </c>
+      <c r="Z138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA138" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -10411,7 +11037,13 @@
       <c r="X139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y139" t="inlineStr">
+      <c r="Y139" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10496,7 +11128,13 @@
       <c r="X140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y140" t="inlineStr">
+      <c r="Y140" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10581,9 +11219,15 @@
       <c r="X141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y141" t="inlineStr">
-        <is>
-          <t>2000</t>
+      <c r="Y141" t="n">
+        <v>2000</v>
+      </c>
+      <c r="Z141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA141" t="inlineStr">
+        <is>
+          <t>2022</t>
         </is>
       </c>
     </row>
@@ -10666,9 +11310,15 @@
       <c r="X142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y142" t="inlineStr">
-        <is>
-          <t>1750</t>
+      <c r="Y142" t="n">
+        <v>1750</v>
+      </c>
+      <c r="Z142" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA142" t="inlineStr">
+        <is>
+          <t>1999</t>
         </is>
       </c>
     </row>
@@ -10751,9 +11401,15 @@
       <c r="X143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y143" t="inlineStr">
-        <is>
-          <t>1398</t>
+      <c r="Y143" t="n">
+        <v>1398</v>
+      </c>
+      <c r="Z143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA143" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10836,7 +11492,13 @@
       <c r="X144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y144" t="inlineStr">
+      <c r="Y144" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10921,7 +11583,13 @@
       <c r="X145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y145" t="inlineStr">
+      <c r="Y145" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11006,7 +11674,13 @@
       <c r="X146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y146" t="inlineStr">
+      <c r="Y146" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11091,7 +11765,13 @@
       <c r="X147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y147" t="inlineStr">
+      <c r="Y147" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11176,7 +11856,13 @@
       <c r="X148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y148" t="inlineStr">
+      <c r="Y148" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11261,7 +11947,13 @@
       <c r="X149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y149" t="inlineStr">
+      <c r="Y149" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11346,7 +12038,13 @@
       <c r="X150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y150" t="inlineStr">
+      <c r="Y150" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11431,9 +12129,15 @@
       <c r="X151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y151" t="inlineStr">
-        <is>
-          <t>3105</t>
+      <c r="Y151" t="n">
+        <v>3105</v>
+      </c>
+      <c r="Z151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA151" t="inlineStr">
+        <is>
+          <t>3135</t>
         </is>
       </c>
     </row>
@@ -11516,7 +12220,13 @@
       <c r="X152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y152" t="inlineStr">
+      <c r="Y152" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11601,7 +12311,13 @@
       <c r="X153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y153" t="inlineStr">
+      <c r="Y153" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11686,7 +12402,13 @@
       <c r="X154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y154" t="inlineStr">
+      <c r="Y154" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11771,7 +12493,13 @@
       <c r="X155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y155" t="inlineStr">
+      <c r="Y155" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11856,7 +12584,13 @@
       <c r="X156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y156" t="inlineStr">
+      <c r="Y156" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11941,7 +12675,13 @@
       <c r="X157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y157" t="inlineStr">
+      <c r="Y157" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12026,7 +12766,13 @@
       <c r="X158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y158" t="inlineStr">
+      <c r="Y158" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12105,9 +12851,15 @@
       <c r="X159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y159" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="Y159" t="n">
+        <v>2711</v>
+      </c>
+      <c r="Z159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA159" t="inlineStr">
+        <is>
+          <t>2709</t>
         </is>
       </c>
     </row>
@@ -12184,9 +12936,15 @@
       <c r="X160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y160" t="inlineStr">
-        <is>
-          <t>1758</t>
+      <c r="Y160" t="n">
+        <v>1758</v>
+      </c>
+      <c r="Z160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA160" t="inlineStr">
+        <is>
+          <t>1784</t>
         </is>
       </c>
     </row>
@@ -12263,9 +13021,15 @@
       <c r="X161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y161" t="inlineStr">
-        <is>
-          <t>1598</t>
+      <c r="Y161" t="n">
+        <v>1598</v>
+      </c>
+      <c r="Z161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA161" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12338,9 +13102,15 @@
       <c r="X162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y162" t="inlineStr">
-        <is>
-          <t>2305</t>
+      <c r="Y162" t="n">
+        <v>2305</v>
+      </c>
+      <c r="Z162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA162" t="inlineStr">
+        <is>
+          <t>2315</t>
         </is>
       </c>
     </row>
@@ -12409,9 +13179,15 @@
       <c r="X163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y163" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="Y163" t="n">
+        <v>2821</v>
+      </c>
+      <c r="Z163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA163" t="inlineStr">
+        <is>
+          <t>2817</t>
         </is>
       </c>
     </row>
@@ -12459,6 +13235,8 @@
       <c r="W164" t="inlineStr"/>
       <c r="X164" s="3" t="inlineStr"/>
       <c r="Y164" t="inlineStr"/>
+      <c r="Z164" s="3" t="inlineStr"/>
+      <c r="AA164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -12512,6 +13290,8 @@
       <c r="W165" t="inlineStr"/>
       <c r="X165" s="3" t="inlineStr"/>
       <c r="Y165" t="inlineStr"/>
+      <c r="Z165" s="3" t="inlineStr"/>
+      <c r="AA165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -12565,6 +13345,8 @@
       </c>
       <c r="X166" s="3" t="inlineStr"/>
       <c r="Y166" t="inlineStr"/>
+      <c r="Z166" s="3" t="inlineStr"/>
+      <c r="AA166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -12606,6 +13388,8 @@
       <c r="W167" t="inlineStr"/>
       <c r="X167" s="3" t="inlineStr"/>
       <c r="Y167" t="inlineStr"/>
+      <c r="Z167" s="3" t="inlineStr"/>
+      <c r="AA167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -12648,17 +13432,21 @@
       <c r="X168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y168" t="inlineStr">
-        <is>
-          <t>1229</t>
+      <c r="Y168" t="n">
+        <v>1229</v>
+      </c>
+      <c r="Z168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA168" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>24787683</t>
-        </is>
+      <c r="A169" t="n">
+        <v>24787683</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -12693,9 +13481,56 @@
       <c r="X169" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y169" t="inlineStr">
-        <is>
-          <t>4096</t>
+      <c r="Y169" t="n">
+        <v>4096</v>
+      </c>
+      <c r="Z169" s="3" t="inlineStr"/>
+      <c r="AA169" t="inlineStr"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>57531381</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>㊥蝦雞霸丸</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr"/>
+      <c r="D170" t="inlineStr"/>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F170" s="3" t="inlineStr"/>
+      <c r="G170" t="inlineStr"/>
+      <c r="H170" s="3" t="inlineStr"/>
+      <c r="I170" t="inlineStr"/>
+      <c r="J170" s="3" t="inlineStr"/>
+      <c r="K170" t="inlineStr"/>
+      <c r="L170" s="3" t="inlineStr"/>
+      <c r="M170" t="inlineStr"/>
+      <c r="N170" s="3" t="inlineStr"/>
+      <c r="O170" t="inlineStr"/>
+      <c r="P170" s="3" t="inlineStr"/>
+      <c r="Q170" t="inlineStr"/>
+      <c r="R170" s="3" t="inlineStr"/>
+      <c r="S170" t="inlineStr"/>
+      <c r="T170" s="3" t="inlineStr"/>
+      <c r="U170" t="inlineStr"/>
+      <c r="V170" s="3" t="inlineStr"/>
+      <c r="W170" t="inlineStr"/>
+      <c r="X170" s="3" t="inlineStr"/>
+      <c r="Y170" t="inlineStr"/>
+      <c r="Z170" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA170" t="inlineStr">
+        <is>
+          <t>5042</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-08 05:10:48
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA170"/>
+  <dimension ref="A1:AC170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>04-06_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>04-07_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>04-07_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -603,6 +613,8 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" s="3" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
+      <c r="AB2" s="3" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -644,6 +656,8 @@
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" s="3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
+      <c r="AB3" s="3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -685,6 +699,8 @@
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" s="3" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
+      <c r="AB4" s="3" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -746,6 +762,8 @@
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" s="3" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
+      <c r="AB5" s="3" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -787,6 +805,8 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" s="3" t="inlineStr"/>
       <c r="AA6" t="inlineStr"/>
+      <c r="AB6" s="3" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -828,6 +848,8 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" s="3" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
+      <c r="AB7" s="3" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -893,6 +915,8 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" s="3" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
+      <c r="AB8" s="3" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -934,6 +958,8 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" s="3" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
+      <c r="AB9" s="3" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1011,6 +1037,8 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" s="3" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
+      <c r="AB10" s="3" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1064,6 +1092,8 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" s="3" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
+      <c r="AB11" s="3" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1141,6 +1171,8 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" s="3" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
+      <c r="AB12" s="3" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1227,7 +1259,13 @@
       <c r="Z13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA13" t="inlineStr">
+      <c r="AA13" t="n">
+        <v>5808</v>
+      </c>
+      <c r="AB13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC13" t="inlineStr">
         <is>
           <t>5808</t>
         </is>
@@ -1309,6 +1347,8 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" s="3" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
+      <c r="AB14" s="3" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1386,6 +1426,8 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" s="3" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
+      <c r="AB15" s="3" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1439,6 +1481,8 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" s="3" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
+      <c r="AB16" s="3" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1504,6 +1548,8 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" s="3" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
+      <c r="AB17" s="3" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1565,6 +1611,8 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" s="3" t="inlineStr"/>
       <c r="AA18" t="inlineStr"/>
+      <c r="AB18" s="3" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1618,6 +1666,8 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" s="3" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
+      <c r="AB19" s="3" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1659,6 +1709,8 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" s="3" t="inlineStr"/>
       <c r="AA20" t="inlineStr"/>
+      <c r="AB20" s="3" t="inlineStr"/>
+      <c r="AC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1728,6 +1780,8 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" s="3" t="inlineStr"/>
       <c r="AA21" t="inlineStr"/>
+      <c r="AB21" s="3" t="inlineStr"/>
+      <c r="AC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1769,6 +1823,8 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" s="3" t="inlineStr"/>
       <c r="AA22" t="inlineStr"/>
+      <c r="AB22" s="3" t="inlineStr"/>
+      <c r="AC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1830,6 +1886,8 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" s="3" t="inlineStr"/>
       <c r="AA23" t="inlineStr"/>
+      <c r="AB23" s="3" t="inlineStr"/>
+      <c r="AC23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1907,6 +1965,8 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" s="3" t="inlineStr"/>
       <c r="AA24" t="inlineStr"/>
+      <c r="AB24" s="3" t="inlineStr"/>
+      <c r="AC24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1948,6 +2008,8 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" s="3" t="inlineStr"/>
       <c r="AA25" t="inlineStr"/>
+      <c r="AB25" s="3" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1989,6 +2051,8 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" s="3" t="inlineStr"/>
       <c r="AA26" t="inlineStr"/>
+      <c r="AB26" s="3" t="inlineStr"/>
+      <c r="AC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2030,6 +2094,8 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" s="3" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
+      <c r="AB27" s="3" t="inlineStr"/>
+      <c r="AC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2071,6 +2137,8 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" s="3" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
+      <c r="AB28" s="3" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2112,6 +2180,8 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" s="3" t="inlineStr"/>
       <c r="AA29" t="inlineStr"/>
+      <c r="AB29" s="3" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2153,6 +2223,8 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" s="3" t="inlineStr"/>
       <c r="AA30" t="inlineStr"/>
+      <c r="AB30" s="3" t="inlineStr"/>
+      <c r="AC30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2194,6 +2266,8 @@
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" s="3" t="inlineStr"/>
       <c r="AA31" t="inlineStr"/>
+      <c r="AB31" s="3" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2235,6 +2309,8 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" s="3" t="inlineStr"/>
       <c r="AA32" t="inlineStr"/>
+      <c r="AB32" s="3" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2276,6 +2352,8 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" s="3" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
+      <c r="AB33" s="3" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2317,6 +2395,8 @@
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" s="3" t="inlineStr"/>
       <c r="AA34" t="inlineStr"/>
+      <c r="AB34" s="3" t="inlineStr"/>
+      <c r="AC34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2403,7 +2483,13 @@
       <c r="Z35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA35" t="inlineStr">
+      <c r="AA35" t="n">
+        <v>2559</v>
+      </c>
+      <c r="AB35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="inlineStr">
         <is>
           <t>2559</t>
         </is>
@@ -2465,6 +2551,8 @@
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" s="3" t="inlineStr"/>
       <c r="AA36" t="inlineStr"/>
+      <c r="AB36" s="3" t="inlineStr"/>
+      <c r="AC36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2506,6 +2594,8 @@
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" s="3" t="inlineStr"/>
       <c r="AA37" t="inlineStr"/>
+      <c r="AB37" s="3" t="inlineStr"/>
+      <c r="AC37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2547,6 +2637,8 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" s="3" t="inlineStr"/>
       <c r="AA38" t="inlineStr"/>
+      <c r="AB38" s="3" t="inlineStr"/>
+      <c r="AC38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2633,7 +2725,13 @@
       <c r="Z39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="AA39" t="inlineStr">
+      <c r="AA39" t="n">
+        <v>5598</v>
+      </c>
+      <c r="AB39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC39" t="inlineStr">
         <is>
           <t>5598</t>
         </is>
@@ -2724,7 +2822,13 @@
       <c r="Z40" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA40" t="inlineStr">
+      <c r="AA40" t="n">
+        <v>5189</v>
+      </c>
+      <c r="AB40" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC40" t="inlineStr">
         <is>
           <t>5189</t>
         </is>
@@ -2770,6 +2874,8 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" s="3" t="inlineStr"/>
       <c r="AA41" t="inlineStr"/>
+      <c r="AB41" s="3" t="inlineStr"/>
+      <c r="AC41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2856,7 +2962,13 @@
       <c r="Z42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA42" t="inlineStr">
+      <c r="AA42" t="n">
+        <v>5192</v>
+      </c>
+      <c r="AB42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC42" t="inlineStr">
         <is>
           <t>5192</t>
         </is>
@@ -2902,6 +3014,8 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" s="3" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
+      <c r="AB43" s="3" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2988,7 +3102,13 @@
       <c r="Z44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA44" t="inlineStr">
+      <c r="AA44" t="n">
+        <v>4577</v>
+      </c>
+      <c r="AB44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC44" t="inlineStr">
         <is>
           <t>4577</t>
         </is>
@@ -3079,7 +3199,13 @@
       <c r="Z45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA45" t="inlineStr">
+      <c r="AA45" t="n">
+        <v>4729</v>
+      </c>
+      <c r="AB45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC45" t="inlineStr">
         <is>
           <t>4729</t>
         </is>
@@ -3170,7 +3296,13 @@
       <c r="Z46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA46" t="inlineStr">
+      <c r="AA46" t="n">
+        <v>3736</v>
+      </c>
+      <c r="AB46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC46" t="inlineStr">
         <is>
           <t>3736</t>
         </is>
@@ -3261,7 +3393,13 @@
       <c r="Z47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA47" t="inlineStr">
+      <c r="AA47" t="n">
+        <v>3349</v>
+      </c>
+      <c r="AB47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC47" t="inlineStr">
         <is>
           <t>3349</t>
         </is>
@@ -3352,7 +3490,13 @@
       <c r="Z48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA48" t="inlineStr">
+      <c r="AA48" t="n">
+        <v>2563</v>
+      </c>
+      <c r="AB48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" t="inlineStr">
         <is>
           <t>2563</t>
         </is>
@@ -3443,7 +3587,13 @@
       <c r="Z49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA49" t="inlineStr">
+      <c r="AA49" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3501,6 +3651,8 @@
       <c r="Y50" t="inlineStr"/>
       <c r="Z50" s="3" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
+      <c r="AB50" s="3" t="inlineStr"/>
+      <c r="AC50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3542,6 +3694,8 @@
       <c r="Y51" t="inlineStr"/>
       <c r="Z51" s="3" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
+      <c r="AB51" s="3" t="inlineStr"/>
+      <c r="AC51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3628,7 +3782,13 @@
       <c r="Z52" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="AA52" t="inlineStr">
+      <c r="AA52" t="n">
+        <v>5513</v>
+      </c>
+      <c r="AB52" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC52" t="inlineStr">
         <is>
           <t>5513</t>
         </is>
@@ -3719,7 +3879,13 @@
       <c r="Z53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA53" t="inlineStr">
+      <c r="AA53" t="n">
+        <v>5154</v>
+      </c>
+      <c r="AB53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC53" t="inlineStr">
         <is>
           <t>5154</t>
         </is>
@@ -3765,6 +3931,8 @@
       <c r="Y54" t="inlineStr"/>
       <c r="Z54" s="3" t="inlineStr"/>
       <c r="AA54" t="inlineStr"/>
+      <c r="AB54" s="3" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3851,7 +4019,13 @@
       <c r="Z55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA55" t="inlineStr">
+      <c r="AA55" t="n">
+        <v>5539</v>
+      </c>
+      <c r="AB55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC55" t="inlineStr">
         <is>
           <t>5539</t>
         </is>
@@ -3942,7 +4116,13 @@
       <c r="Z56" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA56" t="inlineStr">
+      <c r="AA56" t="n">
+        <v>5754</v>
+      </c>
+      <c r="AB56" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC56" t="inlineStr">
         <is>
           <t>5754</t>
         </is>
@@ -4033,7 +4213,13 @@
       <c r="Z57" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA57" t="inlineStr">
+      <c r="AA57" t="n">
+        <v>5472</v>
+      </c>
+      <c r="AB57" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC57" t="inlineStr">
         <is>
           <t>5472</t>
         </is>
@@ -4124,7 +4310,13 @@
       <c r="Z58" s="4" t="n">
         <v>31</v>
       </c>
-      <c r="AA58" t="inlineStr">
+      <c r="AA58" t="n">
+        <v>5291</v>
+      </c>
+      <c r="AB58" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC58" t="inlineStr">
         <is>
           <t>5291</t>
         </is>
@@ -4215,7 +4407,13 @@
       <c r="Z59" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="AA59" t="inlineStr">
+      <c r="AA59" t="n">
+        <v>5054</v>
+      </c>
+      <c r="AB59" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC59" t="inlineStr">
         <is>
           <t>5054</t>
         </is>
@@ -4306,7 +4504,13 @@
       <c r="Z60" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA60" t="inlineStr">
+      <c r="AA60" t="n">
+        <v>5212</v>
+      </c>
+      <c r="AB60" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC60" t="inlineStr">
         <is>
           <t>5212</t>
         </is>
@@ -4397,7 +4601,13 @@
       <c r="Z61" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA61" t="inlineStr">
+      <c r="AA61" t="n">
+        <v>4964</v>
+      </c>
+      <c r="AB61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC61" t="inlineStr">
         <is>
           <t>4964</t>
         </is>
@@ -4488,7 +4698,13 @@
       <c r="Z62" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="AA62" t="inlineStr">
+      <c r="AA62" t="n">
+        <v>6131</v>
+      </c>
+      <c r="AB62" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC62" t="inlineStr">
         <is>
           <t>6131</t>
         </is>
@@ -4579,7 +4795,13 @@
       <c r="Z63" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA63" t="inlineStr">
+      <c r="AA63" t="n">
+        <v>5918</v>
+      </c>
+      <c r="AB63" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC63" t="inlineStr">
         <is>
           <t>5918</t>
         </is>
@@ -4670,7 +4892,13 @@
       <c r="Z64" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA64" t="inlineStr">
+      <c r="AA64" t="n">
+        <v>5941</v>
+      </c>
+      <c r="AB64" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC64" t="inlineStr">
         <is>
           <t>5941</t>
         </is>
@@ -4716,6 +4944,8 @@
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" s="3" t="inlineStr"/>
       <c r="AA65" t="inlineStr"/>
+      <c r="AB65" s="3" t="inlineStr"/>
+      <c r="AC65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4802,7 +5032,13 @@
       <c r="Z66" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA66" t="inlineStr">
+      <c r="AA66" t="n">
+        <v>5609</v>
+      </c>
+      <c r="AB66" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC66" t="inlineStr">
         <is>
           <t>5609</t>
         </is>
@@ -4893,7 +5129,13 @@
       <c r="Z67" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA67" t="inlineStr">
+      <c r="AA67" t="n">
+        <v>5279</v>
+      </c>
+      <c r="AB67" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC67" t="inlineStr">
         <is>
           <t>5279</t>
         </is>
@@ -4984,7 +5226,13 @@
       <c r="Z68" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="AA68" t="inlineStr">
+      <c r="AA68" t="n">
+        <v>5282</v>
+      </c>
+      <c r="AB68" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC68" t="inlineStr">
         <is>
           <t>5282</t>
         </is>
@@ -5075,7 +5323,13 @@
       <c r="Z69" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA69" t="inlineStr">
+      <c r="AA69" t="n">
+        <v>4945</v>
+      </c>
+      <c r="AB69" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC69" t="inlineStr">
         <is>
           <t>4945</t>
         </is>
@@ -5166,7 +5420,13 @@
       <c r="Z70" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="AA70" t="inlineStr">
+      <c r="AA70" t="n">
+        <v>4953</v>
+      </c>
+      <c r="AB70" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC70" t="inlineStr">
         <is>
           <t>4953</t>
         </is>
@@ -5257,7 +5517,13 @@
       <c r="Z71" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA71" t="inlineStr">
+      <c r="AA71" t="n">
+        <v>5728</v>
+      </c>
+      <c r="AB71" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC71" t="inlineStr">
         <is>
           <t>5728</t>
         </is>
@@ -5348,7 +5614,13 @@
       <c r="Z72" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA72" t="inlineStr">
+      <c r="AA72" t="n">
+        <v>5075</v>
+      </c>
+      <c r="AB72" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC72" t="inlineStr">
         <is>
           <t>5075</t>
         </is>
@@ -5439,7 +5711,13 @@
       <c r="Z73" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA73" t="inlineStr">
+      <c r="AA73" t="n">
+        <v>3958</v>
+      </c>
+      <c r="AB73" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC73" t="inlineStr">
         <is>
           <t>3958</t>
         </is>
@@ -5530,7 +5808,13 @@
       <c r="Z74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA74" t="inlineStr">
+      <c r="AA74" t="n">
+        <v>4584</v>
+      </c>
+      <c r="AB74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" t="inlineStr">
         <is>
           <t>4584</t>
         </is>
@@ -5621,7 +5905,13 @@
       <c r="Z75" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA75" t="inlineStr">
+      <c r="AA75" t="n">
+        <v>3809</v>
+      </c>
+      <c r="AB75" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC75" t="inlineStr">
         <is>
           <t>3809</t>
         </is>
@@ -5707,6 +5997,8 @@
       <c r="Y76" t="inlineStr"/>
       <c r="Z76" s="3" t="inlineStr"/>
       <c r="AA76" t="inlineStr"/>
+      <c r="AB76" s="3" t="inlineStr"/>
+      <c r="AC76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5793,7 +6085,13 @@
       <c r="Z77" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA77" t="inlineStr">
+      <c r="AA77" t="n">
+        <v>4804</v>
+      </c>
+      <c r="AB77" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC77" t="inlineStr">
         <is>
           <t>4804</t>
         </is>
@@ -5884,7 +6182,13 @@
       <c r="Z78" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA78" t="inlineStr">
+      <c r="AA78" t="n">
+        <v>4405</v>
+      </c>
+      <c r="AB78" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC78" t="inlineStr">
         <is>
           <t>4405</t>
         </is>
@@ -5975,7 +6279,13 @@
       <c r="Z79" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA79" t="inlineStr">
+      <c r="AA79" t="n">
+        <v>4128</v>
+      </c>
+      <c r="AB79" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC79" t="inlineStr">
         <is>
           <t>4128</t>
         </is>
@@ -6066,7 +6376,13 @@
       <c r="Z80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA80" t="inlineStr">
+      <c r="AA80" t="n">
+        <v>4053</v>
+      </c>
+      <c r="AB80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC80" t="inlineStr">
         <is>
           <t>4053</t>
         </is>
@@ -6157,7 +6473,13 @@
       <c r="Z81" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA81" t="inlineStr">
+      <c r="AA81" t="n">
+        <v>4173</v>
+      </c>
+      <c r="AB81" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC81" t="inlineStr">
         <is>
           <t>4173</t>
         </is>
@@ -6248,7 +6570,13 @@
       <c r="Z82" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA82" t="inlineStr">
+      <c r="AA82" t="n">
+        <v>4149</v>
+      </c>
+      <c r="AB82" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC82" t="inlineStr">
         <is>
           <t>4149</t>
         </is>
@@ -6339,7 +6667,13 @@
       <c r="Z83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA83" t="inlineStr">
+      <c r="AA83" t="n">
+        <v>2659</v>
+      </c>
+      <c r="AB83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC83" t="inlineStr">
         <is>
           <t>2659</t>
         </is>
@@ -6401,6 +6735,8 @@
       <c r="Y84" t="inlineStr"/>
       <c r="Z84" s="3" t="inlineStr"/>
       <c r="AA84" t="inlineStr"/>
+      <c r="AB84" s="3" t="inlineStr"/>
+      <c r="AC84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -6450,6 +6786,8 @@
       <c r="Y85" t="inlineStr"/>
       <c r="Z85" s="3" t="inlineStr"/>
       <c r="AA85" t="inlineStr"/>
+      <c r="AB85" s="3" t="inlineStr"/>
+      <c r="AC85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -6507,6 +6845,8 @@
       <c r="Y86" t="inlineStr"/>
       <c r="Z86" s="3" t="inlineStr"/>
       <c r="AA86" t="inlineStr"/>
+      <c r="AB86" s="3" t="inlineStr"/>
+      <c r="AC86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -6593,7 +6933,13 @@
       <c r="Z87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA87" t="inlineStr">
+      <c r="AA87" t="n">
+        <v>4189</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
         <is>
           <t>4189</t>
         </is>
@@ -6647,6 +6993,8 @@
       <c r="Y88" t="inlineStr"/>
       <c r="Z88" s="3" t="inlineStr"/>
       <c r="AA88" t="inlineStr"/>
+      <c r="AB88" s="3" t="inlineStr"/>
+      <c r="AC88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6688,6 +7036,8 @@
       <c r="Y89" t="inlineStr"/>
       <c r="Z89" s="3" t="inlineStr"/>
       <c r="AA89" t="inlineStr"/>
+      <c r="AB89" s="3" t="inlineStr"/>
+      <c r="AC89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6774,7 +7124,13 @@
       <c r="Z90" s="4" t="n">
         <v>32</v>
       </c>
-      <c r="AA90" t="inlineStr">
+      <c r="AA90" t="n">
+        <v>5399</v>
+      </c>
+      <c r="AB90" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC90" t="inlineStr">
         <is>
           <t>5399</t>
         </is>
@@ -6865,7 +7221,13 @@
       <c r="Z91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA91" t="inlineStr">
+      <c r="AA91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6956,7 +7318,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>2744</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>2744</t>
         </is>
@@ -7047,7 +7415,13 @@
       <c r="Z93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA93" t="inlineStr">
+      <c r="AA93" t="n">
+        <v>2540</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="inlineStr">
         <is>
           <t>2540</t>
         </is>
@@ -7138,7 +7512,13 @@
       <c r="Z94" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="AA94" t="inlineStr">
+      <c r="AA94" t="n">
+        <v>4819</v>
+      </c>
+      <c r="AB94" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC94" t="inlineStr">
         <is>
           <t>4819</t>
         </is>
@@ -7229,7 +7609,13 @@
       <c r="Z95" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA95" t="inlineStr">
+      <c r="AA95" t="n">
+        <v>4773</v>
+      </c>
+      <c r="AB95" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC95" t="inlineStr">
         <is>
           <t>4773</t>
         </is>
@@ -7320,7 +7706,13 @@
       <c r="Z96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA96" t="inlineStr">
+      <c r="AA96" t="n">
+        <v>2918</v>
+      </c>
+      <c r="AB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" t="inlineStr">
         <is>
           <t>2918</t>
         </is>
@@ -7411,7 +7803,13 @@
       <c r="Z97" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AA97" t="inlineStr">
+      <c r="AA97" t="n">
+        <v>4743</v>
+      </c>
+      <c r="AB97" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC97" t="inlineStr">
         <is>
           <t>4743</t>
         </is>
@@ -7502,7 +7900,13 @@
       <c r="Z98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA98" t="inlineStr">
+      <c r="AA98" t="n">
+        <v>3361</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
         <is>
           <t>3361</t>
         </is>
@@ -7593,7 +7997,13 @@
       <c r="Z99" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AA99" t="inlineStr">
+      <c r="AA99" t="n">
+        <v>4376</v>
+      </c>
+      <c r="AB99" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC99" t="inlineStr">
         <is>
           <t>4376</t>
         </is>
@@ -7684,7 +8094,13 @@
       <c r="Z100" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA100" t="inlineStr">
+      <c r="AA100" t="n">
+        <v>4497</v>
+      </c>
+      <c r="AB100" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC100" t="inlineStr">
         <is>
           <t>4497</t>
         </is>
@@ -7775,7 +8191,13 @@
       <c r="Z101" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA101" t="inlineStr">
+      <c r="AA101" t="n">
+        <v>4957</v>
+      </c>
+      <c r="AB101" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC101" t="inlineStr">
         <is>
           <t>4957</t>
         </is>
@@ -7866,7 +8288,13 @@
       <c r="Z102" s="5" t="n">
         <v>16</v>
       </c>
-      <c r="AA102" t="inlineStr">
+      <c r="AA102" t="n">
+        <v>4499</v>
+      </c>
+      <c r="AB102" s="5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC102" t="inlineStr">
         <is>
           <t>4499</t>
         </is>
@@ -7957,7 +8385,13 @@
       <c r="Z103" s="5" t="n">
         <v>17</v>
       </c>
-      <c r="AA103" t="inlineStr">
+      <c r="AA103" t="n">
+        <v>4465</v>
+      </c>
+      <c r="AB103" s="5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC103" t="inlineStr">
         <is>
           <t>4465</t>
         </is>
@@ -8048,7 +8482,13 @@
       <c r="Z104" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA104" t="inlineStr">
+      <c r="AA104" t="n">
+        <v>4332</v>
+      </c>
+      <c r="AB104" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC104" t="inlineStr">
         <is>
           <t>4332</t>
         </is>
@@ -8139,7 +8579,13 @@
       <c r="Z105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA105" t="inlineStr">
+      <c r="AA105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8230,7 +8676,13 @@
       <c r="Z106" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA106" t="inlineStr">
+      <c r="AA106" t="n">
+        <v>4410</v>
+      </c>
+      <c r="AB106" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC106" t="inlineStr">
         <is>
           <t>4410</t>
         </is>
@@ -8321,7 +8773,13 @@
       <c r="Z107" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA107" t="inlineStr">
+      <c r="AA107" t="n">
+        <v>4316</v>
+      </c>
+      <c r="AB107" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC107" t="inlineStr">
         <is>
           <t>4316</t>
         </is>
@@ -8412,7 +8870,13 @@
       <c r="Z108" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="AA108" t="inlineStr">
+      <c r="AA108" t="n">
+        <v>4370</v>
+      </c>
+      <c r="AB108" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC108" t="inlineStr">
         <is>
           <t>4370</t>
         </is>
@@ -8503,7 +8967,13 @@
       <c r="Z109" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AA109" t="inlineStr">
+      <c r="AA109" t="n">
+        <v>3169</v>
+      </c>
+      <c r="AB109" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC109" t="inlineStr">
         <is>
           <t>3169</t>
         </is>
@@ -8594,7 +9064,13 @@
       <c r="Z110" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA110" t="inlineStr">
+      <c r="AA110" t="n">
+        <v>4217</v>
+      </c>
+      <c r="AB110" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC110" t="inlineStr">
         <is>
           <t>4217</t>
         </is>
@@ -8640,6 +9116,8 @@
       <c r="Y111" t="inlineStr"/>
       <c r="Z111" s="3" t="inlineStr"/>
       <c r="AA111" t="inlineStr"/>
+      <c r="AB111" s="3" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8726,7 +9204,13 @@
       <c r="Z112" s="5" t="n">
         <v>18</v>
       </c>
-      <c r="AA112" t="inlineStr">
+      <c r="AA112" t="n">
+        <v>4123</v>
+      </c>
+      <c r="AB112" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC112" t="inlineStr">
         <is>
           <t>4123</t>
         </is>
@@ -8817,7 +9301,13 @@
       <c r="Z113" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="AA113" t="inlineStr">
+      <c r="AA113" t="n">
+        <v>3590</v>
+      </c>
+      <c r="AB113" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC113" t="inlineStr">
         <is>
           <t>3590</t>
         </is>
@@ -8908,7 +9398,13 @@
       <c r="Z114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA114" t="inlineStr">
+      <c r="AA114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8995,7 +9491,13 @@
       <c r="Z115" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA115" t="inlineStr">
+      <c r="AA115" t="n">
+        <v>3445</v>
+      </c>
+      <c r="AB115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC115" t="inlineStr">
         <is>
           <t>3445</t>
         </is>
@@ -9086,7 +9588,13 @@
       <c r="Z116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA116" t="inlineStr">
+      <c r="AA116" t="n">
+        <v>3161</v>
+      </c>
+      <c r="AB116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC116" t="inlineStr">
         <is>
           <t>3161</t>
         </is>
@@ -9140,6 +9648,8 @@
       <c r="Y117" t="inlineStr"/>
       <c r="Z117" s="3" t="inlineStr"/>
       <c r="AA117" t="inlineStr"/>
+      <c r="AB117" s="3" t="inlineStr"/>
+      <c r="AC117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -9181,6 +9691,8 @@
       <c r="Y118" t="inlineStr"/>
       <c r="Z118" s="3" t="inlineStr"/>
       <c r="AA118" t="inlineStr"/>
+      <c r="AB118" s="3" t="inlineStr"/>
+      <c r="AC118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -9267,7 +9779,13 @@
       <c r="Z119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA119" t="inlineStr">
+      <c r="AA119" t="n">
+        <v>2744</v>
+      </c>
+      <c r="AB119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" t="inlineStr">
         <is>
           <t>2744</t>
         </is>
@@ -9349,6 +9867,8 @@
       <c r="Y120" t="inlineStr"/>
       <c r="Z120" s="3" t="inlineStr"/>
       <c r="AA120" t="inlineStr"/>
+      <c r="AB120" s="3" t="inlineStr"/>
+      <c r="AC120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -9435,7 +9955,13 @@
       <c r="Z121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA121" t="inlineStr">
+      <c r="AA121" t="n">
+        <v>2888</v>
+      </c>
+      <c r="AB121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="inlineStr">
         <is>
           <t>2888</t>
         </is>
@@ -9526,7 +10052,13 @@
       <c r="Z122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA122" t="inlineStr">
+      <c r="AA122" t="n">
+        <v>3323</v>
+      </c>
+      <c r="AB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC122" t="inlineStr">
         <is>
           <t>3323</t>
         </is>
@@ -9592,6 +10124,8 @@
       <c r="Y123" t="inlineStr"/>
       <c r="Z123" s="3" t="inlineStr"/>
       <c r="AA123" t="inlineStr"/>
+      <c r="AB123" s="3" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -9678,7 +10212,13 @@
       <c r="Z124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA124" t="inlineStr">
+      <c r="AA124" t="n">
+        <v>2444</v>
+      </c>
+      <c r="AB124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC124" t="inlineStr">
         <is>
           <t>2444</t>
         </is>
@@ -9769,7 +10309,13 @@
       <c r="Z125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA125" t="inlineStr">
+      <c r="AA125" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC125" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9860,7 +10406,13 @@
       <c r="Z126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA126" t="inlineStr">
+      <c r="AA126" t="n">
+        <v>1464</v>
+      </c>
+      <c r="AB126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC126" t="inlineStr">
         <is>
           <t>1464</t>
         </is>
@@ -9951,7 +10503,13 @@
       <c r="Z127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA127" t="inlineStr">
+      <c r="AA127" t="n">
+        <v>1613</v>
+      </c>
+      <c r="AB127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC127" t="inlineStr">
         <is>
           <t>1613</t>
         </is>
@@ -10042,7 +10600,13 @@
       <c r="Z128" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA128" t="inlineStr">
+      <c r="AA128" t="n">
+        <v>1230</v>
+      </c>
+      <c r="AB128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC128" t="inlineStr">
         <is>
           <t>1230</t>
         </is>
@@ -10133,7 +10697,13 @@
       <c r="Z129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA129" t="inlineStr">
+      <c r="AA129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC129" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10224,7 +10794,13 @@
       <c r="Z130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA130" t="inlineStr">
+      <c r="AA130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10315,7 +10891,13 @@
       <c r="Z131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA131" t="inlineStr">
+      <c r="AA131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10406,7 +10988,13 @@
       <c r="Z132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA132" t="inlineStr">
+      <c r="AA132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC132" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10497,7 +11085,13 @@
       <c r="Z133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA133" t="inlineStr">
+      <c r="AA133" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC133" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10588,7 +11182,13 @@
       <c r="Z134" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA134" t="inlineStr">
+      <c r="AA134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC134" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10679,7 +11279,13 @@
       <c r="Z135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA135" t="inlineStr">
+      <c r="AA135" t="n">
+        <v>3034</v>
+      </c>
+      <c r="AB135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC135" t="inlineStr">
         <is>
           <t>3034</t>
         </is>
@@ -10770,7 +11376,13 @@
       <c r="Z136" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA136" t="inlineStr">
+      <c r="AA136" t="n">
+        <v>4048</v>
+      </c>
+      <c r="AB136" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC136" t="inlineStr">
         <is>
           <t>4048</t>
         </is>
@@ -10861,7 +11473,13 @@
       <c r="Z137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA137" t="inlineStr">
+      <c r="AA137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC137" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10952,7 +11570,13 @@
       <c r="Z138" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA138" t="inlineStr">
+      <c r="AA138" t="n">
+        <v>2899</v>
+      </c>
+      <c r="AB138" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC138" t="inlineStr">
         <is>
           <t>2899</t>
         </is>
@@ -11043,7 +11667,13 @@
       <c r="Z139" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA139" t="inlineStr">
+      <c r="AA139" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB139" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC139" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11134,7 +11764,13 @@
       <c r="Z140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA140" t="inlineStr">
+      <c r="AA140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC140" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11225,7 +11861,13 @@
       <c r="Z141" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA141" t="inlineStr">
+      <c r="AA141" t="n">
+        <v>2022</v>
+      </c>
+      <c r="AB141" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC141" t="inlineStr">
         <is>
           <t>2022</t>
         </is>
@@ -11316,7 +11958,13 @@
       <c r="Z142" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="AA142" t="inlineStr">
+      <c r="AA142" t="n">
+        <v>1999</v>
+      </c>
+      <c r="AB142" s="5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC142" t="inlineStr">
         <is>
           <t>1999</t>
         </is>
@@ -11407,7 +12055,13 @@
       <c r="Z143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA143" t="inlineStr">
+      <c r="AA143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11498,7 +12152,13 @@
       <c r="Z144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA144" t="inlineStr">
+      <c r="AA144" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC144" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11589,7 +12249,13 @@
       <c r="Z145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA145" t="inlineStr">
+      <c r="AA145" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC145" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11680,7 +12346,13 @@
       <c r="Z146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA146" t="inlineStr">
+      <c r="AA146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11771,7 +12443,13 @@
       <c r="Z147" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA147" t="inlineStr">
+      <c r="AA147" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB147" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC147" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11862,7 +12540,13 @@
       <c r="Z148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA148" t="inlineStr">
+      <c r="AA148" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC148" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11953,7 +12637,13 @@
       <c r="Z149" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA149" t="inlineStr">
+      <c r="AA149" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB149" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC149" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12044,7 +12734,13 @@
       <c r="Z150" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA150" t="inlineStr">
+      <c r="AA150" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB150" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC150" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12135,7 +12831,13 @@
       <c r="Z151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA151" t="inlineStr">
+      <c r="AA151" t="n">
+        <v>3135</v>
+      </c>
+      <c r="AB151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC151" t="inlineStr">
         <is>
           <t>3135</t>
         </is>
@@ -12226,7 +12928,13 @@
       <c r="Z152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA152" t="inlineStr">
+      <c r="AA152" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC152" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12317,7 +13025,13 @@
       <c r="Z153" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA153" t="inlineStr">
+      <c r="AA153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB153" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC153" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12408,7 +13122,13 @@
       <c r="Z154" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA154" t="inlineStr">
+      <c r="AA154" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB154" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC154" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12499,7 +13219,13 @@
       <c r="Z155" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA155" t="inlineStr">
+      <c r="AA155" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB155" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC155" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12590,7 +13316,13 @@
       <c r="Z156" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA156" t="inlineStr">
+      <c r="AA156" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB156" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC156" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12681,7 +13413,13 @@
       <c r="Z157" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA157" t="inlineStr">
+      <c r="AA157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB157" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC157" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12772,7 +13510,13 @@
       <c r="Z158" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA158" t="inlineStr">
+      <c r="AA158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB158" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC158" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12857,7 +13601,13 @@
       <c r="Z159" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA159" t="inlineStr">
+      <c r="AA159" t="n">
+        <v>2709</v>
+      </c>
+      <c r="AB159" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC159" t="inlineStr">
         <is>
           <t>2709</t>
         </is>
@@ -12942,7 +13692,13 @@
       <c r="Z160" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA160" t="inlineStr">
+      <c r="AA160" t="n">
+        <v>1784</v>
+      </c>
+      <c r="AB160" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC160" t="inlineStr">
         <is>
           <t>1784</t>
         </is>
@@ -13027,7 +13783,13 @@
       <c r="Z161" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA161" t="inlineStr">
+      <c r="AA161" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB161" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC161" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13108,7 +13870,13 @@
       <c r="Z162" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA162" t="inlineStr">
+      <c r="AA162" t="n">
+        <v>2315</v>
+      </c>
+      <c r="AB162" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC162" t="inlineStr">
         <is>
           <t>2315</t>
         </is>
@@ -13185,7 +13953,13 @@
       <c r="Z163" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA163" t="inlineStr">
+      <c r="AA163" t="n">
+        <v>2817</v>
+      </c>
+      <c r="AB163" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC163" t="inlineStr">
         <is>
           <t>2817</t>
         </is>
@@ -13237,6 +14011,8 @@
       <c r="Y164" t="inlineStr"/>
       <c r="Z164" s="3" t="inlineStr"/>
       <c r="AA164" t="inlineStr"/>
+      <c r="AB164" s="3" t="inlineStr"/>
+      <c r="AC164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -13292,6 +14068,8 @@
       <c r="Y165" t="inlineStr"/>
       <c r="Z165" s="3" t="inlineStr"/>
       <c r="AA165" t="inlineStr"/>
+      <c r="AB165" s="3" t="inlineStr"/>
+      <c r="AC165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -13347,6 +14125,8 @@
       <c r="Y166" t="inlineStr"/>
       <c r="Z166" s="3" t="inlineStr"/>
       <c r="AA166" t="inlineStr"/>
+      <c r="AB166" s="3" t="inlineStr"/>
+      <c r="AC166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -13390,6 +14170,8 @@
       <c r="Y167" t="inlineStr"/>
       <c r="Z167" s="3" t="inlineStr"/>
       <c r="AA167" t="inlineStr"/>
+      <c r="AB167" s="3" t="inlineStr"/>
+      <c r="AC167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -13438,7 +14220,13 @@
       <c r="Z168" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA168" t="inlineStr">
+      <c r="AA168" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB168" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC168" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13486,12 +14274,12 @@
       </c>
       <c r="Z169" s="3" t="inlineStr"/>
       <c r="AA169" t="inlineStr"/>
+      <c r="AB169" s="3" t="inlineStr"/>
+      <c r="AC169" t="inlineStr"/>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>57531381</t>
-        </is>
+      <c r="A170" t="n">
+        <v>57531381</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -13528,7 +14316,13 @@
       <c r="Z170" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA170" t="inlineStr">
+      <c r="AA170" t="n">
+        <v>5042</v>
+      </c>
+      <c r="AB170" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC170" t="inlineStr">
         <is>
           <t>5042</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-08 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/87.xlsx
+++ b/Season_Attack/87.xlsx
@@ -1267,7 +1267,7 @@
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>5808</t>
+          <t>6052</t>
         </is>
       </c>
     </row>
@@ -2729,11 +2729,11 @@
         <v>5598</v>
       </c>
       <c r="AB39" s="3" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC39" t="inlineStr">
         <is>
-          <t>5598</t>
+          <t>5848</t>
         </is>
       </c>
     </row>
@@ -2826,11 +2826,11 @@
         <v>5189</v>
       </c>
       <c r="AB40" s="3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AC40" t="inlineStr">
         <is>
-          <t>5189</t>
+          <t>5339</t>
         </is>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="AC42" t="inlineStr">
         <is>
-          <t>5192</t>
+          <t>5339</t>
         </is>
       </c>
     </row>
@@ -3203,11 +3203,11 @@
         <v>4729</v>
       </c>
       <c r="AB45" s="3" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AC45" t="inlineStr">
         <is>
-          <t>4729</t>
+          <t>4773</t>
         </is>
       </c>
     </row>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="AC47" t="inlineStr">
         <is>
-          <t>3349</t>
+          <t>3380</t>
         </is>
       </c>
     </row>
@@ -3493,12 +3493,12 @@
       <c r="AA48" t="n">
         <v>2563</v>
       </c>
-      <c r="AB48" s="2" t="n">
-        <v>0</v>
+      <c r="AB48" s="4" t="n">
+        <v>40</v>
       </c>
       <c r="AC48" t="inlineStr">
         <is>
-          <t>2563</t>
+          <t>3807</t>
         </is>
       </c>
     </row>
@@ -3790,7 +3790,7 @@
       </c>
       <c r="AC52" t="inlineStr">
         <is>
-          <t>5513</t>
+          <t>5641</t>
         </is>
       </c>
     </row>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="AC53" t="inlineStr">
         <is>
-          <t>5154</t>
+          <t>5285</t>
         </is>
       </c>
     </row>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="AC55" t="inlineStr">
         <is>
-          <t>5539</t>
+          <t>5762</t>
         </is>
       </c>
     </row>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="AC56" t="inlineStr">
         <is>
-          <t>5754</t>
+          <t>5906</t>
         </is>
       </c>
     </row>
@@ -4221,7 +4221,7 @@
       </c>
       <c r="AC57" t="inlineStr">
         <is>
-          <t>5472</t>
+          <t>5760</t>
         </is>
       </c>
     </row>
@@ -4313,12 +4313,12 @@
       <c r="AA58" t="n">
         <v>5291</v>
       </c>
-      <c r="AB58" s="4" t="n">
-        <v>31</v>
+      <c r="AB58" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="AC58" t="inlineStr">
         <is>
-          <t>5291</t>
+          <t>5430</t>
         </is>
       </c>
     </row>
@@ -4410,12 +4410,12 @@
       <c r="AA59" t="n">
         <v>5054</v>
       </c>
-      <c r="AB59" s="5" t="n">
-        <v>9</v>
+      <c r="AB59" s="4" t="n">
+        <v>40</v>
       </c>
       <c r="AC59" t="inlineStr">
         <is>
-          <t>5054</t>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -4508,11 +4508,11 @@
         <v>5212</v>
       </c>
       <c r="AB60" s="3" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AC60" t="inlineStr">
         <is>
-          <t>5212</t>
+          <t>5373</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="AC61" t="inlineStr">
         <is>
-          <t>4964</t>
+          <t>5058</t>
         </is>
       </c>
     </row>
@@ -4702,11 +4702,11 @@
         <v>6131</v>
       </c>
       <c r="AB62" s="4" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC62" t="inlineStr">
         <is>
-          <t>6131</t>
+          <t>6332</t>
         </is>
       </c>
     </row>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="AC63" t="inlineStr">
         <is>
-          <t>5918</t>
+          <t>6204</t>
         </is>
       </c>
     </row>
@@ -4900,7 +4900,7 @@
       </c>
       <c r="AC64" t="inlineStr">
         <is>
-          <t>5941</t>
+          <t>6089</t>
         </is>
       </c>
     </row>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="AC66" t="inlineStr">
         <is>
-          <t>5609</t>
+          <t>5707</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="AC67" t="inlineStr">
         <is>
-          <t>5279</t>
+          <t>5439</t>
         </is>
       </c>
     </row>
@@ -5230,11 +5230,11 @@
         <v>5282</v>
       </c>
       <c r="AB68" s="4" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC68" t="inlineStr">
         <is>
-          <t>5282</t>
+          <t>5447</t>
         </is>
       </c>
     </row>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="AC69" t="inlineStr">
         <is>
-          <t>4945</t>
+          <t>5083</t>
         </is>
       </c>
     </row>
@@ -5423,12 +5423,12 @@
       <c r="AA70" t="n">
         <v>4953</v>
       </c>
-      <c r="AB70" s="5" t="n">
-        <v>8</v>
+      <c r="AB70" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AC70" t="inlineStr">
         <is>
-          <t>4953</t>
+          <t>5120</t>
         </is>
       </c>
     </row>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="AC71" t="inlineStr">
         <is>
-          <t>5728</t>
+          <t>5958</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="AC72" t="inlineStr">
         <is>
-          <t>5075</t>
+          <t>5150</t>
         </is>
       </c>
     </row>
@@ -5719,7 +5719,7 @@
       </c>
       <c r="AC73" t="inlineStr">
         <is>
-          <t>3958</t>
+          <t>4529</t>
         </is>
       </c>
     </row>
@@ -5811,12 +5811,12 @@
       <c r="AA74" t="n">
         <v>4584</v>
       </c>
-      <c r="AB74" s="2" t="n">
-        <v>0</v>
+      <c r="AB74" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AC74" t="inlineStr">
         <is>
-          <t>4584</t>
+          <t>4761</t>
         </is>
       </c>
     </row>
@@ -5913,7 +5913,7 @@
       </c>
       <c r="AC75" t="inlineStr">
         <is>
-          <t>3809</t>
+          <t>4245</t>
         </is>
       </c>
     </row>
@@ -6093,7 +6093,7 @@
       </c>
       <c r="AC77" t="inlineStr">
         <is>
-          <t>4804</t>
+          <t>4954</t>
         </is>
       </c>
     </row>
@@ -6190,7 +6190,7 @@
       </c>
       <c r="AC78" t="inlineStr">
         <is>
-          <t>4405</t>
+          <t>4533</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="AC79" t="inlineStr">
         <is>
-          <t>4128</t>
+          <t>4175</t>
         </is>
       </c>
     </row>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="AC80" t="inlineStr">
         <is>
-          <t>4053</t>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="AC81" t="inlineStr">
         <is>
-          <t>4173</t>
+          <t>4168</t>
         </is>
       </c>
     </row>
@@ -6578,7 +6578,7 @@
       </c>
       <c r="AC82" t="inlineStr">
         <is>
-          <t>4149</t>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -6675,7 +6675,7 @@
       </c>
       <c r="AC83" t="inlineStr">
         <is>
-          <t>2659</t>
+          <t>2691</t>
         </is>
       </c>
     </row>
@@ -7127,12 +7127,12 @@
       <c r="AA90" t="n">
         <v>5399</v>
       </c>
-      <c r="AB90" s="4" t="n">
-        <v>32</v>
+      <c r="AB90" s="5" t="n">
+        <v>2</v>
       </c>
       <c r="AC90" t="inlineStr">
         <is>
-          <t>5399</t>
+          <t>5392</t>
         </is>
       </c>
     </row>
@@ -7326,7 +7326,7 @@
       </c>
       <c r="AC92" t="inlineStr">
         <is>
-          <t>2744</t>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="AC93" t="inlineStr">
         <is>
-          <t>2540</t>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -7515,12 +7515,12 @@
       <c r="AA94" t="n">
         <v>4819</v>
       </c>
-      <c r="AB94" s="5" t="n">
-        <v>8</v>
+      <c r="AB94" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AC94" t="inlineStr">
         <is>
-          <t>4819</t>
+          <t>4915</t>
         </is>
       </c>
     </row>
@@ -7617,7 +7617,7 @@
       </c>
       <c r="AC95" t="inlineStr">
         <is>
-          <t>4773</t>
+          <t>5026</t>
         </is>
       </c>
     </row>
@@ -7714,7 +7714,7 @@
       </c>
       <c r="AC96" t="inlineStr">
         <is>
-          <t>2918</t>
+          <t>2916</t>
         </is>
       </c>
     </row>
@@ -7806,12 +7806,12 @@
       <c r="AA97" t="n">
         <v>4743</v>
       </c>
-      <c r="AB97" s="5" t="n">
-        <v>15</v>
+      <c r="AB97" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AC97" t="inlineStr">
         <is>
-          <t>4743</t>
+          <t>4810</t>
         </is>
       </c>
     </row>
@@ -7908,7 +7908,7 @@
       </c>
       <c r="AC98" t="inlineStr">
         <is>
-          <t>3361</t>
+          <t>3373</t>
         </is>
       </c>
     </row>
@@ -8001,11 +8001,11 @@
         <v>4376</v>
       </c>
       <c r="AB99" s="5" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AC99" t="inlineStr">
         <is>
-          <t>4376</t>
+          <t>4638</t>
         </is>
       </c>
     </row>
@@ -8098,11 +8098,11 @@
         <v>4497</v>
       </c>
       <c r="AB100" s="3" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="AC100" t="inlineStr">
         <is>
-          <t>4497</t>
+          <t>4538</t>
         </is>
       </c>
     </row>
@@ -8195,11 +8195,11 @@
         <v>4957</v>
       </c>
       <c r="AB101" s="3" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="AC101" t="inlineStr">
         <is>
-          <t>4957</t>
+          <t>5020</t>
         </is>
       </c>
     </row>
@@ -8291,12 +8291,12 @@
       <c r="AA102" t="n">
         <v>4499</v>
       </c>
-      <c r="AB102" s="5" t="n">
-        <v>16</v>
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AC102" t="inlineStr">
         <is>
-          <t>4499</t>
+          <t>4599</t>
         </is>
       </c>
     </row>
@@ -8389,11 +8389,11 @@
         <v>4465</v>
       </c>
       <c r="AB103" s="5" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AC103" t="inlineStr">
         <is>
-          <t>4465</t>
+          <t>4469</t>
         </is>
       </c>
     </row>
@@ -8486,11 +8486,11 @@
         <v>4332</v>
       </c>
       <c r="AB104" s="3" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AC104" t="inlineStr">
         <is>
-          <t>4332</t>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -8684,7 +8684,7 @@
       </c>
       <c r="AC106" t="inlineStr">
         <is>
-          <t>4410</t>
+          <t>4524</t>
         </is>
       </c>
     </row>
@@ -8776,12 +8776,12 @@
       <c r="AA107" t="n">
         <v>4316</v>
       </c>
-      <c r="AB107" s="3" t="n">
-        <v>20</v>
+      <c r="AB107" s="5" t="n">
+        <v>17</v>
       </c>
       <c r="AC107" t="inlineStr">
         <is>
-          <t>4316</t>
+          <t>4435</t>
         </is>
       </c>
     </row>
@@ -8873,12 +8873,12 @@
       <c r="AA108" t="n">
         <v>4370</v>
       </c>
-      <c r="AB108" s="5" t="n">
-        <v>4</v>
+      <c r="AB108" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AC108" t="inlineStr">
         <is>
-          <t>4370</t>
+          <t>4483</t>
         </is>
       </c>
     </row>
@@ -8970,8 +8970,8 @@
       <c r="AA109" t="n">
         <v>3169</v>
       </c>
-      <c r="AB109" s="5" t="n">
-        <v>5</v>
+      <c r="AB109" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AC109" t="inlineStr">
         <is>
@@ -9072,7 +9072,7 @@
       </c>
       <c r="AC110" t="inlineStr">
         <is>
-          <t>4217</t>
+          <t>4165</t>
         </is>
       </c>
     </row>
@@ -9208,11 +9208,11 @@
         <v>4123</v>
       </c>
       <c r="AB112" s="5" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="AC112" t="inlineStr">
         <is>
-          <t>4123</t>
+          <t>4090</t>
         </is>
       </c>
     </row>
@@ -9309,7 +9309,7 @@
       </c>
       <c r="AC113" t="inlineStr">
         <is>
-          <t>3590</t>
+          <t>3691</t>
         </is>
       </c>
     </row>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="AC115" t="inlineStr">
         <is>
-          <t>3445</t>
+          <t>3475</t>
         </is>
       </c>
     </row>
@@ -9596,7 +9596,7 @@
       </c>
       <c r="AC116" t="inlineStr">
         <is>
-          <t>3161</t>
+          <t>3159</t>
         </is>
       </c>
     </row>
@@ -9787,7 +9787,7 @@
       </c>
       <c r="AC119" t="inlineStr">
         <is>
-          <t>2744</t>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -9963,7 +9963,7 @@
       </c>
       <c r="AC121" t="inlineStr">
         <is>
-          <t>2888</t>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -10060,7 +10060,7 @@
       </c>
       <c r="AC122" t="inlineStr">
         <is>
-          <t>3323</t>
+          <t>3363</t>
         </is>
       </c>
     </row>
@@ -10220,7 +10220,7 @@
       </c>
       <c r="AC124" t="inlineStr">
         <is>
-          <t>2444</t>
+          <t>2439</t>
         </is>
       </c>
     </row>
@@ -10414,7 +10414,7 @@
       </c>
       <c r="AC126" t="inlineStr">
         <is>
-          <t>1464</t>
+          <t>1458</t>
         </is>
       </c>
     </row>
@@ -10511,7 +10511,7 @@
       </c>
       <c r="AC127" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>1612</t>
         </is>
       </c>
     </row>
@@ -10608,7 +10608,7 @@
       </c>
       <c r="AC128" t="inlineStr">
         <is>
-          <t>1230</t>
+          <t>1227</t>
         </is>
       </c>
     </row>
@@ -11287,7 +11287,7 @@
       </c>
       <c r="AC135" t="inlineStr">
         <is>
-          <t>3034</t>
+          <t>3099</t>
         </is>
       </c>
     </row>
@@ -11379,12 +11379,12 @@
       <c r="AA136" t="n">
         <v>4048</v>
       </c>
-      <c r="AB136" s="3" t="n">
-        <v>20</v>
+      <c r="AB136" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AC136" t="inlineStr">
         <is>
-          <t>4048</t>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -11578,7 +11578,7 @@
       </c>
       <c r="AC138" t="inlineStr">
         <is>
-          <t>2899</t>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -11869,7 +11869,7 @@
       </c>
       <c r="AC141" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2040</t>
         </is>
       </c>
     </row>
@@ -11962,11 +11962,11 @@
         <v>1999</v>
       </c>
       <c r="AB142" s="5" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AC142" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>2053</t>
         </is>
       </c>
     </row>
@@ -12063,7 +12063,7 @@
       </c>
       <c r="AC143" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1397</t>
         </is>
       </c>
     </row>
@@ -12839,7 +12839,7 @@
       </c>
       <c r="AC151" t="inlineStr">
         <is>
-          <t>3135</t>
+          <t>3166</t>
         </is>
       </c>
     </row>
@@ -13609,7 +13609,7 @@
       </c>
       <c r="AC159" t="inlineStr">
         <is>
-          <t>2709</t>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -13700,7 +13700,7 @@
       </c>
       <c r="AC160" t="inlineStr">
         <is>
-          <t>1784</t>
+          <t>1796</t>
         </is>
       </c>
     </row>
@@ -13791,7 +13791,7 @@
       </c>
       <c r="AC161" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1616</t>
         </is>
       </c>
     </row>
@@ -13878,7 +13878,7 @@
       </c>
       <c r="AC162" t="inlineStr">
         <is>
-          <t>2315</t>
+          <t>2330</t>
         </is>
       </c>
     </row>
@@ -13961,7 +13961,7 @@
       </c>
       <c r="AC163" t="inlineStr">
         <is>
-          <t>2817</t>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -14320,11 +14320,11 @@
         <v>5042</v>
       </c>
       <c r="AB170" s="3" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AC170" t="inlineStr">
         <is>
-          <t>5042</t>
+          <t>5192</t>
         </is>
       </c>
     </row>

</xml_diff>